<commit_message>
PP updated Signed-off-by: Hazem Mekawy <dextermekawy@gmail.com>
</commit_message>
<xml_diff>
--- a/SW deliveries log/PP.xlsx
+++ b/SW deliveries log/PP.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22325"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22430"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\ITI COURSES\Software Engineering\SWE_WORKSPACE\SW deliveries log\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EED363AA-D7B9-4859-9102-E07517D909C1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBA07FC4-C9FE-4EDA-BDF4-5CA014B5156E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="106" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PP" sheetId="1" r:id="rId1"/>
@@ -587,10 +587,13 @@
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="16" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -602,9 +605,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="16" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -825,8 +825,8 @@
   </sheetPr>
   <dimension ref="A1:KA1007"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection sqref="A1:E1"/>
+    <sheetView tabSelected="1" topLeftCell="D13" workbookViewId="0">
+      <selection activeCell="H19" sqref="H19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1"/>
@@ -842,7 +842,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:287" ht="28.2">
-      <c r="A1" s="36" t="s">
+      <c r="A1" s="38" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="37"/>
@@ -1148,11 +1148,11 @@
       <c r="E2" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="38" t="s">
+      <c r="F2" s="39" t="s">
         <v>6</v>
       </c>
-      <c r="G2" s="39"/>
-      <c r="H2" s="39"/>
+      <c r="G2" s="40"/>
+      <c r="H2" s="40"/>
       <c r="I2" s="8"/>
       <c r="J2" s="8"/>
       <c r="K2" s="8"/>
@@ -1736,7 +1736,7 @@
       <c r="A4" s="20" t="s">
         <v>12</v>
       </c>
-      <c r="B4" s="40" t="s">
+      <c r="B4" s="41" t="s">
         <v>13</v>
       </c>
       <c r="C4" s="37"/>
@@ -2060,18 +2060,18 @@
       <c r="KA5" s="19"/>
     </row>
     <row r="6" spans="1:287" ht="30.75" customHeight="1">
-      <c r="A6" s="41" t="s">
+      <c r="A6" s="42" t="s">
         <v>25</v>
       </c>
-      <c r="B6" s="42"/>
-      <c r="C6" s="42"/>
-      <c r="D6" s="42"/>
-      <c r="E6" s="42"/>
-      <c r="F6" s="42"/>
-      <c r="G6" s="42"/>
-      <c r="H6" s="42"/>
-      <c r="I6" s="42"/>
-      <c r="J6" s="42"/>
+      <c r="B6" s="43"/>
+      <c r="C6" s="43"/>
+      <c r="D6" s="43"/>
+      <c r="E6" s="43"/>
+      <c r="F6" s="43"/>
+      <c r="G6" s="43"/>
+      <c r="H6" s="43"/>
+      <c r="I6" s="43"/>
+      <c r="J6" s="43"/>
       <c r="K6" s="28"/>
       <c r="L6" s="28"/>
       <c r="M6" s="28"/>
@@ -2351,7 +2351,7 @@
       <c r="KA6" s="28"/>
     </row>
     <row r="7" spans="1:287" ht="30.75" customHeight="1">
-      <c r="A7" s="43" t="s">
+      <c r="A7" s="36" t="s">
         <v>26</v>
       </c>
       <c r="B7" s="37"/>
@@ -2965,10 +2965,10 @@
         <v>43854</v>
       </c>
       <c r="F9" s="31">
-        <v>43853</v>
+        <v>43852</v>
       </c>
       <c r="G9" s="31">
-        <v>43854</v>
+        <v>43853</v>
       </c>
       <c r="H9" s="30">
         <v>2</v>
@@ -3274,10 +3274,10 @@
         <v>43854</v>
       </c>
       <c r="F10" s="31">
-        <v>43852</v>
+        <v>43853</v>
       </c>
       <c r="G10" s="31">
-        <v>43853</v>
+        <v>43854</v>
       </c>
       <c r="H10" s="30">
         <v>2</v>
@@ -3583,10 +3583,10 @@
         <v>43854</v>
       </c>
       <c r="F11" s="31">
-        <v>43852</v>
+        <v>43853</v>
       </c>
       <c r="G11" s="31">
-        <v>43853</v>
+        <v>43854</v>
       </c>
       <c r="H11" s="30">
         <v>2</v>
@@ -3892,10 +3892,10 @@
         <v>43854</v>
       </c>
       <c r="F12" s="31">
-        <v>43852</v>
+        <v>43853</v>
       </c>
       <c r="G12" s="31">
-        <v>43853</v>
+        <v>43854</v>
       </c>
       <c r="H12" s="30">
         <v>2</v>
@@ -4185,7 +4185,7 @@
       <c r="KA12" s="28"/>
     </row>
     <row r="13" spans="1:287" ht="30.75" customHeight="1">
-      <c r="A13" s="43" t="s">
+      <c r="A13" s="36" t="s">
         <v>42</v>
       </c>
       <c r="B13" s="37"/>
@@ -4491,11 +4491,15 @@
       <c r="E14" s="31">
         <v>43865</v>
       </c>
-      <c r="F14" s="28"/>
-      <c r="G14" s="28"/>
+      <c r="F14" s="31">
+        <v>43865</v>
+      </c>
+      <c r="G14" s="31">
+        <v>43866</v>
+      </c>
       <c r="H14" s="28"/>
       <c r="I14" s="29" t="s">
-        <v>44</v>
+        <v>33</v>
       </c>
       <c r="J14" s="28"/>
       <c r="K14" s="28"/>
@@ -5394,11 +5398,13 @@
       <c r="E17" s="31">
         <v>43866</v>
       </c>
-      <c r="F17" s="28"/>
-      <c r="G17" s="28"/>
+      <c r="F17" s="31">
+        <v>43865</v>
+      </c>
+      <c r="G17" s="31"/>
       <c r="H17" s="28"/>
       <c r="I17" s="29" t="s">
-        <v>44</v>
+        <v>30</v>
       </c>
       <c r="J17" s="28"/>
       <c r="K17" s="28"/>
@@ -6000,7 +6006,7 @@
       <c r="G19" s="28"/>
       <c r="H19" s="28"/>
       <c r="I19" s="29" t="s">
-        <v>44</v>
+        <v>30</v>
       </c>
       <c r="J19" s="28"/>
       <c r="K19" s="28"/>
@@ -6598,11 +6604,15 @@
       <c r="E21" s="31">
         <v>43866</v>
       </c>
-      <c r="F21" s="28"/>
-      <c r="G21" s="28"/>
+      <c r="F21" s="31">
+        <v>43865</v>
+      </c>
+      <c r="G21" s="31">
+        <v>43866</v>
+      </c>
       <c r="H21" s="28"/>
       <c r="I21" s="29" t="s">
-        <v>44</v>
+        <v>33</v>
       </c>
       <c r="J21" s="28"/>
       <c r="K21" s="28"/>
@@ -7486,7 +7496,7 @@
       <c r="KA23" s="28"/>
     </row>
     <row r="24" spans="1:287" ht="30.75" customHeight="1">
-      <c r="A24" s="43" t="s">
+      <c r="A24" s="36" t="s">
         <v>54</v>
       </c>
       <c r="B24" s="37"/>

</xml_diff>

<commit_message>
- Updating PP - Adding RTM
Signed-off-by: Hazemmekawy <dextermekawy@gmail.com>
</commit_message>
<xml_diff>
--- a/SW deliveries log/PP.xlsx
+++ b/SW deliveries log/PP.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\ITI COURSES\Software Engineering\SWE_WORKSPACE\SW deliveries log\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hazem Mekawy\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBA07FC4-C9FE-4EDA-BDF4-5CA014B5156E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{275079F4-0308-4DC3-9677-6C50192D10FB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="106" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -194,7 +194,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="mmmm\ d\,\ yyyy"/>
   </numFmts>
-  <fonts count="21">
+  <fonts count="22">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -304,14 +304,21 @@
       <name val="Comfortaa"/>
     </font>
     <font>
-      <sz val="12"/>
-      <name val="Arial"/>
-    </font>
-    <font>
       <b/>
       <sz val="10"/>
       <color theme="1"/>
       <name val="Comfortaa"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Georgia"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <name val="Georgia"/>
+      <family val="1"/>
     </font>
   </fonts>
   <fills count="7">
@@ -480,7 +487,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -578,14 +585,17 @@
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="20" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="21" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -825,8 +835,8 @@
   </sheetPr>
   <dimension ref="A1:KA1007"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D13" workbookViewId="0">
-      <selection activeCell="H19" sqref="H19"/>
+    <sheetView tabSelected="1" topLeftCell="C15" workbookViewId="0">
+      <selection activeCell="H25" sqref="H25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1"/>
@@ -842,13 +852,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:287" ht="28.2">
-      <c r="A1" s="38" t="s">
+      <c r="A1" s="39" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="37"/>
-      <c r="C1" s="37"/>
-      <c r="D1" s="37"/>
-      <c r="E1" s="37"/>
+      <c r="B1" s="38"/>
+      <c r="C1" s="38"/>
+      <c r="D1" s="38"/>
+      <c r="E1" s="38"/>
       <c r="F1" s="1"/>
       <c r="G1" s="1"/>
       <c r="H1" s="1"/>
@@ -1148,11 +1158,11 @@
       <c r="E2" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="39" t="s">
+      <c r="F2" s="40" t="s">
         <v>6</v>
       </c>
-      <c r="G2" s="40"/>
-      <c r="H2" s="40"/>
+      <c r="G2" s="41"/>
+      <c r="H2" s="41"/>
       <c r="I2" s="8"/>
       <c r="J2" s="8"/>
       <c r="K2" s="8"/>
@@ -1736,12 +1746,12 @@
       <c r="A4" s="20" t="s">
         <v>12</v>
       </c>
-      <c r="B4" s="41" t="s">
+      <c r="B4" s="42" t="s">
         <v>13</v>
       </c>
-      <c r="C4" s="37"/>
-      <c r="D4" s="37"/>
-      <c r="E4" s="37"/>
+      <c r="C4" s="38"/>
+      <c r="D4" s="38"/>
+      <c r="E4" s="38"/>
       <c r="F4" s="21"/>
       <c r="G4" s="21"/>
       <c r="H4" s="22"/>
@@ -2060,18 +2070,18 @@
       <c r="KA5" s="19"/>
     </row>
     <row r="6" spans="1:287" ht="30.75" customHeight="1">
-      <c r="A6" s="42" t="s">
+      <c r="A6" s="43" t="s">
         <v>25</v>
       </c>
-      <c r="B6" s="43"/>
-      <c r="C6" s="43"/>
-      <c r="D6" s="43"/>
-      <c r="E6" s="43"/>
-      <c r="F6" s="43"/>
-      <c r="G6" s="43"/>
-      <c r="H6" s="43"/>
-      <c r="I6" s="43"/>
-      <c r="J6" s="43"/>
+      <c r="B6" s="44"/>
+      <c r="C6" s="44"/>
+      <c r="D6" s="44"/>
+      <c r="E6" s="44"/>
+      <c r="F6" s="44"/>
+      <c r="G6" s="44"/>
+      <c r="H6" s="44"/>
+      <c r="I6" s="44"/>
+      <c r="J6" s="44"/>
       <c r="K6" s="28"/>
       <c r="L6" s="28"/>
       <c r="M6" s="28"/>
@@ -2351,18 +2361,18 @@
       <c r="KA6" s="28"/>
     </row>
     <row r="7" spans="1:287" ht="30.75" customHeight="1">
-      <c r="A7" s="36" t="s">
+      <c r="A7" s="37" t="s">
         <v>26</v>
       </c>
-      <c r="B7" s="37"/>
-      <c r="C7" s="37"/>
-      <c r="D7" s="37"/>
-      <c r="E7" s="37"/>
-      <c r="F7" s="37"/>
-      <c r="G7" s="37"/>
-      <c r="H7" s="37"/>
-      <c r="I7" s="37"/>
-      <c r="J7" s="37"/>
+      <c r="B7" s="38"/>
+      <c r="C7" s="38"/>
+      <c r="D7" s="38"/>
+      <c r="E7" s="38"/>
+      <c r="F7" s="38"/>
+      <c r="G7" s="38"/>
+      <c r="H7" s="38"/>
+      <c r="I7" s="38"/>
+      <c r="J7" s="38"/>
       <c r="K7" s="28"/>
       <c r="L7" s="28"/>
       <c r="M7" s="28"/>
@@ -4185,18 +4195,18 @@
       <c r="KA12" s="28"/>
     </row>
     <row r="13" spans="1:287" ht="30.75" customHeight="1">
-      <c r="A13" s="36" t="s">
+      <c r="A13" s="37" t="s">
         <v>42</v>
       </c>
-      <c r="B13" s="37"/>
-      <c r="C13" s="37"/>
-      <c r="D13" s="37"/>
-      <c r="E13" s="37"/>
-      <c r="F13" s="37"/>
-      <c r="G13" s="37"/>
-      <c r="H13" s="37"/>
-      <c r="I13" s="37"/>
-      <c r="J13" s="37"/>
+      <c r="B13" s="38"/>
+      <c r="C13" s="38"/>
+      <c r="D13" s="38"/>
+      <c r="E13" s="38"/>
+      <c r="F13" s="38"/>
+      <c r="G13" s="38"/>
+      <c r="H13" s="38"/>
+      <c r="I13" s="38"/>
+      <c r="J13" s="38"/>
       <c r="K13" s="28"/>
       <c r="L13" s="28"/>
       <c r="M13" s="28"/>
@@ -4497,7 +4507,9 @@
       <c r="G14" s="31">
         <v>43866</v>
       </c>
-      <c r="H14" s="28"/>
+      <c r="H14" s="28">
+        <v>2</v>
+      </c>
       <c r="I14" s="29" t="s">
         <v>33</v>
       </c>
@@ -4796,11 +4808,17 @@
       <c r="E15" s="31">
         <v>43866</v>
       </c>
-      <c r="F15" s="28"/>
-      <c r="G15" s="28"/>
-      <c r="H15" s="28"/>
+      <c r="F15" s="31">
+        <v>43865</v>
+      </c>
+      <c r="G15" s="31">
+        <v>43866</v>
+      </c>
+      <c r="H15" s="28">
+        <v>2</v>
+      </c>
       <c r="I15" s="29" t="s">
-        <v>44</v>
+        <v>33</v>
       </c>
       <c r="J15" s="28"/>
       <c r="K15" s="28"/>
@@ -5097,11 +5115,17 @@
       <c r="E16" s="31">
         <v>43867</v>
       </c>
-      <c r="F16" s="28"/>
-      <c r="G16" s="28"/>
-      <c r="H16" s="28"/>
+      <c r="F16" s="31">
+        <v>43866</v>
+      </c>
+      <c r="G16" s="31">
+        <v>43866</v>
+      </c>
+      <c r="H16" s="28">
+        <v>1</v>
+      </c>
       <c r="I16" s="29" t="s">
-        <v>44</v>
+        <v>33</v>
       </c>
       <c r="J16" s="28"/>
       <c r="K16" s="28"/>
@@ -5392,19 +5416,23 @@
       <c r="C17" s="30" t="s">
         <v>32</v>
       </c>
-      <c r="D17" s="31">
+      <c r="D17" s="35">
         <v>43865</v>
       </c>
-      <c r="E17" s="31">
+      <c r="E17" s="35">
         <v>43866</v>
       </c>
       <c r="F17" s="31">
-        <v>43865</v>
+        <v>43864</v>
       </c>
-      <c r="G17" s="31"/>
-      <c r="H17" s="28"/>
+      <c r="G17" s="31">
+        <v>43866</v>
+      </c>
+      <c r="H17" s="28">
+        <v>3</v>
+      </c>
       <c r="I17" s="29" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="J17" s="28"/>
       <c r="K17" s="28"/>
@@ -5686,8 +5714,8 @@
       <c r="KA17" s="28"/>
     </row>
     <row r="18" spans="1:287" ht="30.75" customHeight="1">
-      <c r="A18" s="32" t="s">
-        <v>48</v>
+      <c r="A18" s="29" t="s">
+        <v>50</v>
       </c>
       <c r="B18" s="30" t="s">
         <v>28</v>
@@ -5695,17 +5723,23 @@
       <c r="C18" s="30" t="s">
         <v>8</v>
       </c>
-      <c r="D18" s="33">
+      <c r="D18" s="35">
         <v>43866</v>
       </c>
-      <c r="E18" s="33">
+      <c r="E18" s="35">
         <v>43867</v>
       </c>
-      <c r="F18" s="28"/>
-      <c r="G18" s="28"/>
-      <c r="H18" s="28"/>
+      <c r="F18" s="35">
+        <v>43866</v>
+      </c>
+      <c r="G18" s="31">
+        <v>43867</v>
+      </c>
+      <c r="H18" s="28">
+        <v>2</v>
+      </c>
       <c r="I18" s="29" t="s">
-        <v>44</v>
+        <v>33</v>
       </c>
       <c r="J18" s="28"/>
       <c r="K18" s="28"/>
@@ -5988,25 +6022,31 @@
     </row>
     <row r="19" spans="1:287" ht="30.75" customHeight="1">
       <c r="A19" s="32" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B19" s="30" t="s">
         <v>28</v>
       </c>
       <c r="C19" s="30" t="s">
-        <v>38</v>
+        <v>8</v>
       </c>
-      <c r="D19" s="33">
+      <c r="D19" s="36">
+        <v>43866</v>
+      </c>
+      <c r="E19" s="36">
         <v>43867</v>
       </c>
-      <c r="E19" s="33">
+      <c r="F19" s="31">
         <v>43867</v>
       </c>
-      <c r="F19" s="28"/>
-      <c r="G19" s="28"/>
-      <c r="H19" s="28"/>
+      <c r="G19" s="31">
+        <v>43867</v>
+      </c>
+      <c r="H19" s="28">
+        <v>1</v>
+      </c>
       <c r="I19" s="29" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="J19" s="28"/>
       <c r="K19" s="28"/>
@@ -6288,19 +6328,19 @@
       <c r="KA19" s="28"/>
     </row>
     <row r="20" spans="1:287" ht="30.75" customHeight="1">
-      <c r="A20" s="29" t="s">
-        <v>50</v>
+      <c r="A20" s="32" t="s">
+        <v>49</v>
       </c>
       <c r="B20" s="30" t="s">
         <v>28</v>
       </c>
       <c r="C20" s="30" t="s">
-        <v>8</v>
+        <v>38</v>
       </c>
-      <c r="D20" s="31">
-        <v>43866</v>
+      <c r="D20" s="36">
+        <v>43867</v>
       </c>
-      <c r="E20" s="31">
+      <c r="E20" s="36">
         <v>43867</v>
       </c>
       <c r="F20" s="28"/>
@@ -6598,10 +6638,10 @@
       <c r="C21" s="30" t="s">
         <v>40</v>
       </c>
-      <c r="D21" s="31">
+      <c r="D21" s="35">
         <v>43865</v>
       </c>
-      <c r="E21" s="31">
+      <c r="E21" s="35">
         <v>43866</v>
       </c>
       <c r="F21" s="31">
@@ -6610,7 +6650,9 @@
       <c r="G21" s="31">
         <v>43866</v>
       </c>
-      <c r="H21" s="28"/>
+      <c r="H21" s="28">
+        <v>2</v>
+      </c>
       <c r="I21" s="29" t="s">
         <v>33</v>
       </c>
@@ -6903,17 +6945,19 @@
       <c r="C22" s="30" t="s">
         <v>36</v>
       </c>
-      <c r="D22" s="31">
+      <c r="D22" s="35">
         <v>43866</v>
       </c>
-      <c r="E22" s="31">
+      <c r="E22" s="35">
         <v>43867</v>
       </c>
-      <c r="F22" s="28"/>
+      <c r="F22" s="35">
+        <v>43866</v>
+      </c>
       <c r="G22" s="28"/>
       <c r="H22" s="28"/>
       <c r="I22" s="29" t="s">
-        <v>44</v>
+        <v>30</v>
       </c>
       <c r="J22" s="28"/>
       <c r="K22" s="28"/>
@@ -7204,10 +7248,10 @@
       <c r="C23" s="30" t="s">
         <v>8</v>
       </c>
-      <c r="D23" s="31">
+      <c r="D23" s="35">
         <v>43867</v>
       </c>
-      <c r="E23" s="33">
+      <c r="E23" s="36">
         <v>43868</v>
       </c>
       <c r="F23" s="28"/>
@@ -7496,18 +7540,18 @@
       <c r="KA23" s="28"/>
     </row>
     <row r="24" spans="1:287" ht="30.75" customHeight="1">
-      <c r="A24" s="36" t="s">
+      <c r="A24" s="37" t="s">
         <v>54</v>
       </c>
-      <c r="B24" s="37"/>
-      <c r="C24" s="37"/>
-      <c r="D24" s="37"/>
-      <c r="E24" s="37"/>
-      <c r="F24" s="37"/>
-      <c r="G24" s="37"/>
-      <c r="H24" s="37"/>
-      <c r="I24" s="37"/>
-      <c r="J24" s="37"/>
+      <c r="B24" s="38"/>
+      <c r="C24" s="38"/>
+      <c r="D24" s="38"/>
+      <c r="E24" s="38"/>
+      <c r="F24" s="38"/>
+      <c r="G24" s="38"/>
+      <c r="H24" s="38"/>
+      <c r="I24" s="38"/>
+      <c r="J24" s="38"/>
       <c r="K24" s="28"/>
       <c r="L24" s="28"/>
       <c r="M24" s="28"/>
@@ -7787,7 +7831,7 @@
       <c r="KA24" s="28"/>
     </row>
     <row r="25" spans="1:287" ht="30.75" customHeight="1">
-      <c r="A25" s="34"/>
+      <c r="A25" s="33"/>
       <c r="B25" s="28"/>
       <c r="C25" s="30"/>
       <c r="D25" s="28"/>
@@ -8076,7 +8120,7 @@
       <c r="KA25" s="28"/>
     </row>
     <row r="26" spans="1:287" ht="30.75" customHeight="1">
-      <c r="A26" s="34"/>
+      <c r="A26" s="33"/>
       <c r="B26" s="28"/>
       <c r="C26" s="30"/>
       <c r="D26" s="28"/>
@@ -8365,7 +8409,7 @@
       <c r="KA26" s="28"/>
     </row>
     <row r="27" spans="1:287" ht="30.75" customHeight="1">
-      <c r="A27" s="34"/>
+      <c r="A27" s="33"/>
       <c r="B27" s="28"/>
       <c r="C27" s="30"/>
       <c r="D27" s="28"/>
@@ -8654,7 +8698,7 @@
       <c r="KA27" s="28"/>
     </row>
     <row r="28" spans="1:287" ht="30.75" customHeight="1">
-      <c r="A28" s="34"/>
+      <c r="A28" s="33"/>
       <c r="B28" s="28"/>
       <c r="C28" s="30"/>
       <c r="D28" s="28"/>
@@ -8943,7 +8987,7 @@
       <c r="KA28" s="28"/>
     </row>
     <row r="29" spans="1:287" ht="30.75" customHeight="1">
-      <c r="A29" s="34"/>
+      <c r="A29" s="33"/>
       <c r="B29" s="28"/>
       <c r="C29" s="30"/>
       <c r="D29" s="28"/>
@@ -9232,7 +9276,7 @@
       <c r="KA29" s="28"/>
     </row>
     <row r="30" spans="1:287" ht="30.75" customHeight="1">
-      <c r="A30" s="34"/>
+      <c r="A30" s="33"/>
       <c r="B30" s="28"/>
       <c r="C30" s="30"/>
       <c r="D30" s="28"/>
@@ -9521,7 +9565,7 @@
       <c r="KA30" s="28"/>
     </row>
     <row r="31" spans="1:287" ht="30.75" customHeight="1">
-      <c r="A31" s="34"/>
+      <c r="A31" s="33"/>
       <c r="B31" s="28"/>
       <c r="C31" s="30"/>
       <c r="D31" s="28"/>
@@ -9810,7 +9854,7 @@
       <c r="KA31" s="28"/>
     </row>
     <row r="32" spans="1:287" ht="30.75" customHeight="1">
-      <c r="A32" s="34"/>
+      <c r="A32" s="33"/>
       <c r="B32" s="28"/>
       <c r="C32" s="30"/>
       <c r="D32" s="28"/>
@@ -10099,7 +10143,7 @@
       <c r="KA32" s="28"/>
     </row>
     <row r="33" spans="1:287" ht="30.75" customHeight="1">
-      <c r="A33" s="34"/>
+      <c r="A33" s="33"/>
       <c r="B33" s="28"/>
       <c r="C33" s="30"/>
       <c r="D33" s="28"/>
@@ -10388,7 +10432,7 @@
       <c r="KA33" s="28"/>
     </row>
     <row r="34" spans="1:287" ht="30.75" customHeight="1">
-      <c r="A34" s="34"/>
+      <c r="A34" s="33"/>
       <c r="B34" s="28"/>
       <c r="C34" s="30"/>
       <c r="D34" s="28"/>
@@ -10677,7 +10721,7 @@
       <c r="KA34" s="28"/>
     </row>
     <row r="35" spans="1:287" ht="30.75" customHeight="1">
-      <c r="A35" s="34"/>
+      <c r="A35" s="33"/>
       <c r="B35" s="28"/>
       <c r="C35" s="30"/>
       <c r="D35" s="28"/>
@@ -10966,7 +11010,7 @@
       <c r="KA35" s="28"/>
     </row>
     <row r="36" spans="1:287" ht="30.75" customHeight="1">
-      <c r="A36" s="34"/>
+      <c r="A36" s="33"/>
       <c r="B36" s="28"/>
       <c r="C36" s="30"/>
       <c r="D36" s="28"/>
@@ -11255,7 +11299,7 @@
       <c r="KA36" s="28"/>
     </row>
     <row r="37" spans="1:287" ht="30.75" customHeight="1">
-      <c r="A37" s="34"/>
+      <c r="A37" s="33"/>
       <c r="B37" s="28"/>
       <c r="C37" s="30"/>
       <c r="D37" s="28"/>
@@ -11544,7 +11588,7 @@
       <c r="KA37" s="28"/>
     </row>
     <row r="38" spans="1:287" ht="30.75" customHeight="1">
-      <c r="A38" s="34"/>
+      <c r="A38" s="33"/>
       <c r="B38" s="28"/>
       <c r="C38" s="30"/>
       <c r="D38" s="28"/>
@@ -11833,7 +11877,7 @@
       <c r="KA38" s="28"/>
     </row>
     <row r="39" spans="1:287" ht="30.75" customHeight="1">
-      <c r="A39" s="34"/>
+      <c r="A39" s="33"/>
       <c r="B39" s="28"/>
       <c r="C39" s="30"/>
       <c r="D39" s="28"/>
@@ -12122,7 +12166,7 @@
       <c r="KA39" s="28"/>
     </row>
     <row r="40" spans="1:287" ht="30.75" customHeight="1">
-      <c r="A40" s="34"/>
+      <c r="A40" s="33"/>
       <c r="B40" s="28"/>
       <c r="C40" s="30"/>
       <c r="D40" s="28"/>
@@ -12411,7 +12455,7 @@
       <c r="KA40" s="28"/>
     </row>
     <row r="41" spans="1:287" ht="30.75" customHeight="1">
-      <c r="A41" s="34"/>
+      <c r="A41" s="33"/>
       <c r="B41" s="28"/>
       <c r="C41" s="30"/>
       <c r="D41" s="28"/>
@@ -12700,7 +12744,7 @@
       <c r="KA41" s="28"/>
     </row>
     <row r="42" spans="1:287" ht="30.75" customHeight="1">
-      <c r="A42" s="34"/>
+      <c r="A42" s="33"/>
       <c r="B42" s="28"/>
       <c r="C42" s="30"/>
       <c r="D42" s="28"/>
@@ -12989,7 +13033,7 @@
       <c r="KA42" s="28"/>
     </row>
     <row r="43" spans="1:287" ht="30.75" customHeight="1">
-      <c r="A43" s="34"/>
+      <c r="A43" s="33"/>
       <c r="B43" s="28"/>
       <c r="C43" s="30"/>
       <c r="D43" s="28"/>
@@ -13278,7 +13322,7 @@
       <c r="KA43" s="28"/>
     </row>
     <row r="44" spans="1:287" ht="30.75" customHeight="1">
-      <c r="A44" s="34"/>
+      <c r="A44" s="33"/>
       <c r="B44" s="28"/>
       <c r="C44" s="30"/>
       <c r="D44" s="28"/>
@@ -13567,7 +13611,7 @@
       <c r="KA44" s="28"/>
     </row>
     <row r="45" spans="1:287" ht="30.75" customHeight="1">
-      <c r="A45" s="34"/>
+      <c r="A45" s="33"/>
       <c r="B45" s="28"/>
       <c r="C45" s="30"/>
       <c r="D45" s="28"/>
@@ -13856,7 +13900,7 @@
       <c r="KA45" s="28"/>
     </row>
     <row r="46" spans="1:287" ht="30.75" customHeight="1">
-      <c r="A46" s="34"/>
+      <c r="A46" s="33"/>
       <c r="B46" s="28"/>
       <c r="C46" s="30"/>
       <c r="D46" s="28"/>
@@ -14145,7 +14189,7 @@
       <c r="KA46" s="28"/>
     </row>
     <row r="47" spans="1:287" ht="30.75" customHeight="1">
-      <c r="A47" s="34"/>
+      <c r="A47" s="33"/>
       <c r="B47" s="28"/>
       <c r="C47" s="30"/>
       <c r="D47" s="28"/>
@@ -14434,7 +14478,7 @@
       <c r="KA47" s="28"/>
     </row>
     <row r="48" spans="1:287" ht="30.75" customHeight="1">
-      <c r="A48" s="34"/>
+      <c r="A48" s="33"/>
       <c r="B48" s="28"/>
       <c r="C48" s="30"/>
       <c r="D48" s="28"/>
@@ -14723,7 +14767,7 @@
       <c r="KA48" s="28"/>
     </row>
     <row r="49" spans="1:287" ht="30.75" customHeight="1">
-      <c r="A49" s="34"/>
+      <c r="A49" s="33"/>
       <c r="B49" s="28"/>
       <c r="C49" s="30"/>
       <c r="D49" s="28"/>
@@ -15012,7 +15056,7 @@
       <c r="KA49" s="28"/>
     </row>
     <row r="50" spans="1:287" ht="30.75" customHeight="1">
-      <c r="A50" s="34"/>
+      <c r="A50" s="33"/>
       <c r="B50" s="28"/>
       <c r="C50" s="30"/>
       <c r="D50" s="28"/>
@@ -15301,7 +15345,7 @@
       <c r="KA50" s="28"/>
     </row>
     <row r="51" spans="1:287" ht="30.75" customHeight="1">
-      <c r="A51" s="34"/>
+      <c r="A51" s="33"/>
       <c r="B51" s="28"/>
       <c r="C51" s="30"/>
       <c r="D51" s="28"/>
@@ -15590,7 +15634,7 @@
       <c r="KA51" s="28"/>
     </row>
     <row r="52" spans="1:287" ht="30.75" customHeight="1">
-      <c r="A52" s="34"/>
+      <c r="A52" s="33"/>
       <c r="B52" s="28"/>
       <c r="C52" s="30"/>
       <c r="D52" s="28"/>
@@ -15879,7 +15923,7 @@
       <c r="KA52" s="28"/>
     </row>
     <row r="53" spans="1:287" ht="30.75" customHeight="1">
-      <c r="A53" s="34"/>
+      <c r="A53" s="33"/>
       <c r="B53" s="28"/>
       <c r="C53" s="30"/>
       <c r="D53" s="28"/>
@@ -16168,7 +16212,7 @@
       <c r="KA53" s="28"/>
     </row>
     <row r="54" spans="1:287" ht="30.75" customHeight="1">
-      <c r="A54" s="34"/>
+      <c r="A54" s="33"/>
       <c r="B54" s="28"/>
       <c r="C54" s="30"/>
       <c r="D54" s="28"/>
@@ -16457,7 +16501,7 @@
       <c r="KA54" s="28"/>
     </row>
     <row r="55" spans="1:287" ht="30.75" customHeight="1">
-      <c r="A55" s="34"/>
+      <c r="A55" s="33"/>
       <c r="B55" s="28"/>
       <c r="C55" s="30"/>
       <c r="D55" s="28"/>
@@ -16746,7 +16790,7 @@
       <c r="KA55" s="28"/>
     </row>
     <row r="56" spans="1:287" ht="30.75" customHeight="1">
-      <c r="A56" s="34"/>
+      <c r="A56" s="33"/>
       <c r="B56" s="28"/>
       <c r="C56" s="30"/>
       <c r="D56" s="28"/>
@@ -17035,7 +17079,7 @@
       <c r="KA56" s="28"/>
     </row>
     <row r="57" spans="1:287" ht="30.75" customHeight="1">
-      <c r="A57" s="34"/>
+      <c r="A57" s="33"/>
       <c r="B57" s="28"/>
       <c r="C57" s="30"/>
       <c r="D57" s="28"/>
@@ -17324,7 +17368,7 @@
       <c r="KA57" s="28"/>
     </row>
     <row r="58" spans="1:287" ht="30.75" customHeight="1">
-      <c r="A58" s="34"/>
+      <c r="A58" s="33"/>
       <c r="B58" s="28"/>
       <c r="C58" s="30"/>
       <c r="D58" s="28"/>
@@ -17613,7 +17657,7 @@
       <c r="KA58" s="28"/>
     </row>
     <row r="59" spans="1:287" ht="30.75" customHeight="1">
-      <c r="A59" s="34"/>
+      <c r="A59" s="33"/>
       <c r="B59" s="28"/>
       <c r="C59" s="30"/>
       <c r="D59" s="28"/>
@@ -17902,2848 +17946,2848 @@
       <c r="KA59" s="28"/>
     </row>
     <row r="60" spans="1:287" ht="13.2">
-      <c r="A60" s="35"/>
+      <c r="A60" s="34"/>
     </row>
     <row r="61" spans="1:287" ht="13.2">
-      <c r="A61" s="35"/>
+      <c r="A61" s="34"/>
     </row>
     <row r="62" spans="1:287" ht="13.2">
-      <c r="A62" s="35"/>
+      <c r="A62" s="34"/>
     </row>
     <row r="63" spans="1:287" ht="13.2">
-      <c r="A63" s="35"/>
+      <c r="A63" s="34"/>
     </row>
     <row r="64" spans="1:287" ht="13.2">
-      <c r="A64" s="35"/>
+      <c r="A64" s="34"/>
     </row>
     <row r="65" spans="1:1" ht="13.2">
-      <c r="A65" s="35"/>
+      <c r="A65" s="34"/>
     </row>
     <row r="66" spans="1:1" ht="13.2">
-      <c r="A66" s="35"/>
+      <c r="A66" s="34"/>
     </row>
     <row r="67" spans="1:1" ht="13.2">
-      <c r="A67" s="35"/>
+      <c r="A67" s="34"/>
     </row>
     <row r="68" spans="1:1" ht="13.2">
-      <c r="A68" s="35"/>
+      <c r="A68" s="34"/>
     </row>
     <row r="69" spans="1:1" ht="13.2">
-      <c r="A69" s="35"/>
+      <c r="A69" s="34"/>
     </row>
     <row r="70" spans="1:1" ht="13.2">
-      <c r="A70" s="35"/>
+      <c r="A70" s="34"/>
     </row>
     <row r="71" spans="1:1" ht="13.2">
-      <c r="A71" s="35"/>
+      <c r="A71" s="34"/>
     </row>
     <row r="72" spans="1:1" ht="13.2">
-      <c r="A72" s="35"/>
+      <c r="A72" s="34"/>
     </row>
     <row r="73" spans="1:1" ht="13.2">
-      <c r="A73" s="35"/>
+      <c r="A73" s="34"/>
     </row>
     <row r="74" spans="1:1" ht="13.2">
-      <c r="A74" s="35"/>
+      <c r="A74" s="34"/>
     </row>
     <row r="75" spans="1:1" ht="13.2">
-      <c r="A75" s="35"/>
+      <c r="A75" s="34"/>
     </row>
     <row r="76" spans="1:1" ht="13.2">
-      <c r="A76" s="35"/>
+      <c r="A76" s="34"/>
     </row>
     <row r="77" spans="1:1" ht="13.2">
-      <c r="A77" s="35"/>
+      <c r="A77" s="34"/>
     </row>
     <row r="78" spans="1:1" ht="13.2">
-      <c r="A78" s="35"/>
+      <c r="A78" s="34"/>
     </row>
     <row r="79" spans="1:1" ht="13.2">
-      <c r="A79" s="35"/>
+      <c r="A79" s="34"/>
     </row>
     <row r="80" spans="1:1" ht="13.2">
-      <c r="A80" s="35"/>
+      <c r="A80" s="34"/>
     </row>
     <row r="81" spans="1:1" ht="13.2">
-      <c r="A81" s="35"/>
+      <c r="A81" s="34"/>
     </row>
     <row r="82" spans="1:1" ht="13.2">
-      <c r="A82" s="35"/>
+      <c r="A82" s="34"/>
     </row>
     <row r="83" spans="1:1" ht="13.2">
-      <c r="A83" s="35"/>
+      <c r="A83" s="34"/>
     </row>
     <row r="84" spans="1:1" ht="13.2">
-      <c r="A84" s="35"/>
+      <c r="A84" s="34"/>
     </row>
     <row r="85" spans="1:1" ht="13.2">
-      <c r="A85" s="35"/>
+      <c r="A85" s="34"/>
     </row>
     <row r="86" spans="1:1" ht="13.2">
-      <c r="A86" s="35"/>
+      <c r="A86" s="34"/>
     </row>
     <row r="87" spans="1:1" ht="13.2">
-      <c r="A87" s="35"/>
+      <c r="A87" s="34"/>
     </row>
     <row r="88" spans="1:1" ht="13.2">
-      <c r="A88" s="35"/>
+      <c r="A88" s="34"/>
     </row>
     <row r="89" spans="1:1" ht="13.2">
-      <c r="A89" s="35"/>
+      <c r="A89" s="34"/>
     </row>
     <row r="90" spans="1:1" ht="13.2">
-      <c r="A90" s="35"/>
+      <c r="A90" s="34"/>
     </row>
     <row r="91" spans="1:1" ht="13.2">
-      <c r="A91" s="35"/>
+      <c r="A91" s="34"/>
     </row>
     <row r="92" spans="1:1" ht="13.2">
-      <c r="A92" s="35"/>
+      <c r="A92" s="34"/>
     </row>
     <row r="93" spans="1:1" ht="13.2">
-      <c r="A93" s="35"/>
+      <c r="A93" s="34"/>
     </row>
     <row r="94" spans="1:1" ht="13.2">
-      <c r="A94" s="35"/>
+      <c r="A94" s="34"/>
     </row>
     <row r="95" spans="1:1" ht="13.2">
-      <c r="A95" s="35"/>
+      <c r="A95" s="34"/>
     </row>
     <row r="96" spans="1:1" ht="13.2">
-      <c r="A96" s="35"/>
+      <c r="A96" s="34"/>
     </row>
     <row r="97" spans="1:1" ht="13.2">
-      <c r="A97" s="35"/>
+      <c r="A97" s="34"/>
     </row>
     <row r="98" spans="1:1" ht="13.2">
-      <c r="A98" s="35"/>
+      <c r="A98" s="34"/>
     </row>
     <row r="99" spans="1:1" ht="13.2">
-      <c r="A99" s="35"/>
+      <c r="A99" s="34"/>
     </row>
     <row r="100" spans="1:1" ht="13.2">
-      <c r="A100" s="35"/>
+      <c r="A100" s="34"/>
     </row>
     <row r="101" spans="1:1" ht="13.2">
-      <c r="A101" s="35"/>
+      <c r="A101" s="34"/>
     </row>
     <row r="102" spans="1:1" ht="13.2">
-      <c r="A102" s="35"/>
+      <c r="A102" s="34"/>
     </row>
     <row r="103" spans="1:1" ht="13.2">
-      <c r="A103" s="35"/>
+      <c r="A103" s="34"/>
     </row>
     <row r="104" spans="1:1" ht="13.2">
-      <c r="A104" s="35"/>
+      <c r="A104" s="34"/>
     </row>
     <row r="105" spans="1:1" ht="13.2">
-      <c r="A105" s="35"/>
+      <c r="A105" s="34"/>
     </row>
     <row r="106" spans="1:1" ht="13.2">
-      <c r="A106" s="35"/>
+      <c r="A106" s="34"/>
     </row>
     <row r="107" spans="1:1" ht="13.2">
-      <c r="A107" s="35"/>
+      <c r="A107" s="34"/>
     </row>
     <row r="108" spans="1:1" ht="13.2">
-      <c r="A108" s="35"/>
+      <c r="A108" s="34"/>
     </row>
     <row r="109" spans="1:1" ht="13.2">
-      <c r="A109" s="35"/>
+      <c r="A109" s="34"/>
     </row>
     <row r="110" spans="1:1" ht="13.2">
-      <c r="A110" s="35"/>
+      <c r="A110" s="34"/>
     </row>
     <row r="111" spans="1:1" ht="13.2">
-      <c r="A111" s="35"/>
+      <c r="A111" s="34"/>
     </row>
     <row r="112" spans="1:1" ht="13.2">
-      <c r="A112" s="35"/>
+      <c r="A112" s="34"/>
     </row>
     <row r="113" spans="1:1" ht="13.2">
-      <c r="A113" s="35"/>
+      <c r="A113" s="34"/>
     </row>
     <row r="114" spans="1:1" ht="13.2">
-      <c r="A114" s="35"/>
+      <c r="A114" s="34"/>
     </row>
     <row r="115" spans="1:1" ht="13.2">
-      <c r="A115" s="35"/>
+      <c r="A115" s="34"/>
     </row>
     <row r="116" spans="1:1" ht="13.2">
-      <c r="A116" s="35"/>
+      <c r="A116" s="34"/>
     </row>
     <row r="117" spans="1:1" ht="13.2">
-      <c r="A117" s="35"/>
+      <c r="A117" s="34"/>
     </row>
     <row r="118" spans="1:1" ht="13.2">
-      <c r="A118" s="35"/>
+      <c r="A118" s="34"/>
     </row>
     <row r="119" spans="1:1" ht="13.2">
-      <c r="A119" s="35"/>
+      <c r="A119" s="34"/>
     </row>
     <row r="120" spans="1:1" ht="13.2">
-      <c r="A120" s="35"/>
+      <c r="A120" s="34"/>
     </row>
     <row r="121" spans="1:1" ht="13.2">
-      <c r="A121" s="35"/>
+      <c r="A121" s="34"/>
     </row>
     <row r="122" spans="1:1" ht="13.2">
-      <c r="A122" s="35"/>
+      <c r="A122" s="34"/>
     </row>
     <row r="123" spans="1:1" ht="13.2">
-      <c r="A123" s="35"/>
+      <c r="A123" s="34"/>
     </row>
     <row r="124" spans="1:1" ht="13.2">
-      <c r="A124" s="35"/>
+      <c r="A124" s="34"/>
     </row>
     <row r="125" spans="1:1" ht="13.2">
-      <c r="A125" s="35"/>
+      <c r="A125" s="34"/>
     </row>
     <row r="126" spans="1:1" ht="13.2">
-      <c r="A126" s="35"/>
+      <c r="A126" s="34"/>
     </row>
     <row r="127" spans="1:1" ht="13.2">
-      <c r="A127" s="35"/>
+      <c r="A127" s="34"/>
     </row>
     <row r="128" spans="1:1" ht="13.2">
-      <c r="A128" s="35"/>
+      <c r="A128" s="34"/>
     </row>
     <row r="129" spans="1:1" ht="13.2">
-      <c r="A129" s="35"/>
+      <c r="A129" s="34"/>
     </row>
     <row r="130" spans="1:1" ht="13.2">
-      <c r="A130" s="35"/>
+      <c r="A130" s="34"/>
     </row>
     <row r="131" spans="1:1" ht="13.2">
-      <c r="A131" s="35"/>
+      <c r="A131" s="34"/>
     </row>
     <row r="132" spans="1:1" ht="13.2">
-      <c r="A132" s="35"/>
+      <c r="A132" s="34"/>
     </row>
     <row r="133" spans="1:1" ht="13.2">
-      <c r="A133" s="35"/>
+      <c r="A133" s="34"/>
     </row>
     <row r="134" spans="1:1" ht="13.2">
-      <c r="A134" s="35"/>
+      <c r="A134" s="34"/>
     </row>
     <row r="135" spans="1:1" ht="13.2">
-      <c r="A135" s="35"/>
+      <c r="A135" s="34"/>
     </row>
     <row r="136" spans="1:1" ht="13.2">
-      <c r="A136" s="35"/>
+      <c r="A136" s="34"/>
     </row>
     <row r="137" spans="1:1" ht="13.2">
-      <c r="A137" s="35"/>
+      <c r="A137" s="34"/>
     </row>
     <row r="138" spans="1:1" ht="13.2">
-      <c r="A138" s="35"/>
+      <c r="A138" s="34"/>
     </row>
     <row r="139" spans="1:1" ht="13.2">
-      <c r="A139" s="35"/>
+      <c r="A139" s="34"/>
     </row>
     <row r="140" spans="1:1" ht="13.2">
-      <c r="A140" s="35"/>
+      <c r="A140" s="34"/>
     </row>
     <row r="141" spans="1:1" ht="13.2">
-      <c r="A141" s="35"/>
+      <c r="A141" s="34"/>
     </row>
     <row r="142" spans="1:1" ht="13.2">
-      <c r="A142" s="35"/>
+      <c r="A142" s="34"/>
     </row>
     <row r="143" spans="1:1" ht="13.2">
-      <c r="A143" s="35"/>
+      <c r="A143" s="34"/>
     </row>
     <row r="144" spans="1:1" ht="13.2">
-      <c r="A144" s="35"/>
+      <c r="A144" s="34"/>
     </row>
     <row r="145" spans="1:1" ht="13.2">
-      <c r="A145" s="35"/>
+      <c r="A145" s="34"/>
     </row>
     <row r="146" spans="1:1" ht="13.2">
-      <c r="A146" s="35"/>
+      <c r="A146" s="34"/>
     </row>
     <row r="147" spans="1:1" ht="13.2">
-      <c r="A147" s="35"/>
+      <c r="A147" s="34"/>
     </row>
     <row r="148" spans="1:1" ht="13.2">
-      <c r="A148" s="35"/>
+      <c r="A148" s="34"/>
     </row>
     <row r="149" spans="1:1" ht="13.2">
-      <c r="A149" s="35"/>
+      <c r="A149" s="34"/>
     </row>
     <row r="150" spans="1:1" ht="13.2">
-      <c r="A150" s="35"/>
+      <c r="A150" s="34"/>
     </row>
     <row r="151" spans="1:1" ht="13.2">
-      <c r="A151" s="35"/>
+      <c r="A151" s="34"/>
     </row>
     <row r="152" spans="1:1" ht="13.2">
-      <c r="A152" s="35"/>
+      <c r="A152" s="34"/>
     </row>
     <row r="153" spans="1:1" ht="13.2">
-      <c r="A153" s="35"/>
+      <c r="A153" s="34"/>
     </row>
     <row r="154" spans="1:1" ht="13.2">
-      <c r="A154" s="35"/>
+      <c r="A154" s="34"/>
     </row>
     <row r="155" spans="1:1" ht="13.2">
-      <c r="A155" s="35"/>
+      <c r="A155" s="34"/>
     </row>
     <row r="156" spans="1:1" ht="13.2">
-      <c r="A156" s="35"/>
+      <c r="A156" s="34"/>
     </row>
     <row r="157" spans="1:1" ht="13.2">
-      <c r="A157" s="35"/>
+      <c r="A157" s="34"/>
     </row>
     <row r="158" spans="1:1" ht="13.2">
-      <c r="A158" s="35"/>
+      <c r="A158" s="34"/>
     </row>
     <row r="159" spans="1:1" ht="13.2">
-      <c r="A159" s="35"/>
+      <c r="A159" s="34"/>
     </row>
     <row r="160" spans="1:1" ht="13.2">
-      <c r="A160" s="35"/>
+      <c r="A160" s="34"/>
     </row>
     <row r="161" spans="1:1" ht="13.2">
-      <c r="A161" s="35"/>
+      <c r="A161" s="34"/>
     </row>
     <row r="162" spans="1:1" ht="13.2">
-      <c r="A162" s="35"/>
+      <c r="A162" s="34"/>
     </row>
     <row r="163" spans="1:1" ht="13.2">
-      <c r="A163" s="35"/>
+      <c r="A163" s="34"/>
     </row>
     <row r="164" spans="1:1" ht="13.2">
-      <c r="A164" s="35"/>
+      <c r="A164" s="34"/>
     </row>
     <row r="165" spans="1:1" ht="13.2">
-      <c r="A165" s="35"/>
+      <c r="A165" s="34"/>
     </row>
     <row r="166" spans="1:1" ht="13.2">
-      <c r="A166" s="35"/>
+      <c r="A166" s="34"/>
     </row>
     <row r="167" spans="1:1" ht="13.2">
-      <c r="A167" s="35"/>
+      <c r="A167" s="34"/>
     </row>
     <row r="168" spans="1:1" ht="13.2">
-      <c r="A168" s="35"/>
+      <c r="A168" s="34"/>
     </row>
     <row r="169" spans="1:1" ht="13.2">
-      <c r="A169" s="35"/>
+      <c r="A169" s="34"/>
     </row>
     <row r="170" spans="1:1" ht="13.2">
-      <c r="A170" s="35"/>
+      <c r="A170" s="34"/>
     </row>
     <row r="171" spans="1:1" ht="13.2">
-      <c r="A171" s="35"/>
+      <c r="A171" s="34"/>
     </row>
     <row r="172" spans="1:1" ht="13.2">
-      <c r="A172" s="35"/>
+      <c r="A172" s="34"/>
     </row>
     <row r="173" spans="1:1" ht="13.2">
-      <c r="A173" s="35"/>
+      <c r="A173" s="34"/>
     </row>
     <row r="174" spans="1:1" ht="13.2">
-      <c r="A174" s="35"/>
+      <c r="A174" s="34"/>
     </row>
     <row r="175" spans="1:1" ht="13.2">
-      <c r="A175" s="35"/>
+      <c r="A175" s="34"/>
     </row>
     <row r="176" spans="1:1" ht="13.2">
-      <c r="A176" s="35"/>
+      <c r="A176" s="34"/>
     </row>
     <row r="177" spans="1:1" ht="13.2">
-      <c r="A177" s="35"/>
+      <c r="A177" s="34"/>
     </row>
     <row r="178" spans="1:1" ht="13.2">
-      <c r="A178" s="35"/>
+      <c r="A178" s="34"/>
     </row>
     <row r="179" spans="1:1" ht="13.2">
-      <c r="A179" s="35"/>
+      <c r="A179" s="34"/>
     </row>
     <row r="180" spans="1:1" ht="13.2">
-      <c r="A180" s="35"/>
+      <c r="A180" s="34"/>
     </row>
     <row r="181" spans="1:1" ht="13.2">
-      <c r="A181" s="35"/>
+      <c r="A181" s="34"/>
     </row>
     <row r="182" spans="1:1" ht="13.2">
-      <c r="A182" s="35"/>
+      <c r="A182" s="34"/>
     </row>
     <row r="183" spans="1:1" ht="13.2">
-      <c r="A183" s="35"/>
+      <c r="A183" s="34"/>
     </row>
     <row r="184" spans="1:1" ht="13.2">
-      <c r="A184" s="35"/>
+      <c r="A184" s="34"/>
     </row>
     <row r="185" spans="1:1" ht="13.2">
-      <c r="A185" s="35"/>
+      <c r="A185" s="34"/>
     </row>
     <row r="186" spans="1:1" ht="13.2">
-      <c r="A186" s="35"/>
+      <c r="A186" s="34"/>
     </row>
     <row r="187" spans="1:1" ht="13.2">
-      <c r="A187" s="35"/>
+      <c r="A187" s="34"/>
     </row>
     <row r="188" spans="1:1" ht="13.2">
-      <c r="A188" s="35"/>
+      <c r="A188" s="34"/>
     </row>
     <row r="189" spans="1:1" ht="13.2">
-      <c r="A189" s="35"/>
+      <c r="A189" s="34"/>
     </row>
     <row r="190" spans="1:1" ht="13.2">
-      <c r="A190" s="35"/>
+      <c r="A190" s="34"/>
     </row>
     <row r="191" spans="1:1" ht="13.2">
-      <c r="A191" s="35"/>
+      <c r="A191" s="34"/>
     </row>
     <row r="192" spans="1:1" ht="13.2">
-      <c r="A192" s="35"/>
+      <c r="A192" s="34"/>
     </row>
     <row r="193" spans="1:1" ht="13.2">
-      <c r="A193" s="35"/>
+      <c r="A193" s="34"/>
     </row>
     <row r="194" spans="1:1" ht="13.2">
-      <c r="A194" s="35"/>
+      <c r="A194" s="34"/>
     </row>
     <row r="195" spans="1:1" ht="13.2">
-      <c r="A195" s="35"/>
+      <c r="A195" s="34"/>
     </row>
     <row r="196" spans="1:1" ht="13.2">
-      <c r="A196" s="35"/>
+      <c r="A196" s="34"/>
     </row>
     <row r="197" spans="1:1" ht="13.2">
-      <c r="A197" s="35"/>
+      <c r="A197" s="34"/>
     </row>
     <row r="198" spans="1:1" ht="13.2">
-      <c r="A198" s="35"/>
+      <c r="A198" s="34"/>
     </row>
     <row r="199" spans="1:1" ht="13.2">
-      <c r="A199" s="35"/>
+      <c r="A199" s="34"/>
     </row>
     <row r="200" spans="1:1" ht="13.2">
-      <c r="A200" s="35"/>
+      <c r="A200" s="34"/>
     </row>
     <row r="201" spans="1:1" ht="13.2">
-      <c r="A201" s="35"/>
+      <c r="A201" s="34"/>
     </row>
     <row r="202" spans="1:1" ht="13.2">
-      <c r="A202" s="35"/>
+      <c r="A202" s="34"/>
     </row>
     <row r="203" spans="1:1" ht="13.2">
-      <c r="A203" s="35"/>
+      <c r="A203" s="34"/>
     </row>
     <row r="204" spans="1:1" ht="13.2">
-      <c r="A204" s="35"/>
+      <c r="A204" s="34"/>
     </row>
     <row r="205" spans="1:1" ht="13.2">
-      <c r="A205" s="35"/>
+      <c r="A205" s="34"/>
     </row>
     <row r="206" spans="1:1" ht="13.2">
-      <c r="A206" s="35"/>
+      <c r="A206" s="34"/>
     </row>
     <row r="207" spans="1:1" ht="13.2">
-      <c r="A207" s="35"/>
+      <c r="A207" s="34"/>
     </row>
     <row r="208" spans="1:1" ht="13.2">
-      <c r="A208" s="35"/>
+      <c r="A208" s="34"/>
     </row>
     <row r="209" spans="1:1" ht="13.2">
-      <c r="A209" s="35"/>
+      <c r="A209" s="34"/>
     </row>
     <row r="210" spans="1:1" ht="13.2">
-      <c r="A210" s="35"/>
+      <c r="A210" s="34"/>
     </row>
     <row r="211" spans="1:1" ht="13.2">
-      <c r="A211" s="35"/>
+      <c r="A211" s="34"/>
     </row>
     <row r="212" spans="1:1" ht="13.2">
-      <c r="A212" s="35"/>
+      <c r="A212" s="34"/>
     </row>
     <row r="213" spans="1:1" ht="13.2">
-      <c r="A213" s="35"/>
+      <c r="A213" s="34"/>
     </row>
     <row r="214" spans="1:1" ht="13.2">
-      <c r="A214" s="35"/>
+      <c r="A214" s="34"/>
     </row>
     <row r="215" spans="1:1" ht="13.2">
-      <c r="A215" s="35"/>
+      <c r="A215" s="34"/>
     </row>
     <row r="216" spans="1:1" ht="13.2">
-      <c r="A216" s="35"/>
+      <c r="A216" s="34"/>
     </row>
     <row r="217" spans="1:1" ht="13.2">
-      <c r="A217" s="35"/>
+      <c r="A217" s="34"/>
     </row>
     <row r="218" spans="1:1" ht="13.2">
-      <c r="A218" s="35"/>
+      <c r="A218" s="34"/>
     </row>
     <row r="219" spans="1:1" ht="13.2">
-      <c r="A219" s="35"/>
+      <c r="A219" s="34"/>
     </row>
     <row r="220" spans="1:1" ht="13.2">
-      <c r="A220" s="35"/>
+      <c r="A220" s="34"/>
     </row>
     <row r="221" spans="1:1" ht="13.2">
-      <c r="A221" s="35"/>
+      <c r="A221" s="34"/>
     </row>
     <row r="222" spans="1:1" ht="13.2">
-      <c r="A222" s="35"/>
+      <c r="A222" s="34"/>
     </row>
     <row r="223" spans="1:1" ht="13.2">
-      <c r="A223" s="35"/>
+      <c r="A223" s="34"/>
     </row>
     <row r="224" spans="1:1" ht="13.2">
-      <c r="A224" s="35"/>
+      <c r="A224" s="34"/>
     </row>
     <row r="225" spans="1:1" ht="13.2">
-      <c r="A225" s="35"/>
+      <c r="A225" s="34"/>
     </row>
     <row r="226" spans="1:1" ht="13.2">
-      <c r="A226" s="35"/>
+      <c r="A226" s="34"/>
     </row>
     <row r="227" spans="1:1" ht="13.2">
-      <c r="A227" s="35"/>
+      <c r="A227" s="34"/>
     </row>
     <row r="228" spans="1:1" ht="13.2">
-      <c r="A228" s="35"/>
+      <c r="A228" s="34"/>
     </row>
     <row r="229" spans="1:1" ht="13.2">
-      <c r="A229" s="35"/>
+      <c r="A229" s="34"/>
     </row>
     <row r="230" spans="1:1" ht="13.2">
-      <c r="A230" s="35"/>
+      <c r="A230" s="34"/>
     </row>
     <row r="231" spans="1:1" ht="13.2">
-      <c r="A231" s="35"/>
+      <c r="A231" s="34"/>
     </row>
     <row r="232" spans="1:1" ht="13.2">
-      <c r="A232" s="35"/>
+      <c r="A232" s="34"/>
     </row>
     <row r="233" spans="1:1" ht="13.2">
-      <c r="A233" s="35"/>
+      <c r="A233" s="34"/>
     </row>
     <row r="234" spans="1:1" ht="13.2">
-      <c r="A234" s="35"/>
+      <c r="A234" s="34"/>
     </row>
     <row r="235" spans="1:1" ht="13.2">
-      <c r="A235" s="35"/>
+      <c r="A235" s="34"/>
     </row>
     <row r="236" spans="1:1" ht="13.2">
-      <c r="A236" s="35"/>
+      <c r="A236" s="34"/>
     </row>
     <row r="237" spans="1:1" ht="13.2">
-      <c r="A237" s="35"/>
+      <c r="A237" s="34"/>
     </row>
     <row r="238" spans="1:1" ht="13.2">
-      <c r="A238" s="35"/>
+      <c r="A238" s="34"/>
     </row>
     <row r="239" spans="1:1" ht="13.2">
-      <c r="A239" s="35"/>
+      <c r="A239" s="34"/>
     </row>
     <row r="240" spans="1:1" ht="13.2">
-      <c r="A240" s="35"/>
+      <c r="A240" s="34"/>
     </row>
     <row r="241" spans="1:1" ht="13.2">
-      <c r="A241" s="35"/>
+      <c r="A241" s="34"/>
     </row>
     <row r="242" spans="1:1" ht="13.2">
-      <c r="A242" s="35"/>
+      <c r="A242" s="34"/>
     </row>
     <row r="243" spans="1:1" ht="13.2">
-      <c r="A243" s="35"/>
+      <c r="A243" s="34"/>
     </row>
     <row r="244" spans="1:1" ht="13.2">
-      <c r="A244" s="35"/>
+      <c r="A244" s="34"/>
     </row>
     <row r="245" spans="1:1" ht="13.2">
-      <c r="A245" s="35"/>
+      <c r="A245" s="34"/>
     </row>
     <row r="246" spans="1:1" ht="13.2">
-      <c r="A246" s="35"/>
+      <c r="A246" s="34"/>
     </row>
     <row r="247" spans="1:1" ht="13.2">
-      <c r="A247" s="35"/>
+      <c r="A247" s="34"/>
     </row>
     <row r="248" spans="1:1" ht="13.2">
-      <c r="A248" s="35"/>
+      <c r="A248" s="34"/>
     </row>
     <row r="249" spans="1:1" ht="13.2">
-      <c r="A249" s="35"/>
+      <c r="A249" s="34"/>
     </row>
     <row r="250" spans="1:1" ht="13.2">
-      <c r="A250" s="35"/>
+      <c r="A250" s="34"/>
     </row>
     <row r="251" spans="1:1" ht="13.2">
-      <c r="A251" s="35"/>
+      <c r="A251" s="34"/>
     </row>
     <row r="252" spans="1:1" ht="13.2">
-      <c r="A252" s="35"/>
+      <c r="A252" s="34"/>
     </row>
     <row r="253" spans="1:1" ht="13.2">
-      <c r="A253" s="35"/>
+      <c r="A253" s="34"/>
     </row>
     <row r="254" spans="1:1" ht="13.2">
-      <c r="A254" s="35"/>
+      <c r="A254" s="34"/>
     </row>
     <row r="255" spans="1:1" ht="13.2">
-      <c r="A255" s="35"/>
+      <c r="A255" s="34"/>
     </row>
     <row r="256" spans="1:1" ht="13.2">
-      <c r="A256" s="35"/>
+      <c r="A256" s="34"/>
     </row>
     <row r="257" spans="1:1" ht="13.2">
-      <c r="A257" s="35"/>
+      <c r="A257" s="34"/>
     </row>
     <row r="258" spans="1:1" ht="13.2">
-      <c r="A258" s="35"/>
+      <c r="A258" s="34"/>
     </row>
     <row r="259" spans="1:1" ht="13.2">
-      <c r="A259" s="35"/>
+      <c r="A259" s="34"/>
     </row>
     <row r="260" spans="1:1" ht="13.2">
-      <c r="A260" s="35"/>
+      <c r="A260" s="34"/>
     </row>
     <row r="261" spans="1:1" ht="13.2">
-      <c r="A261" s="35"/>
+      <c r="A261" s="34"/>
     </row>
     <row r="262" spans="1:1" ht="13.2">
-      <c r="A262" s="35"/>
+      <c r="A262" s="34"/>
     </row>
     <row r="263" spans="1:1" ht="13.2">
-      <c r="A263" s="35"/>
+      <c r="A263" s="34"/>
     </row>
     <row r="264" spans="1:1" ht="13.2">
-      <c r="A264" s="35"/>
+      <c r="A264" s="34"/>
     </row>
     <row r="265" spans="1:1" ht="13.2">
-      <c r="A265" s="35"/>
+      <c r="A265" s="34"/>
     </row>
     <row r="266" spans="1:1" ht="13.2">
-      <c r="A266" s="35"/>
+      <c r="A266" s="34"/>
     </row>
     <row r="267" spans="1:1" ht="13.2">
-      <c r="A267" s="35"/>
+      <c r="A267" s="34"/>
     </row>
     <row r="268" spans="1:1" ht="13.2">
-      <c r="A268" s="35"/>
+      <c r="A268" s="34"/>
     </row>
     <row r="269" spans="1:1" ht="13.2">
-      <c r="A269" s="35"/>
+      <c r="A269" s="34"/>
     </row>
     <row r="270" spans="1:1" ht="13.2">
-      <c r="A270" s="35"/>
+      <c r="A270" s="34"/>
     </row>
     <row r="271" spans="1:1" ht="13.2">
-      <c r="A271" s="35"/>
+      <c r="A271" s="34"/>
     </row>
     <row r="272" spans="1:1" ht="13.2">
-      <c r="A272" s="35"/>
+      <c r="A272" s="34"/>
     </row>
     <row r="273" spans="1:1" ht="13.2">
-      <c r="A273" s="35"/>
+      <c r="A273" s="34"/>
     </row>
     <row r="274" spans="1:1" ht="13.2">
-      <c r="A274" s="35"/>
+      <c r="A274" s="34"/>
     </row>
     <row r="275" spans="1:1" ht="13.2">
-      <c r="A275" s="35"/>
+      <c r="A275" s="34"/>
     </row>
     <row r="276" spans="1:1" ht="13.2">
-      <c r="A276" s="35"/>
+      <c r="A276" s="34"/>
     </row>
     <row r="277" spans="1:1" ht="13.2">
-      <c r="A277" s="35"/>
+      <c r="A277" s="34"/>
     </row>
     <row r="278" spans="1:1" ht="13.2">
-      <c r="A278" s="35"/>
+      <c r="A278" s="34"/>
     </row>
     <row r="279" spans="1:1" ht="13.2">
-      <c r="A279" s="35"/>
+      <c r="A279" s="34"/>
     </row>
     <row r="280" spans="1:1" ht="13.2">
-      <c r="A280" s="35"/>
+      <c r="A280" s="34"/>
     </row>
     <row r="281" spans="1:1" ht="13.2">
-      <c r="A281" s="35"/>
+      <c r="A281" s="34"/>
     </row>
     <row r="282" spans="1:1" ht="13.2">
-      <c r="A282" s="35"/>
+      <c r="A282" s="34"/>
     </row>
     <row r="283" spans="1:1" ht="13.2">
-      <c r="A283" s="35"/>
+      <c r="A283" s="34"/>
     </row>
     <row r="284" spans="1:1" ht="13.2">
-      <c r="A284" s="35"/>
+      <c r="A284" s="34"/>
     </row>
     <row r="285" spans="1:1" ht="13.2">
-      <c r="A285" s="35"/>
+      <c r="A285" s="34"/>
     </row>
     <row r="286" spans="1:1" ht="13.2">
-      <c r="A286" s="35"/>
+      <c r="A286" s="34"/>
     </row>
     <row r="287" spans="1:1" ht="13.2">
-      <c r="A287" s="35"/>
+      <c r="A287" s="34"/>
     </row>
     <row r="288" spans="1:1" ht="13.2">
-      <c r="A288" s="35"/>
+      <c r="A288" s="34"/>
     </row>
     <row r="289" spans="1:1" ht="13.2">
-      <c r="A289" s="35"/>
+      <c r="A289" s="34"/>
     </row>
     <row r="290" spans="1:1" ht="13.2">
-      <c r="A290" s="35"/>
+      <c r="A290" s="34"/>
     </row>
     <row r="291" spans="1:1" ht="13.2">
-      <c r="A291" s="35"/>
+      <c r="A291" s="34"/>
     </row>
     <row r="292" spans="1:1" ht="13.2">
-      <c r="A292" s="35"/>
+      <c r="A292" s="34"/>
     </row>
     <row r="293" spans="1:1" ht="13.2">
-      <c r="A293" s="35"/>
+      <c r="A293" s="34"/>
     </row>
     <row r="294" spans="1:1" ht="13.2">
-      <c r="A294" s="35"/>
+      <c r="A294" s="34"/>
     </row>
     <row r="295" spans="1:1" ht="13.2">
-      <c r="A295" s="35"/>
+      <c r="A295" s="34"/>
     </row>
     <row r="296" spans="1:1" ht="13.2">
-      <c r="A296" s="35"/>
+      <c r="A296" s="34"/>
     </row>
     <row r="297" spans="1:1" ht="13.2">
-      <c r="A297" s="35"/>
+      <c r="A297" s="34"/>
     </row>
     <row r="298" spans="1:1" ht="13.2">
-      <c r="A298" s="35"/>
+      <c r="A298" s="34"/>
     </row>
     <row r="299" spans="1:1" ht="13.2">
-      <c r="A299" s="35"/>
+      <c r="A299" s="34"/>
     </row>
     <row r="300" spans="1:1" ht="13.2">
-      <c r="A300" s="35"/>
+      <c r="A300" s="34"/>
     </row>
     <row r="301" spans="1:1" ht="13.2">
-      <c r="A301" s="35"/>
+      <c r="A301" s="34"/>
     </row>
     <row r="302" spans="1:1" ht="13.2">
-      <c r="A302" s="35"/>
+      <c r="A302" s="34"/>
     </row>
     <row r="303" spans="1:1" ht="13.2">
-      <c r="A303" s="35"/>
+      <c r="A303" s="34"/>
     </row>
     <row r="304" spans="1:1" ht="13.2">
-      <c r="A304" s="35"/>
+      <c r="A304" s="34"/>
     </row>
     <row r="305" spans="1:1" ht="13.2">
-      <c r="A305" s="35"/>
+      <c r="A305" s="34"/>
     </row>
     <row r="306" spans="1:1" ht="13.2">
-      <c r="A306" s="35"/>
+      <c r="A306" s="34"/>
     </row>
     <row r="307" spans="1:1" ht="13.2">
-      <c r="A307" s="35"/>
+      <c r="A307" s="34"/>
     </row>
     <row r="308" spans="1:1" ht="13.2">
-      <c r="A308" s="35"/>
+      <c r="A308" s="34"/>
     </row>
     <row r="309" spans="1:1" ht="13.2">
-      <c r="A309" s="35"/>
+      <c r="A309" s="34"/>
     </row>
     <row r="310" spans="1:1" ht="13.2">
-      <c r="A310" s="35"/>
+      <c r="A310" s="34"/>
     </row>
     <row r="311" spans="1:1" ht="13.2">
-      <c r="A311" s="35"/>
+      <c r="A311" s="34"/>
     </row>
     <row r="312" spans="1:1" ht="13.2">
-      <c r="A312" s="35"/>
+      <c r="A312" s="34"/>
     </row>
     <row r="313" spans="1:1" ht="13.2">
-      <c r="A313" s="35"/>
+      <c r="A313" s="34"/>
     </row>
     <row r="314" spans="1:1" ht="13.2">
-      <c r="A314" s="35"/>
+      <c r="A314" s="34"/>
     </row>
     <row r="315" spans="1:1" ht="13.2">
-      <c r="A315" s="35"/>
+      <c r="A315" s="34"/>
     </row>
     <row r="316" spans="1:1" ht="13.2">
-      <c r="A316" s="35"/>
+      <c r="A316" s="34"/>
     </row>
     <row r="317" spans="1:1" ht="13.2">
-      <c r="A317" s="35"/>
+      <c r="A317" s="34"/>
     </row>
     <row r="318" spans="1:1" ht="13.2">
-      <c r="A318" s="35"/>
+      <c r="A318" s="34"/>
     </row>
     <row r="319" spans="1:1" ht="13.2">
-      <c r="A319" s="35"/>
+      <c r="A319" s="34"/>
     </row>
     <row r="320" spans="1:1" ht="13.2">
-      <c r="A320" s="35"/>
+      <c r="A320" s="34"/>
     </row>
     <row r="321" spans="1:1" ht="13.2">
-      <c r="A321" s="35"/>
+      <c r="A321" s="34"/>
     </row>
     <row r="322" spans="1:1" ht="13.2">
-      <c r="A322" s="35"/>
+      <c r="A322" s="34"/>
     </row>
     <row r="323" spans="1:1" ht="13.2">
-      <c r="A323" s="35"/>
+      <c r="A323" s="34"/>
     </row>
     <row r="324" spans="1:1" ht="13.2">
-      <c r="A324" s="35"/>
+      <c r="A324" s="34"/>
     </row>
     <row r="325" spans="1:1" ht="13.2">
-      <c r="A325" s="35"/>
+      <c r="A325" s="34"/>
     </row>
     <row r="326" spans="1:1" ht="13.2">
-      <c r="A326" s="35"/>
+      <c r="A326" s="34"/>
     </row>
     <row r="327" spans="1:1" ht="13.2">
-      <c r="A327" s="35"/>
+      <c r="A327" s="34"/>
     </row>
     <row r="328" spans="1:1" ht="13.2">
-      <c r="A328" s="35"/>
+      <c r="A328" s="34"/>
     </row>
     <row r="329" spans="1:1" ht="13.2">
-      <c r="A329" s="35"/>
+      <c r="A329" s="34"/>
     </row>
     <row r="330" spans="1:1" ht="13.2">
-      <c r="A330" s="35"/>
+      <c r="A330" s="34"/>
     </row>
     <row r="331" spans="1:1" ht="13.2">
-      <c r="A331" s="35"/>
+      <c r="A331" s="34"/>
     </row>
     <row r="332" spans="1:1" ht="13.2">
-      <c r="A332" s="35"/>
+      <c r="A332" s="34"/>
     </row>
     <row r="333" spans="1:1" ht="13.2">
-      <c r="A333" s="35"/>
+      <c r="A333" s="34"/>
     </row>
     <row r="334" spans="1:1" ht="13.2">
-      <c r="A334" s="35"/>
+      <c r="A334" s="34"/>
     </row>
     <row r="335" spans="1:1" ht="13.2">
-      <c r="A335" s="35"/>
+      <c r="A335" s="34"/>
     </row>
     <row r="336" spans="1:1" ht="13.2">
-      <c r="A336" s="35"/>
+      <c r="A336" s="34"/>
     </row>
     <row r="337" spans="1:1" ht="13.2">
-      <c r="A337" s="35"/>
+      <c r="A337" s="34"/>
     </row>
     <row r="338" spans="1:1" ht="13.2">
-      <c r="A338" s="35"/>
+      <c r="A338" s="34"/>
     </row>
     <row r="339" spans="1:1" ht="13.2">
-      <c r="A339" s="35"/>
+      <c r="A339" s="34"/>
     </row>
     <row r="340" spans="1:1" ht="13.2">
-      <c r="A340" s="35"/>
+      <c r="A340" s="34"/>
     </row>
     <row r="341" spans="1:1" ht="13.2">
-      <c r="A341" s="35"/>
+      <c r="A341" s="34"/>
     </row>
     <row r="342" spans="1:1" ht="13.2">
-      <c r="A342" s="35"/>
+      <c r="A342" s="34"/>
     </row>
     <row r="343" spans="1:1" ht="13.2">
-      <c r="A343" s="35"/>
+      <c r="A343" s="34"/>
     </row>
     <row r="344" spans="1:1" ht="13.2">
-      <c r="A344" s="35"/>
+      <c r="A344" s="34"/>
     </row>
     <row r="345" spans="1:1" ht="13.2">
-      <c r="A345" s="35"/>
+      <c r="A345" s="34"/>
     </row>
     <row r="346" spans="1:1" ht="13.2">
-      <c r="A346" s="35"/>
+      <c r="A346" s="34"/>
     </row>
     <row r="347" spans="1:1" ht="13.2">
-      <c r="A347" s="35"/>
+      <c r="A347" s="34"/>
     </row>
     <row r="348" spans="1:1" ht="13.2">
-      <c r="A348" s="35"/>
+      <c r="A348" s="34"/>
     </row>
     <row r="349" spans="1:1" ht="13.2">
-      <c r="A349" s="35"/>
+      <c r="A349" s="34"/>
     </row>
     <row r="350" spans="1:1" ht="13.2">
-      <c r="A350" s="35"/>
+      <c r="A350" s="34"/>
     </row>
     <row r="351" spans="1:1" ht="13.2">
-      <c r="A351" s="35"/>
+      <c r="A351" s="34"/>
     </row>
     <row r="352" spans="1:1" ht="13.2">
-      <c r="A352" s="35"/>
+      <c r="A352" s="34"/>
     </row>
     <row r="353" spans="1:1" ht="13.2">
-      <c r="A353" s="35"/>
+      <c r="A353" s="34"/>
     </row>
     <row r="354" spans="1:1" ht="13.2">
-      <c r="A354" s="35"/>
+      <c r="A354" s="34"/>
     </row>
     <row r="355" spans="1:1" ht="13.2">
-      <c r="A355" s="35"/>
+      <c r="A355" s="34"/>
     </row>
     <row r="356" spans="1:1" ht="13.2">
-      <c r="A356" s="35"/>
+      <c r="A356" s="34"/>
     </row>
     <row r="357" spans="1:1" ht="13.2">
-      <c r="A357" s="35"/>
+      <c r="A357" s="34"/>
     </row>
     <row r="358" spans="1:1" ht="13.2">
-      <c r="A358" s="35"/>
+      <c r="A358" s="34"/>
     </row>
     <row r="359" spans="1:1" ht="13.2">
-      <c r="A359" s="35"/>
+      <c r="A359" s="34"/>
     </row>
     <row r="360" spans="1:1" ht="13.2">
-      <c r="A360" s="35"/>
+      <c r="A360" s="34"/>
     </row>
     <row r="361" spans="1:1" ht="13.2">
-      <c r="A361" s="35"/>
+      <c r="A361" s="34"/>
     </row>
     <row r="362" spans="1:1" ht="13.2">
-      <c r="A362" s="35"/>
+      <c r="A362" s="34"/>
     </row>
     <row r="363" spans="1:1" ht="13.2">
-      <c r="A363" s="35"/>
+      <c r="A363" s="34"/>
     </row>
     <row r="364" spans="1:1" ht="13.2">
-      <c r="A364" s="35"/>
+      <c r="A364" s="34"/>
     </row>
     <row r="365" spans="1:1" ht="13.2">
-      <c r="A365" s="35"/>
+      <c r="A365" s="34"/>
     </row>
     <row r="366" spans="1:1" ht="13.2">
-      <c r="A366" s="35"/>
+      <c r="A366" s="34"/>
     </row>
     <row r="367" spans="1:1" ht="13.2">
-      <c r="A367" s="35"/>
+      <c r="A367" s="34"/>
     </row>
     <row r="368" spans="1:1" ht="13.2">
-      <c r="A368" s="35"/>
+      <c r="A368" s="34"/>
     </row>
     <row r="369" spans="1:1" ht="13.2">
-      <c r="A369" s="35"/>
+      <c r="A369" s="34"/>
     </row>
     <row r="370" spans="1:1" ht="13.2">
-      <c r="A370" s="35"/>
+      <c r="A370" s="34"/>
     </row>
     <row r="371" spans="1:1" ht="13.2">
-      <c r="A371" s="35"/>
+      <c r="A371" s="34"/>
     </row>
     <row r="372" spans="1:1" ht="13.2">
-      <c r="A372" s="35"/>
+      <c r="A372" s="34"/>
     </row>
     <row r="373" spans="1:1" ht="13.2">
-      <c r="A373" s="35"/>
+      <c r="A373" s="34"/>
     </row>
     <row r="374" spans="1:1" ht="13.2">
-      <c r="A374" s="35"/>
+      <c r="A374" s="34"/>
     </row>
     <row r="375" spans="1:1" ht="13.2">
-      <c r="A375" s="35"/>
+      <c r="A375" s="34"/>
     </row>
     <row r="376" spans="1:1" ht="13.2">
-      <c r="A376" s="35"/>
+      <c r="A376" s="34"/>
     </row>
     <row r="377" spans="1:1" ht="13.2">
-      <c r="A377" s="35"/>
+      <c r="A377" s="34"/>
     </row>
     <row r="378" spans="1:1" ht="13.2">
-      <c r="A378" s="35"/>
+      <c r="A378" s="34"/>
     </row>
     <row r="379" spans="1:1" ht="13.2">
-      <c r="A379" s="35"/>
+      <c r="A379" s="34"/>
     </row>
     <row r="380" spans="1:1" ht="13.2">
-      <c r="A380" s="35"/>
+      <c r="A380" s="34"/>
     </row>
     <row r="381" spans="1:1" ht="13.2">
-      <c r="A381" s="35"/>
+      <c r="A381" s="34"/>
     </row>
     <row r="382" spans="1:1" ht="13.2">
-      <c r="A382" s="35"/>
+      <c r="A382" s="34"/>
     </row>
     <row r="383" spans="1:1" ht="13.2">
-      <c r="A383" s="35"/>
+      <c r="A383" s="34"/>
     </row>
     <row r="384" spans="1:1" ht="13.2">
-      <c r="A384" s="35"/>
+      <c r="A384" s="34"/>
     </row>
     <row r="385" spans="1:1" ht="13.2">
-      <c r="A385" s="35"/>
+      <c r="A385" s="34"/>
     </row>
     <row r="386" spans="1:1" ht="13.2">
-      <c r="A386" s="35"/>
+      <c r="A386" s="34"/>
     </row>
     <row r="387" spans="1:1" ht="13.2">
-      <c r="A387" s="35"/>
+      <c r="A387" s="34"/>
     </row>
     <row r="388" spans="1:1" ht="13.2">
-      <c r="A388" s="35"/>
+      <c r="A388" s="34"/>
     </row>
     <row r="389" spans="1:1" ht="13.2">
-      <c r="A389" s="35"/>
+      <c r="A389" s="34"/>
     </row>
     <row r="390" spans="1:1" ht="13.2">
-      <c r="A390" s="35"/>
+      <c r="A390" s="34"/>
     </row>
     <row r="391" spans="1:1" ht="13.2">
-      <c r="A391" s="35"/>
+      <c r="A391" s="34"/>
     </row>
     <row r="392" spans="1:1" ht="13.2">
-      <c r="A392" s="35"/>
+      <c r="A392" s="34"/>
     </row>
     <row r="393" spans="1:1" ht="13.2">
-      <c r="A393" s="35"/>
+      <c r="A393" s="34"/>
     </row>
     <row r="394" spans="1:1" ht="13.2">
-      <c r="A394" s="35"/>
+      <c r="A394" s="34"/>
     </row>
     <row r="395" spans="1:1" ht="13.2">
-      <c r="A395" s="35"/>
+      <c r="A395" s="34"/>
     </row>
     <row r="396" spans="1:1" ht="13.2">
-      <c r="A396" s="35"/>
+      <c r="A396" s="34"/>
     </row>
     <row r="397" spans="1:1" ht="13.2">
-      <c r="A397" s="35"/>
+      <c r="A397" s="34"/>
     </row>
     <row r="398" spans="1:1" ht="13.2">
-      <c r="A398" s="35"/>
+      <c r="A398" s="34"/>
     </row>
     <row r="399" spans="1:1" ht="13.2">
-      <c r="A399" s="35"/>
+      <c r="A399" s="34"/>
     </row>
     <row r="400" spans="1:1" ht="13.2">
-      <c r="A400" s="35"/>
+      <c r="A400" s="34"/>
     </row>
     <row r="401" spans="1:1" ht="13.2">
-      <c r="A401" s="35"/>
+      <c r="A401" s="34"/>
     </row>
     <row r="402" spans="1:1" ht="13.2">
-      <c r="A402" s="35"/>
+      <c r="A402" s="34"/>
     </row>
     <row r="403" spans="1:1" ht="13.2">
-      <c r="A403" s="35"/>
+      <c r="A403" s="34"/>
     </row>
     <row r="404" spans="1:1" ht="13.2">
-      <c r="A404" s="35"/>
+      <c r="A404" s="34"/>
     </row>
     <row r="405" spans="1:1" ht="13.2">
-      <c r="A405" s="35"/>
+      <c r="A405" s="34"/>
     </row>
     <row r="406" spans="1:1" ht="13.2">
-      <c r="A406" s="35"/>
+      <c r="A406" s="34"/>
     </row>
     <row r="407" spans="1:1" ht="13.2">
-      <c r="A407" s="35"/>
+      <c r="A407" s="34"/>
     </row>
     <row r="408" spans="1:1" ht="13.2">
-      <c r="A408" s="35"/>
+      <c r="A408" s="34"/>
     </row>
     <row r="409" spans="1:1" ht="13.2">
-      <c r="A409" s="35"/>
+      <c r="A409" s="34"/>
     </row>
     <row r="410" spans="1:1" ht="13.2">
-      <c r="A410" s="35"/>
+      <c r="A410" s="34"/>
     </row>
     <row r="411" spans="1:1" ht="13.2">
-      <c r="A411" s="35"/>
+      <c r="A411" s="34"/>
     </row>
     <row r="412" spans="1:1" ht="13.2">
-      <c r="A412" s="35"/>
+      <c r="A412" s="34"/>
     </row>
     <row r="413" spans="1:1" ht="13.2">
-      <c r="A413" s="35"/>
+      <c r="A413" s="34"/>
     </row>
     <row r="414" spans="1:1" ht="13.2">
-      <c r="A414" s="35"/>
+      <c r="A414" s="34"/>
     </row>
     <row r="415" spans="1:1" ht="13.2">
-      <c r="A415" s="35"/>
+      <c r="A415" s="34"/>
     </row>
     <row r="416" spans="1:1" ht="13.2">
-      <c r="A416" s="35"/>
+      <c r="A416" s="34"/>
     </row>
     <row r="417" spans="1:1" ht="13.2">
-      <c r="A417" s="35"/>
+      <c r="A417" s="34"/>
     </row>
     <row r="418" spans="1:1" ht="13.2">
-      <c r="A418" s="35"/>
+      <c r="A418" s="34"/>
     </row>
     <row r="419" spans="1:1" ht="13.2">
-      <c r="A419" s="35"/>
+      <c r="A419" s="34"/>
     </row>
     <row r="420" spans="1:1" ht="13.2">
-      <c r="A420" s="35"/>
+      <c r="A420" s="34"/>
     </row>
     <row r="421" spans="1:1" ht="13.2">
-      <c r="A421" s="35"/>
+      <c r="A421" s="34"/>
     </row>
     <row r="422" spans="1:1" ht="13.2">
-      <c r="A422" s="35"/>
+      <c r="A422" s="34"/>
     </row>
     <row r="423" spans="1:1" ht="13.2">
-      <c r="A423" s="35"/>
+      <c r="A423" s="34"/>
     </row>
     <row r="424" spans="1:1" ht="13.2">
-      <c r="A424" s="35"/>
+      <c r="A424" s="34"/>
     </row>
     <row r="425" spans="1:1" ht="13.2">
-      <c r="A425" s="35"/>
+      <c r="A425" s="34"/>
     </row>
     <row r="426" spans="1:1" ht="13.2">
-      <c r="A426" s="35"/>
+      <c r="A426" s="34"/>
     </row>
     <row r="427" spans="1:1" ht="13.2">
-      <c r="A427" s="35"/>
+      <c r="A427" s="34"/>
     </row>
     <row r="428" spans="1:1" ht="13.2">
-      <c r="A428" s="35"/>
+      <c r="A428" s="34"/>
     </row>
     <row r="429" spans="1:1" ht="13.2">
-      <c r="A429" s="35"/>
+      <c r="A429" s="34"/>
     </row>
     <row r="430" spans="1:1" ht="13.2">
-      <c r="A430" s="35"/>
+      <c r="A430" s="34"/>
     </row>
     <row r="431" spans="1:1" ht="13.2">
-      <c r="A431" s="35"/>
+      <c r="A431" s="34"/>
     </row>
     <row r="432" spans="1:1" ht="13.2">
-      <c r="A432" s="35"/>
+      <c r="A432" s="34"/>
     </row>
     <row r="433" spans="1:1" ht="13.2">
-      <c r="A433" s="35"/>
+      <c r="A433" s="34"/>
     </row>
     <row r="434" spans="1:1" ht="13.2">
-      <c r="A434" s="35"/>
+      <c r="A434" s="34"/>
     </row>
     <row r="435" spans="1:1" ht="13.2">
-      <c r="A435" s="35"/>
+      <c r="A435" s="34"/>
     </row>
     <row r="436" spans="1:1" ht="13.2">
-      <c r="A436" s="35"/>
+      <c r="A436" s="34"/>
     </row>
     <row r="437" spans="1:1" ht="13.2">
-      <c r="A437" s="35"/>
+      <c r="A437" s="34"/>
     </row>
     <row r="438" spans="1:1" ht="13.2">
-      <c r="A438" s="35"/>
+      <c r="A438" s="34"/>
     </row>
     <row r="439" spans="1:1" ht="13.2">
-      <c r="A439" s="35"/>
+      <c r="A439" s="34"/>
     </row>
     <row r="440" spans="1:1" ht="13.2">
-      <c r="A440" s="35"/>
+      <c r="A440" s="34"/>
     </row>
     <row r="441" spans="1:1" ht="13.2">
-      <c r="A441" s="35"/>
+      <c r="A441" s="34"/>
     </row>
     <row r="442" spans="1:1" ht="13.2">
-      <c r="A442" s="35"/>
+      <c r="A442" s="34"/>
     </row>
     <row r="443" spans="1:1" ht="13.2">
-      <c r="A443" s="35"/>
+      <c r="A443" s="34"/>
     </row>
     <row r="444" spans="1:1" ht="13.2">
-      <c r="A444" s="35"/>
+      <c r="A444" s="34"/>
     </row>
     <row r="445" spans="1:1" ht="13.2">
-      <c r="A445" s="35"/>
+      <c r="A445" s="34"/>
     </row>
     <row r="446" spans="1:1" ht="13.2">
-      <c r="A446" s="35"/>
+      <c r="A446" s="34"/>
     </row>
     <row r="447" spans="1:1" ht="13.2">
-      <c r="A447" s="35"/>
+      <c r="A447" s="34"/>
     </row>
     <row r="448" spans="1:1" ht="13.2">
-      <c r="A448" s="35"/>
+      <c r="A448" s="34"/>
     </row>
     <row r="449" spans="1:1" ht="13.2">
-      <c r="A449" s="35"/>
+      <c r="A449" s="34"/>
     </row>
     <row r="450" spans="1:1" ht="13.2">
-      <c r="A450" s="35"/>
+      <c r="A450" s="34"/>
     </row>
     <row r="451" spans="1:1" ht="13.2">
-      <c r="A451" s="35"/>
+      <c r="A451" s="34"/>
     </row>
     <row r="452" spans="1:1" ht="13.2">
-      <c r="A452" s="35"/>
+      <c r="A452" s="34"/>
     </row>
     <row r="453" spans="1:1" ht="13.2">
-      <c r="A453" s="35"/>
+      <c r="A453" s="34"/>
     </row>
     <row r="454" spans="1:1" ht="13.2">
-      <c r="A454" s="35"/>
+      <c r="A454" s="34"/>
     </row>
     <row r="455" spans="1:1" ht="13.2">
-      <c r="A455" s="35"/>
+      <c r="A455" s="34"/>
     </row>
     <row r="456" spans="1:1" ht="13.2">
-      <c r="A456" s="35"/>
+      <c r="A456" s="34"/>
     </row>
     <row r="457" spans="1:1" ht="13.2">
-      <c r="A457" s="35"/>
+      <c r="A457" s="34"/>
     </row>
     <row r="458" spans="1:1" ht="13.2">
-      <c r="A458" s="35"/>
+      <c r="A458" s="34"/>
     </row>
     <row r="459" spans="1:1" ht="13.2">
-      <c r="A459" s="35"/>
+      <c r="A459" s="34"/>
     </row>
     <row r="460" spans="1:1" ht="13.2">
-      <c r="A460" s="35"/>
+      <c r="A460" s="34"/>
     </row>
     <row r="461" spans="1:1" ht="13.2">
-      <c r="A461" s="35"/>
+      <c r="A461" s="34"/>
     </row>
     <row r="462" spans="1:1" ht="13.2">
-      <c r="A462" s="35"/>
+      <c r="A462" s="34"/>
     </row>
     <row r="463" spans="1:1" ht="13.2">
-      <c r="A463" s="35"/>
+      <c r="A463" s="34"/>
     </row>
     <row r="464" spans="1:1" ht="13.2">
-      <c r="A464" s="35"/>
+      <c r="A464" s="34"/>
     </row>
     <row r="465" spans="1:1" ht="13.2">
-      <c r="A465" s="35"/>
+      <c r="A465" s="34"/>
     </row>
     <row r="466" spans="1:1" ht="13.2">
-      <c r="A466" s="35"/>
+      <c r="A466" s="34"/>
     </row>
     <row r="467" spans="1:1" ht="13.2">
-      <c r="A467" s="35"/>
+      <c r="A467" s="34"/>
     </row>
     <row r="468" spans="1:1" ht="13.2">
-      <c r="A468" s="35"/>
+      <c r="A468" s="34"/>
     </row>
     <row r="469" spans="1:1" ht="13.2">
-      <c r="A469" s="35"/>
+      <c r="A469" s="34"/>
     </row>
     <row r="470" spans="1:1" ht="13.2">
-      <c r="A470" s="35"/>
+      <c r="A470" s="34"/>
     </row>
     <row r="471" spans="1:1" ht="13.2">
-      <c r="A471" s="35"/>
+      <c r="A471" s="34"/>
     </row>
     <row r="472" spans="1:1" ht="13.2">
-      <c r="A472" s="35"/>
+      <c r="A472" s="34"/>
     </row>
     <row r="473" spans="1:1" ht="13.2">
-      <c r="A473" s="35"/>
+      <c r="A473" s="34"/>
     </row>
     <row r="474" spans="1:1" ht="13.2">
-      <c r="A474" s="35"/>
+      <c r="A474" s="34"/>
     </row>
     <row r="475" spans="1:1" ht="13.2">
-      <c r="A475" s="35"/>
+      <c r="A475" s="34"/>
     </row>
     <row r="476" spans="1:1" ht="13.2">
-      <c r="A476" s="35"/>
+      <c r="A476" s="34"/>
     </row>
     <row r="477" spans="1:1" ht="13.2">
-      <c r="A477" s="35"/>
+      <c r="A477" s="34"/>
     </row>
     <row r="478" spans="1:1" ht="13.2">
-      <c r="A478" s="35"/>
+      <c r="A478" s="34"/>
     </row>
     <row r="479" spans="1:1" ht="13.2">
-      <c r="A479" s="35"/>
+      <c r="A479" s="34"/>
     </row>
     <row r="480" spans="1:1" ht="13.2">
-      <c r="A480" s="35"/>
+      <c r="A480" s="34"/>
     </row>
     <row r="481" spans="1:1" ht="13.2">
-      <c r="A481" s="35"/>
+      <c r="A481" s="34"/>
     </row>
     <row r="482" spans="1:1" ht="13.2">
-      <c r="A482" s="35"/>
+      <c r="A482" s="34"/>
     </row>
     <row r="483" spans="1:1" ht="13.2">
-      <c r="A483" s="35"/>
+      <c r="A483" s="34"/>
     </row>
     <row r="484" spans="1:1" ht="13.2">
-      <c r="A484" s="35"/>
+      <c r="A484" s="34"/>
     </row>
     <row r="485" spans="1:1" ht="13.2">
-      <c r="A485" s="35"/>
+      <c r="A485" s="34"/>
     </row>
     <row r="486" spans="1:1" ht="13.2">
-      <c r="A486" s="35"/>
+      <c r="A486" s="34"/>
     </row>
     <row r="487" spans="1:1" ht="13.2">
-      <c r="A487" s="35"/>
+      <c r="A487" s="34"/>
     </row>
     <row r="488" spans="1:1" ht="13.2">
-      <c r="A488" s="35"/>
+      <c r="A488" s="34"/>
     </row>
     <row r="489" spans="1:1" ht="13.2">
-      <c r="A489" s="35"/>
+      <c r="A489" s="34"/>
     </row>
     <row r="490" spans="1:1" ht="13.2">
-      <c r="A490" s="35"/>
+      <c r="A490" s="34"/>
     </row>
     <row r="491" spans="1:1" ht="13.2">
-      <c r="A491" s="35"/>
+      <c r="A491" s="34"/>
     </row>
     <row r="492" spans="1:1" ht="13.2">
-      <c r="A492" s="35"/>
+      <c r="A492" s="34"/>
     </row>
     <row r="493" spans="1:1" ht="13.2">
-      <c r="A493" s="35"/>
+      <c r="A493" s="34"/>
     </row>
     <row r="494" spans="1:1" ht="13.2">
-      <c r="A494" s="35"/>
+      <c r="A494" s="34"/>
     </row>
     <row r="495" spans="1:1" ht="13.2">
-      <c r="A495" s="35"/>
+      <c r="A495" s="34"/>
     </row>
     <row r="496" spans="1:1" ht="13.2">
-      <c r="A496" s="35"/>
+      <c r="A496" s="34"/>
     </row>
     <row r="497" spans="1:1" ht="13.2">
-      <c r="A497" s="35"/>
+      <c r="A497" s="34"/>
     </row>
     <row r="498" spans="1:1" ht="13.2">
-      <c r="A498" s="35"/>
+      <c r="A498" s="34"/>
     </row>
     <row r="499" spans="1:1" ht="13.2">
-      <c r="A499" s="35"/>
+      <c r="A499" s="34"/>
     </row>
     <row r="500" spans="1:1" ht="13.2">
-      <c r="A500" s="35"/>
+      <c r="A500" s="34"/>
     </row>
     <row r="501" spans="1:1" ht="13.2">
-      <c r="A501" s="35"/>
+      <c r="A501" s="34"/>
     </row>
     <row r="502" spans="1:1" ht="13.2">
-      <c r="A502" s="35"/>
+      <c r="A502" s="34"/>
     </row>
     <row r="503" spans="1:1" ht="13.2">
-      <c r="A503" s="35"/>
+      <c r="A503" s="34"/>
     </row>
     <row r="504" spans="1:1" ht="13.2">
-      <c r="A504" s="35"/>
+      <c r="A504" s="34"/>
     </row>
     <row r="505" spans="1:1" ht="13.2">
-      <c r="A505" s="35"/>
+      <c r="A505" s="34"/>
     </row>
     <row r="506" spans="1:1" ht="13.2">
-      <c r="A506" s="35"/>
+      <c r="A506" s="34"/>
     </row>
     <row r="507" spans="1:1" ht="13.2">
-      <c r="A507" s="35"/>
+      <c r="A507" s="34"/>
     </row>
     <row r="508" spans="1:1" ht="13.2">
-      <c r="A508" s="35"/>
+      <c r="A508" s="34"/>
     </row>
     <row r="509" spans="1:1" ht="13.2">
-      <c r="A509" s="35"/>
+      <c r="A509" s="34"/>
     </row>
     <row r="510" spans="1:1" ht="13.2">
-      <c r="A510" s="35"/>
+      <c r="A510" s="34"/>
     </row>
     <row r="511" spans="1:1" ht="13.2">
-      <c r="A511" s="35"/>
+      <c r="A511" s="34"/>
     </row>
     <row r="512" spans="1:1" ht="13.2">
-      <c r="A512" s="35"/>
+      <c r="A512" s="34"/>
     </row>
     <row r="513" spans="1:1" ht="13.2">
-      <c r="A513" s="35"/>
+      <c r="A513" s="34"/>
     </row>
     <row r="514" spans="1:1" ht="13.2">
-      <c r="A514" s="35"/>
+      <c r="A514" s="34"/>
     </row>
     <row r="515" spans="1:1" ht="13.2">
-      <c r="A515" s="35"/>
+      <c r="A515" s="34"/>
     </row>
     <row r="516" spans="1:1" ht="13.2">
-      <c r="A516" s="35"/>
+      <c r="A516" s="34"/>
     </row>
     <row r="517" spans="1:1" ht="13.2">
-      <c r="A517" s="35"/>
+      <c r="A517" s="34"/>
     </row>
     <row r="518" spans="1:1" ht="13.2">
-      <c r="A518" s="35"/>
+      <c r="A518" s="34"/>
     </row>
     <row r="519" spans="1:1" ht="13.2">
-      <c r="A519" s="35"/>
+      <c r="A519" s="34"/>
     </row>
     <row r="520" spans="1:1" ht="13.2">
-      <c r="A520" s="35"/>
+      <c r="A520" s="34"/>
     </row>
     <row r="521" spans="1:1" ht="13.2">
-      <c r="A521" s="35"/>
+      <c r="A521" s="34"/>
     </row>
     <row r="522" spans="1:1" ht="13.2">
-      <c r="A522" s="35"/>
+      <c r="A522" s="34"/>
     </row>
     <row r="523" spans="1:1" ht="13.2">
-      <c r="A523" s="35"/>
+      <c r="A523" s="34"/>
     </row>
     <row r="524" spans="1:1" ht="13.2">
-      <c r="A524" s="35"/>
+      <c r="A524" s="34"/>
     </row>
     <row r="525" spans="1:1" ht="13.2">
-      <c r="A525" s="35"/>
+      <c r="A525" s="34"/>
     </row>
     <row r="526" spans="1:1" ht="13.2">
-      <c r="A526" s="35"/>
+      <c r="A526" s="34"/>
     </row>
     <row r="527" spans="1:1" ht="13.2">
-      <c r="A527" s="35"/>
+      <c r="A527" s="34"/>
     </row>
     <row r="528" spans="1:1" ht="13.2">
-      <c r="A528" s="35"/>
+      <c r="A528" s="34"/>
     </row>
     <row r="529" spans="1:1" ht="13.2">
-      <c r="A529" s="35"/>
+      <c r="A529" s="34"/>
     </row>
     <row r="530" spans="1:1" ht="13.2">
-      <c r="A530" s="35"/>
+      <c r="A530" s="34"/>
     </row>
     <row r="531" spans="1:1" ht="13.2">
-      <c r="A531" s="35"/>
+      <c r="A531" s="34"/>
     </row>
     <row r="532" spans="1:1" ht="13.2">
-      <c r="A532" s="35"/>
+      <c r="A532" s="34"/>
     </row>
     <row r="533" spans="1:1" ht="13.2">
-      <c r="A533" s="35"/>
+      <c r="A533" s="34"/>
     </row>
     <row r="534" spans="1:1" ht="13.2">
-      <c r="A534" s="35"/>
+      <c r="A534" s="34"/>
     </row>
     <row r="535" spans="1:1" ht="13.2">
-      <c r="A535" s="35"/>
+      <c r="A535" s="34"/>
     </row>
     <row r="536" spans="1:1" ht="13.2">
-      <c r="A536" s="35"/>
+      <c r="A536" s="34"/>
     </row>
     <row r="537" spans="1:1" ht="13.2">
-      <c r="A537" s="35"/>
+      <c r="A537" s="34"/>
     </row>
     <row r="538" spans="1:1" ht="13.2">
-      <c r="A538" s="35"/>
+      <c r="A538" s="34"/>
     </row>
     <row r="539" spans="1:1" ht="13.2">
-      <c r="A539" s="35"/>
+      <c r="A539" s="34"/>
     </row>
     <row r="540" spans="1:1" ht="13.2">
-      <c r="A540" s="35"/>
+      <c r="A540" s="34"/>
     </row>
     <row r="541" spans="1:1" ht="13.2">
-      <c r="A541" s="35"/>
+      <c r="A541" s="34"/>
     </row>
     <row r="542" spans="1:1" ht="13.2">
-      <c r="A542" s="35"/>
+      <c r="A542" s="34"/>
     </row>
     <row r="543" spans="1:1" ht="13.2">
-      <c r="A543" s="35"/>
+      <c r="A543" s="34"/>
     </row>
     <row r="544" spans="1:1" ht="13.2">
-      <c r="A544" s="35"/>
+      <c r="A544" s="34"/>
     </row>
     <row r="545" spans="1:1" ht="13.2">
-      <c r="A545" s="35"/>
+      <c r="A545" s="34"/>
     </row>
     <row r="546" spans="1:1" ht="13.2">
-      <c r="A546" s="35"/>
+      <c r="A546" s="34"/>
     </row>
     <row r="547" spans="1:1" ht="13.2">
-      <c r="A547" s="35"/>
+      <c r="A547" s="34"/>
     </row>
     <row r="548" spans="1:1" ht="13.2">
-      <c r="A548" s="35"/>
+      <c r="A548" s="34"/>
     </row>
     <row r="549" spans="1:1" ht="13.2">
-      <c r="A549" s="35"/>
+      <c r="A549" s="34"/>
     </row>
     <row r="550" spans="1:1" ht="13.2">
-      <c r="A550" s="35"/>
+      <c r="A550" s="34"/>
     </row>
     <row r="551" spans="1:1" ht="13.2">
-      <c r="A551" s="35"/>
+      <c r="A551" s="34"/>
     </row>
     <row r="552" spans="1:1" ht="13.2">
-      <c r="A552" s="35"/>
+      <c r="A552" s="34"/>
     </row>
     <row r="553" spans="1:1" ht="13.2">
-      <c r="A553" s="35"/>
+      <c r="A553" s="34"/>
     </row>
     <row r="554" spans="1:1" ht="13.2">
-      <c r="A554" s="35"/>
+      <c r="A554" s="34"/>
     </row>
     <row r="555" spans="1:1" ht="13.2">
-      <c r="A555" s="35"/>
+      <c r="A555" s="34"/>
     </row>
     <row r="556" spans="1:1" ht="13.2">
-      <c r="A556" s="35"/>
+      <c r="A556" s="34"/>
     </row>
     <row r="557" spans="1:1" ht="13.2">
-      <c r="A557" s="35"/>
+      <c r="A557" s="34"/>
     </row>
     <row r="558" spans="1:1" ht="13.2">
-      <c r="A558" s="35"/>
+      <c r="A558" s="34"/>
     </row>
     <row r="559" spans="1:1" ht="13.2">
-      <c r="A559" s="35"/>
+      <c r="A559" s="34"/>
     </row>
     <row r="560" spans="1:1" ht="13.2">
-      <c r="A560" s="35"/>
+      <c r="A560" s="34"/>
     </row>
     <row r="561" spans="1:1" ht="13.2">
-      <c r="A561" s="35"/>
+      <c r="A561" s="34"/>
     </row>
     <row r="562" spans="1:1" ht="13.2">
-      <c r="A562" s="35"/>
+      <c r="A562" s="34"/>
     </row>
     <row r="563" spans="1:1" ht="13.2">
-      <c r="A563" s="35"/>
+      <c r="A563" s="34"/>
     </row>
     <row r="564" spans="1:1" ht="13.2">
-      <c r="A564" s="35"/>
+      <c r="A564" s="34"/>
     </row>
     <row r="565" spans="1:1" ht="13.2">
-      <c r="A565" s="35"/>
+      <c r="A565" s="34"/>
     </row>
     <row r="566" spans="1:1" ht="13.2">
-      <c r="A566" s="35"/>
+      <c r="A566" s="34"/>
     </row>
     <row r="567" spans="1:1" ht="13.2">
-      <c r="A567" s="35"/>
+      <c r="A567" s="34"/>
     </row>
     <row r="568" spans="1:1" ht="13.2">
-      <c r="A568" s="35"/>
+      <c r="A568" s="34"/>
     </row>
     <row r="569" spans="1:1" ht="13.2">
-      <c r="A569" s="35"/>
+      <c r="A569" s="34"/>
     </row>
     <row r="570" spans="1:1" ht="13.2">
-      <c r="A570" s="35"/>
+      <c r="A570" s="34"/>
     </row>
     <row r="571" spans="1:1" ht="13.2">
-      <c r="A571" s="35"/>
+      <c r="A571" s="34"/>
     </row>
     <row r="572" spans="1:1" ht="13.2">
-      <c r="A572" s="35"/>
+      <c r="A572" s="34"/>
     </row>
     <row r="573" spans="1:1" ht="13.2">
-      <c r="A573" s="35"/>
+      <c r="A573" s="34"/>
     </row>
     <row r="574" spans="1:1" ht="13.2">
-      <c r="A574" s="35"/>
+      <c r="A574" s="34"/>
     </row>
     <row r="575" spans="1:1" ht="13.2">
-      <c r="A575" s="35"/>
+      <c r="A575" s="34"/>
     </row>
     <row r="576" spans="1:1" ht="13.2">
-      <c r="A576" s="35"/>
+      <c r="A576" s="34"/>
     </row>
     <row r="577" spans="1:1" ht="13.2">
-      <c r="A577" s="35"/>
+      <c r="A577" s="34"/>
     </row>
     <row r="578" spans="1:1" ht="13.2">
-      <c r="A578" s="35"/>
+      <c r="A578" s="34"/>
     </row>
     <row r="579" spans="1:1" ht="13.2">
-      <c r="A579" s="35"/>
+      <c r="A579" s="34"/>
     </row>
     <row r="580" spans="1:1" ht="13.2">
-      <c r="A580" s="35"/>
+      <c r="A580" s="34"/>
     </row>
     <row r="581" spans="1:1" ht="13.2">
-      <c r="A581" s="35"/>
+      <c r="A581" s="34"/>
     </row>
     <row r="582" spans="1:1" ht="13.2">
-      <c r="A582" s="35"/>
+      <c r="A582" s="34"/>
     </row>
     <row r="583" spans="1:1" ht="13.2">
-      <c r="A583" s="35"/>
+      <c r="A583" s="34"/>
     </row>
     <row r="584" spans="1:1" ht="13.2">
-      <c r="A584" s="35"/>
+      <c r="A584" s="34"/>
     </row>
     <row r="585" spans="1:1" ht="13.2">
-      <c r="A585" s="35"/>
+      <c r="A585" s="34"/>
     </row>
     <row r="586" spans="1:1" ht="13.2">
-      <c r="A586" s="35"/>
+      <c r="A586" s="34"/>
     </row>
     <row r="587" spans="1:1" ht="13.2">
-      <c r="A587" s="35"/>
+      <c r="A587" s="34"/>
     </row>
     <row r="588" spans="1:1" ht="13.2">
-      <c r="A588" s="35"/>
+      <c r="A588" s="34"/>
     </row>
     <row r="589" spans="1:1" ht="13.2">
-      <c r="A589" s="35"/>
+      <c r="A589" s="34"/>
     </row>
     <row r="590" spans="1:1" ht="13.2">
-      <c r="A590" s="35"/>
+      <c r="A590" s="34"/>
     </row>
     <row r="591" spans="1:1" ht="13.2">
-      <c r="A591" s="35"/>
+      <c r="A591" s="34"/>
     </row>
     <row r="592" spans="1:1" ht="13.2">
-      <c r="A592" s="35"/>
+      <c r="A592" s="34"/>
     </row>
     <row r="593" spans="1:1" ht="13.2">
-      <c r="A593" s="35"/>
+      <c r="A593" s="34"/>
     </row>
     <row r="594" spans="1:1" ht="13.2">
-      <c r="A594" s="35"/>
+      <c r="A594" s="34"/>
     </row>
     <row r="595" spans="1:1" ht="13.2">
-      <c r="A595" s="35"/>
+      <c r="A595" s="34"/>
     </row>
     <row r="596" spans="1:1" ht="13.2">
-      <c r="A596" s="35"/>
+      <c r="A596" s="34"/>
     </row>
     <row r="597" spans="1:1" ht="13.2">
-      <c r="A597" s="35"/>
+      <c r="A597" s="34"/>
     </row>
     <row r="598" spans="1:1" ht="13.2">
-      <c r="A598" s="35"/>
+      <c r="A598" s="34"/>
     </row>
     <row r="599" spans="1:1" ht="13.2">
-      <c r="A599" s="35"/>
+      <c r="A599" s="34"/>
     </row>
     <row r="600" spans="1:1" ht="13.2">
-      <c r="A600" s="35"/>
+      <c r="A600" s="34"/>
     </row>
     <row r="601" spans="1:1" ht="13.2">
-      <c r="A601" s="35"/>
+      <c r="A601" s="34"/>
     </row>
     <row r="602" spans="1:1" ht="13.2">
-      <c r="A602" s="35"/>
+      <c r="A602" s="34"/>
     </row>
     <row r="603" spans="1:1" ht="13.2">
-      <c r="A603" s="35"/>
+      <c r="A603" s="34"/>
     </row>
     <row r="604" spans="1:1" ht="13.2">
-      <c r="A604" s="35"/>
+      <c r="A604" s="34"/>
     </row>
     <row r="605" spans="1:1" ht="13.2">
-      <c r="A605" s="35"/>
+      <c r="A605" s="34"/>
     </row>
     <row r="606" spans="1:1" ht="13.2">
-      <c r="A606" s="35"/>
+      <c r="A606" s="34"/>
     </row>
     <row r="607" spans="1:1" ht="13.2">
-      <c r="A607" s="35"/>
+      <c r="A607" s="34"/>
     </row>
     <row r="608" spans="1:1" ht="13.2">
-      <c r="A608" s="35"/>
+      <c r="A608" s="34"/>
     </row>
     <row r="609" spans="1:1" ht="13.2">
-      <c r="A609" s="35"/>
+      <c r="A609" s="34"/>
     </row>
     <row r="610" spans="1:1" ht="13.2">
-      <c r="A610" s="35"/>
+      <c r="A610" s="34"/>
     </row>
     <row r="611" spans="1:1" ht="13.2">
-      <c r="A611" s="35"/>
+      <c r="A611" s="34"/>
     </row>
     <row r="612" spans="1:1" ht="13.2">
-      <c r="A612" s="35"/>
+      <c r="A612" s="34"/>
     </row>
     <row r="613" spans="1:1" ht="13.2">
-      <c r="A613" s="35"/>
+      <c r="A613" s="34"/>
     </row>
     <row r="614" spans="1:1" ht="13.2">
-      <c r="A614" s="35"/>
+      <c r="A614" s="34"/>
     </row>
     <row r="615" spans="1:1" ht="13.2">
-      <c r="A615" s="35"/>
+      <c r="A615" s="34"/>
     </row>
     <row r="616" spans="1:1" ht="13.2">
-      <c r="A616" s="35"/>
+      <c r="A616" s="34"/>
     </row>
     <row r="617" spans="1:1" ht="13.2">
-      <c r="A617" s="35"/>
+      <c r="A617" s="34"/>
     </row>
     <row r="618" spans="1:1" ht="13.2">
-      <c r="A618" s="35"/>
+      <c r="A618" s="34"/>
     </row>
     <row r="619" spans="1:1" ht="13.2">
-      <c r="A619" s="35"/>
+      <c r="A619" s="34"/>
     </row>
     <row r="620" spans="1:1" ht="13.2">
-      <c r="A620" s="35"/>
+      <c r="A620" s="34"/>
     </row>
     <row r="621" spans="1:1" ht="13.2">
-      <c r="A621" s="35"/>
+      <c r="A621" s="34"/>
     </row>
     <row r="622" spans="1:1" ht="13.2">
-      <c r="A622" s="35"/>
+      <c r="A622" s="34"/>
     </row>
     <row r="623" spans="1:1" ht="13.2">
-      <c r="A623" s="35"/>
+      <c r="A623" s="34"/>
     </row>
     <row r="624" spans="1:1" ht="13.2">
-      <c r="A624" s="35"/>
+      <c r="A624" s="34"/>
     </row>
     <row r="625" spans="1:1" ht="13.2">
-      <c r="A625" s="35"/>
+      <c r="A625" s="34"/>
     </row>
     <row r="626" spans="1:1" ht="13.2">
-      <c r="A626" s="35"/>
+      <c r="A626" s="34"/>
     </row>
     <row r="627" spans="1:1" ht="13.2">
-      <c r="A627" s="35"/>
+      <c r="A627" s="34"/>
     </row>
     <row r="628" spans="1:1" ht="13.2">
-      <c r="A628" s="35"/>
+      <c r="A628" s="34"/>
     </row>
     <row r="629" spans="1:1" ht="13.2">
-      <c r="A629" s="35"/>
+      <c r="A629" s="34"/>
     </row>
     <row r="630" spans="1:1" ht="13.2">
-      <c r="A630" s="35"/>
+      <c r="A630" s="34"/>
     </row>
     <row r="631" spans="1:1" ht="13.2">
-      <c r="A631" s="35"/>
+      <c r="A631" s="34"/>
     </row>
     <row r="632" spans="1:1" ht="13.2">
-      <c r="A632" s="35"/>
+      <c r="A632" s="34"/>
     </row>
     <row r="633" spans="1:1" ht="13.2">
-      <c r="A633" s="35"/>
+      <c r="A633" s="34"/>
     </row>
     <row r="634" spans="1:1" ht="13.2">
-      <c r="A634" s="35"/>
+      <c r="A634" s="34"/>
     </row>
     <row r="635" spans="1:1" ht="13.2">
-      <c r="A635" s="35"/>
+      <c r="A635" s="34"/>
     </row>
     <row r="636" spans="1:1" ht="13.2">
-      <c r="A636" s="35"/>
+      <c r="A636" s="34"/>
     </row>
     <row r="637" spans="1:1" ht="13.2">
-      <c r="A637" s="35"/>
+      <c r="A637" s="34"/>
     </row>
     <row r="638" spans="1:1" ht="13.2">
-      <c r="A638" s="35"/>
+      <c r="A638" s="34"/>
     </row>
     <row r="639" spans="1:1" ht="13.2">
-      <c r="A639" s="35"/>
+      <c r="A639" s="34"/>
     </row>
     <row r="640" spans="1:1" ht="13.2">
-      <c r="A640" s="35"/>
+      <c r="A640" s="34"/>
     </row>
     <row r="641" spans="1:1" ht="13.2">
-      <c r="A641" s="35"/>
+      <c r="A641" s="34"/>
     </row>
     <row r="642" spans="1:1" ht="13.2">
-      <c r="A642" s="35"/>
+      <c r="A642" s="34"/>
     </row>
     <row r="643" spans="1:1" ht="13.2">
-      <c r="A643" s="35"/>
+      <c r="A643" s="34"/>
     </row>
     <row r="644" spans="1:1" ht="13.2">
-      <c r="A644" s="35"/>
+      <c r="A644" s="34"/>
     </row>
     <row r="645" spans="1:1" ht="13.2">
-      <c r="A645" s="35"/>
+      <c r="A645" s="34"/>
     </row>
     <row r="646" spans="1:1" ht="13.2">
-      <c r="A646" s="35"/>
+      <c r="A646" s="34"/>
     </row>
     <row r="647" spans="1:1" ht="13.2">
-      <c r="A647" s="35"/>
+      <c r="A647" s="34"/>
     </row>
     <row r="648" spans="1:1" ht="13.2">
-      <c r="A648" s="35"/>
+      <c r="A648" s="34"/>
     </row>
     <row r="649" spans="1:1" ht="13.2">
-      <c r="A649" s="35"/>
+      <c r="A649" s="34"/>
     </row>
     <row r="650" spans="1:1" ht="13.2">
-      <c r="A650" s="35"/>
+      <c r="A650" s="34"/>
     </row>
     <row r="651" spans="1:1" ht="13.2">
-      <c r="A651" s="35"/>
+      <c r="A651" s="34"/>
     </row>
     <row r="652" spans="1:1" ht="13.2">
-      <c r="A652" s="35"/>
+      <c r="A652" s="34"/>
     </row>
     <row r="653" spans="1:1" ht="13.2">
-      <c r="A653" s="35"/>
+      <c r="A653" s="34"/>
     </row>
     <row r="654" spans="1:1" ht="13.2">
-      <c r="A654" s="35"/>
+      <c r="A654" s="34"/>
     </row>
     <row r="655" spans="1:1" ht="13.2">
-      <c r="A655" s="35"/>
+      <c r="A655" s="34"/>
     </row>
     <row r="656" spans="1:1" ht="13.2">
-      <c r="A656" s="35"/>
+      <c r="A656" s="34"/>
     </row>
     <row r="657" spans="1:1" ht="13.2">
-      <c r="A657" s="35"/>
+      <c r="A657" s="34"/>
     </row>
     <row r="658" spans="1:1" ht="13.2">
-      <c r="A658" s="35"/>
+      <c r="A658" s="34"/>
     </row>
     <row r="659" spans="1:1" ht="13.2">
-      <c r="A659" s="35"/>
+      <c r="A659" s="34"/>
     </row>
     <row r="660" spans="1:1" ht="13.2">
-      <c r="A660" s="35"/>
+      <c r="A660" s="34"/>
     </row>
     <row r="661" spans="1:1" ht="13.2">
-      <c r="A661" s="35"/>
+      <c r="A661" s="34"/>
     </row>
     <row r="662" spans="1:1" ht="13.2">
-      <c r="A662" s="35"/>
+      <c r="A662" s="34"/>
     </row>
     <row r="663" spans="1:1" ht="13.2">
-      <c r="A663" s="35"/>
+      <c r="A663" s="34"/>
     </row>
     <row r="664" spans="1:1" ht="13.2">
-      <c r="A664" s="35"/>
+      <c r="A664" s="34"/>
     </row>
     <row r="665" spans="1:1" ht="13.2">
-      <c r="A665" s="35"/>
+      <c r="A665" s="34"/>
     </row>
     <row r="666" spans="1:1" ht="13.2">
-      <c r="A666" s="35"/>
+      <c r="A666" s="34"/>
     </row>
     <row r="667" spans="1:1" ht="13.2">
-      <c r="A667" s="35"/>
+      <c r="A667" s="34"/>
     </row>
     <row r="668" spans="1:1" ht="13.2">
-      <c r="A668" s="35"/>
+      <c r="A668" s="34"/>
     </row>
     <row r="669" spans="1:1" ht="13.2">
-      <c r="A669" s="35"/>
+      <c r="A669" s="34"/>
     </row>
     <row r="670" spans="1:1" ht="13.2">
-      <c r="A670" s="35"/>
+      <c r="A670" s="34"/>
     </row>
     <row r="671" spans="1:1" ht="13.2">
-      <c r="A671" s="35"/>
+      <c r="A671" s="34"/>
     </row>
     <row r="672" spans="1:1" ht="13.2">
-      <c r="A672" s="35"/>
+      <c r="A672" s="34"/>
     </row>
     <row r="673" spans="1:1" ht="13.2">
-      <c r="A673" s="35"/>
+      <c r="A673" s="34"/>
     </row>
     <row r="674" spans="1:1" ht="13.2">
-      <c r="A674" s="35"/>
+      <c r="A674" s="34"/>
     </row>
     <row r="675" spans="1:1" ht="13.2">
-      <c r="A675" s="35"/>
+      <c r="A675" s="34"/>
     </row>
     <row r="676" spans="1:1" ht="13.2">
-      <c r="A676" s="35"/>
+      <c r="A676" s="34"/>
     </row>
     <row r="677" spans="1:1" ht="13.2">
-      <c r="A677" s="35"/>
+      <c r="A677" s="34"/>
     </row>
     <row r="678" spans="1:1" ht="13.2">
-      <c r="A678" s="35"/>
+      <c r="A678" s="34"/>
     </row>
     <row r="679" spans="1:1" ht="13.2">
-      <c r="A679" s="35"/>
+      <c r="A679" s="34"/>
     </row>
     <row r="680" spans="1:1" ht="13.2">
-      <c r="A680" s="35"/>
+      <c r="A680" s="34"/>
     </row>
     <row r="681" spans="1:1" ht="13.2">
-      <c r="A681" s="35"/>
+      <c r="A681" s="34"/>
     </row>
     <row r="682" spans="1:1" ht="13.2">
-      <c r="A682" s="35"/>
+      <c r="A682" s="34"/>
     </row>
     <row r="683" spans="1:1" ht="13.2">
-      <c r="A683" s="35"/>
+      <c r="A683" s="34"/>
     </row>
     <row r="684" spans="1:1" ht="13.2">
-      <c r="A684" s="35"/>
+      <c r="A684" s="34"/>
     </row>
     <row r="685" spans="1:1" ht="13.2">
-      <c r="A685" s="35"/>
+      <c r="A685" s="34"/>
     </row>
     <row r="686" spans="1:1" ht="13.2">
-      <c r="A686" s="35"/>
+      <c r="A686" s="34"/>
     </row>
     <row r="687" spans="1:1" ht="13.2">
-      <c r="A687" s="35"/>
+      <c r="A687" s="34"/>
     </row>
     <row r="688" spans="1:1" ht="13.2">
-      <c r="A688" s="35"/>
+      <c r="A688" s="34"/>
     </row>
     <row r="689" spans="1:1" ht="13.2">
-      <c r="A689" s="35"/>
+      <c r="A689" s="34"/>
     </row>
     <row r="690" spans="1:1" ht="13.2">
-      <c r="A690" s="35"/>
+      <c r="A690" s="34"/>
     </row>
     <row r="691" spans="1:1" ht="13.2">
-      <c r="A691" s="35"/>
+      <c r="A691" s="34"/>
     </row>
     <row r="692" spans="1:1" ht="13.2">
-      <c r="A692" s="35"/>
+      <c r="A692" s="34"/>
     </row>
     <row r="693" spans="1:1" ht="13.2">
-      <c r="A693" s="35"/>
+      <c r="A693" s="34"/>
     </row>
     <row r="694" spans="1:1" ht="13.2">
-      <c r="A694" s="35"/>
+      <c r="A694" s="34"/>
     </row>
     <row r="695" spans="1:1" ht="13.2">
-      <c r="A695" s="35"/>
+      <c r="A695" s="34"/>
     </row>
     <row r="696" spans="1:1" ht="13.2">
-      <c r="A696" s="35"/>
+      <c r="A696" s="34"/>
     </row>
     <row r="697" spans="1:1" ht="13.2">
-      <c r="A697" s="35"/>
+      <c r="A697" s="34"/>
     </row>
     <row r="698" spans="1:1" ht="13.2">
-      <c r="A698" s="35"/>
+      <c r="A698" s="34"/>
     </row>
     <row r="699" spans="1:1" ht="13.2">
-      <c r="A699" s="35"/>
+      <c r="A699" s="34"/>
     </row>
     <row r="700" spans="1:1" ht="13.2">
-      <c r="A700" s="35"/>
+      <c r="A700" s="34"/>
     </row>
     <row r="701" spans="1:1" ht="13.2">
-      <c r="A701" s="35"/>
+      <c r="A701" s="34"/>
     </row>
     <row r="702" spans="1:1" ht="13.2">
-      <c r="A702" s="35"/>
+      <c r="A702" s="34"/>
     </row>
     <row r="703" spans="1:1" ht="13.2">
-      <c r="A703" s="35"/>
+      <c r="A703" s="34"/>
     </row>
     <row r="704" spans="1:1" ht="13.2">
-      <c r="A704" s="35"/>
+      <c r="A704" s="34"/>
     </row>
     <row r="705" spans="1:1" ht="13.2">
-      <c r="A705" s="35"/>
+      <c r="A705" s="34"/>
     </row>
     <row r="706" spans="1:1" ht="13.2">
-      <c r="A706" s="35"/>
+      <c r="A706" s="34"/>
     </row>
     <row r="707" spans="1:1" ht="13.2">
-      <c r="A707" s="35"/>
+      <c r="A707" s="34"/>
     </row>
     <row r="708" spans="1:1" ht="13.2">
-      <c r="A708" s="35"/>
+      <c r="A708" s="34"/>
     </row>
     <row r="709" spans="1:1" ht="13.2">
-      <c r="A709" s="35"/>
+      <c r="A709" s="34"/>
     </row>
     <row r="710" spans="1:1" ht="13.2">
-      <c r="A710" s="35"/>
+      <c r="A710" s="34"/>
     </row>
     <row r="711" spans="1:1" ht="13.2">
-      <c r="A711" s="35"/>
+      <c r="A711" s="34"/>
     </row>
     <row r="712" spans="1:1" ht="13.2">
-      <c r="A712" s="35"/>
+      <c r="A712" s="34"/>
     </row>
     <row r="713" spans="1:1" ht="13.2">
-      <c r="A713" s="35"/>
+      <c r="A713" s="34"/>
     </row>
     <row r="714" spans="1:1" ht="13.2">
-      <c r="A714" s="35"/>
+      <c r="A714" s="34"/>
     </row>
     <row r="715" spans="1:1" ht="13.2">
-      <c r="A715" s="35"/>
+      <c r="A715" s="34"/>
     </row>
     <row r="716" spans="1:1" ht="13.2">
-      <c r="A716" s="35"/>
+      <c r="A716" s="34"/>
     </row>
     <row r="717" spans="1:1" ht="13.2">
-      <c r="A717" s="35"/>
+      <c r="A717" s="34"/>
     </row>
     <row r="718" spans="1:1" ht="13.2">
-      <c r="A718" s="35"/>
+      <c r="A718" s="34"/>
     </row>
     <row r="719" spans="1:1" ht="13.2">
-      <c r="A719" s="35"/>
+      <c r="A719" s="34"/>
     </row>
     <row r="720" spans="1:1" ht="13.2">
-      <c r="A720" s="35"/>
+      <c r="A720" s="34"/>
     </row>
     <row r="721" spans="1:1" ht="13.2">
-      <c r="A721" s="35"/>
+      <c r="A721" s="34"/>
     </row>
     <row r="722" spans="1:1" ht="13.2">
-      <c r="A722" s="35"/>
+      <c r="A722" s="34"/>
     </row>
     <row r="723" spans="1:1" ht="13.2">
-      <c r="A723" s="35"/>
+      <c r="A723" s="34"/>
     </row>
     <row r="724" spans="1:1" ht="13.2">
-      <c r="A724" s="35"/>
+      <c r="A724" s="34"/>
     </row>
     <row r="725" spans="1:1" ht="13.2">
-      <c r="A725" s="35"/>
+      <c r="A725" s="34"/>
     </row>
     <row r="726" spans="1:1" ht="13.2">
-      <c r="A726" s="35"/>
+      <c r="A726" s="34"/>
     </row>
     <row r="727" spans="1:1" ht="13.2">
-      <c r="A727" s="35"/>
+      <c r="A727" s="34"/>
     </row>
     <row r="728" spans="1:1" ht="13.2">
-      <c r="A728" s="35"/>
+      <c r="A728" s="34"/>
     </row>
     <row r="729" spans="1:1" ht="13.2">
-      <c r="A729" s="35"/>
+      <c r="A729" s="34"/>
     </row>
     <row r="730" spans="1:1" ht="13.2">
-      <c r="A730" s="35"/>
+      <c r="A730" s="34"/>
     </row>
     <row r="731" spans="1:1" ht="13.2">
-      <c r="A731" s="35"/>
+      <c r="A731" s="34"/>
     </row>
     <row r="732" spans="1:1" ht="13.2">
-      <c r="A732" s="35"/>
+      <c r="A732" s="34"/>
     </row>
     <row r="733" spans="1:1" ht="13.2">
-      <c r="A733" s="35"/>
+      <c r="A733" s="34"/>
     </row>
     <row r="734" spans="1:1" ht="13.2">
-      <c r="A734" s="35"/>
+      <c r="A734" s="34"/>
     </row>
     <row r="735" spans="1:1" ht="13.2">
-      <c r="A735" s="35"/>
+      <c r="A735" s="34"/>
     </row>
     <row r="736" spans="1:1" ht="13.2">
-      <c r="A736" s="35"/>
+      <c r="A736" s="34"/>
     </row>
     <row r="737" spans="1:1" ht="13.2">
-      <c r="A737" s="35"/>
+      <c r="A737" s="34"/>
     </row>
     <row r="738" spans="1:1" ht="13.2">
-      <c r="A738" s="35"/>
+      <c r="A738" s="34"/>
     </row>
     <row r="739" spans="1:1" ht="13.2">
-      <c r="A739" s="35"/>
+      <c r="A739" s="34"/>
     </row>
     <row r="740" spans="1:1" ht="13.2">
-      <c r="A740" s="35"/>
+      <c r="A740" s="34"/>
     </row>
     <row r="741" spans="1:1" ht="13.2">
-      <c r="A741" s="35"/>
+      <c r="A741" s="34"/>
     </row>
     <row r="742" spans="1:1" ht="13.2">
-      <c r="A742" s="35"/>
+      <c r="A742" s="34"/>
     </row>
     <row r="743" spans="1:1" ht="13.2">
-      <c r="A743" s="35"/>
+      <c r="A743" s="34"/>
     </row>
     <row r="744" spans="1:1" ht="13.2">
-      <c r="A744" s="35"/>
+      <c r="A744" s="34"/>
     </row>
     <row r="745" spans="1:1" ht="13.2">
-      <c r="A745" s="35"/>
+      <c r="A745" s="34"/>
     </row>
     <row r="746" spans="1:1" ht="13.2">
-      <c r="A746" s="35"/>
+      <c r="A746" s="34"/>
     </row>
     <row r="747" spans="1:1" ht="13.2">
-      <c r="A747" s="35"/>
+      <c r="A747" s="34"/>
     </row>
     <row r="748" spans="1:1" ht="13.2">
-      <c r="A748" s="35"/>
+      <c r="A748" s="34"/>
     </row>
     <row r="749" spans="1:1" ht="13.2">
-      <c r="A749" s="35"/>
+      <c r="A749" s="34"/>
     </row>
     <row r="750" spans="1:1" ht="13.2">
-      <c r="A750" s="35"/>
+      <c r="A750" s="34"/>
     </row>
     <row r="751" spans="1:1" ht="13.2">
-      <c r="A751" s="35"/>
+      <c r="A751" s="34"/>
     </row>
     <row r="752" spans="1:1" ht="13.2">
-      <c r="A752" s="35"/>
+      <c r="A752" s="34"/>
     </row>
     <row r="753" spans="1:1" ht="13.2">
-      <c r="A753" s="35"/>
+      <c r="A753" s="34"/>
     </row>
     <row r="754" spans="1:1" ht="13.2">
-      <c r="A754" s="35"/>
+      <c r="A754" s="34"/>
     </row>
     <row r="755" spans="1:1" ht="13.2">
-      <c r="A755" s="35"/>
+      <c r="A755" s="34"/>
     </row>
     <row r="756" spans="1:1" ht="13.2">
-      <c r="A756" s="35"/>
+      <c r="A756" s="34"/>
     </row>
     <row r="757" spans="1:1" ht="13.2">
-      <c r="A757" s="35"/>
+      <c r="A757" s="34"/>
     </row>
     <row r="758" spans="1:1" ht="13.2">
-      <c r="A758" s="35"/>
+      <c r="A758" s="34"/>
     </row>
     <row r="759" spans="1:1" ht="13.2">
-      <c r="A759" s="35"/>
+      <c r="A759" s="34"/>
     </row>
     <row r="760" spans="1:1" ht="13.2">
-      <c r="A760" s="35"/>
+      <c r="A760" s="34"/>
     </row>
     <row r="761" spans="1:1" ht="13.2">
-      <c r="A761" s="35"/>
+      <c r="A761" s="34"/>
     </row>
     <row r="762" spans="1:1" ht="13.2">
-      <c r="A762" s="35"/>
+      <c r="A762" s="34"/>
     </row>
     <row r="763" spans="1:1" ht="13.2">
-      <c r="A763" s="35"/>
+      <c r="A763" s="34"/>
     </row>
     <row r="764" spans="1:1" ht="13.2">
-      <c r="A764" s="35"/>
+      <c r="A764" s="34"/>
     </row>
     <row r="765" spans="1:1" ht="13.2">
-      <c r="A765" s="35"/>
+      <c r="A765" s="34"/>
     </row>
     <row r="766" spans="1:1" ht="13.2">
-      <c r="A766" s="35"/>
+      <c r="A766" s="34"/>
     </row>
     <row r="767" spans="1:1" ht="13.2">
-      <c r="A767" s="35"/>
+      <c r="A767" s="34"/>
     </row>
     <row r="768" spans="1:1" ht="13.2">
-      <c r="A768" s="35"/>
+      <c r="A768" s="34"/>
     </row>
     <row r="769" spans="1:1" ht="13.2">
-      <c r="A769" s="35"/>
+      <c r="A769" s="34"/>
     </row>
     <row r="770" spans="1:1" ht="13.2">
-      <c r="A770" s="35"/>
+      <c r="A770" s="34"/>
     </row>
     <row r="771" spans="1:1" ht="13.2">
-      <c r="A771" s="35"/>
+      <c r="A771" s="34"/>
     </row>
     <row r="772" spans="1:1" ht="13.2">
-      <c r="A772" s="35"/>
+      <c r="A772" s="34"/>
     </row>
     <row r="773" spans="1:1" ht="13.2">
-      <c r="A773" s="35"/>
+      <c r="A773" s="34"/>
     </row>
     <row r="774" spans="1:1" ht="13.2">
-      <c r="A774" s="35"/>
+      <c r="A774" s="34"/>
     </row>
     <row r="775" spans="1:1" ht="13.2">
-      <c r="A775" s="35"/>
+      <c r="A775" s="34"/>
     </row>
     <row r="776" spans="1:1" ht="13.2">
-      <c r="A776" s="35"/>
+      <c r="A776" s="34"/>
     </row>
     <row r="777" spans="1:1" ht="13.2">
-      <c r="A777" s="35"/>
+      <c r="A777" s="34"/>
     </row>
     <row r="778" spans="1:1" ht="13.2">
-      <c r="A778" s="35"/>
+      <c r="A778" s="34"/>
     </row>
     <row r="779" spans="1:1" ht="13.2">
-      <c r="A779" s="35"/>
+      <c r="A779" s="34"/>
     </row>
     <row r="780" spans="1:1" ht="13.2">
-      <c r="A780" s="35"/>
+      <c r="A780" s="34"/>
     </row>
     <row r="781" spans="1:1" ht="13.2">
-      <c r="A781" s="35"/>
+      <c r="A781" s="34"/>
     </row>
     <row r="782" spans="1:1" ht="13.2">
-      <c r="A782" s="35"/>
+      <c r="A782" s="34"/>
     </row>
     <row r="783" spans="1:1" ht="13.2">
-      <c r="A783" s="35"/>
+      <c r="A783" s="34"/>
     </row>
     <row r="784" spans="1:1" ht="13.2">
-      <c r="A784" s="35"/>
+      <c r="A784" s="34"/>
     </row>
     <row r="785" spans="1:1" ht="13.2">
-      <c r="A785" s="35"/>
+      <c r="A785" s="34"/>
     </row>
     <row r="786" spans="1:1" ht="13.2">
-      <c r="A786" s="35"/>
+      <c r="A786" s="34"/>
     </row>
     <row r="787" spans="1:1" ht="13.2">
-      <c r="A787" s="35"/>
+      <c r="A787" s="34"/>
     </row>
     <row r="788" spans="1:1" ht="13.2">
-      <c r="A788" s="35"/>
+      <c r="A788" s="34"/>
     </row>
     <row r="789" spans="1:1" ht="13.2">
-      <c r="A789" s="35"/>
+      <c r="A789" s="34"/>
     </row>
     <row r="790" spans="1:1" ht="13.2">
-      <c r="A790" s="35"/>
+      <c r="A790" s="34"/>
     </row>
     <row r="791" spans="1:1" ht="13.2">
-      <c r="A791" s="35"/>
+      <c r="A791" s="34"/>
     </row>
     <row r="792" spans="1:1" ht="13.2">
-      <c r="A792" s="35"/>
+      <c r="A792" s="34"/>
     </row>
     <row r="793" spans="1:1" ht="13.2">
-      <c r="A793" s="35"/>
+      <c r="A793" s="34"/>
     </row>
     <row r="794" spans="1:1" ht="13.2">
-      <c r="A794" s="35"/>
+      <c r="A794" s="34"/>
     </row>
     <row r="795" spans="1:1" ht="13.2">
-      <c r="A795" s="35"/>
+      <c r="A795" s="34"/>
     </row>
     <row r="796" spans="1:1" ht="13.2">
-      <c r="A796" s="35"/>
+      <c r="A796" s="34"/>
     </row>
     <row r="797" spans="1:1" ht="13.2">
-      <c r="A797" s="35"/>
+      <c r="A797" s="34"/>
     </row>
     <row r="798" spans="1:1" ht="13.2">
-      <c r="A798" s="35"/>
+      <c r="A798" s="34"/>
     </row>
     <row r="799" spans="1:1" ht="13.2">
-      <c r="A799" s="35"/>
+      <c r="A799" s="34"/>
     </row>
     <row r="800" spans="1:1" ht="13.2">
-      <c r="A800" s="35"/>
+      <c r="A800" s="34"/>
     </row>
     <row r="801" spans="1:1" ht="13.2">
-      <c r="A801" s="35"/>
+      <c r="A801" s="34"/>
     </row>
     <row r="802" spans="1:1" ht="13.2">
-      <c r="A802" s="35"/>
+      <c r="A802" s="34"/>
     </row>
     <row r="803" spans="1:1" ht="13.2">
-      <c r="A803" s="35"/>
+      <c r="A803" s="34"/>
     </row>
     <row r="804" spans="1:1" ht="13.2">
-      <c r="A804" s="35"/>
+      <c r="A804" s="34"/>
     </row>
     <row r="805" spans="1:1" ht="13.2">
-      <c r="A805" s="35"/>
+      <c r="A805" s="34"/>
     </row>
     <row r="806" spans="1:1" ht="13.2">
-      <c r="A806" s="35"/>
+      <c r="A806" s="34"/>
     </row>
     <row r="807" spans="1:1" ht="13.2">
-      <c r="A807" s="35"/>
+      <c r="A807" s="34"/>
     </row>
     <row r="808" spans="1:1" ht="13.2">
-      <c r="A808" s="35"/>
+      <c r="A808" s="34"/>
     </row>
     <row r="809" spans="1:1" ht="13.2">
-      <c r="A809" s="35"/>
+      <c r="A809" s="34"/>
     </row>
     <row r="810" spans="1:1" ht="13.2">
-      <c r="A810" s="35"/>
+      <c r="A810" s="34"/>
     </row>
     <row r="811" spans="1:1" ht="13.2">
-      <c r="A811" s="35"/>
+      <c r="A811" s="34"/>
     </row>
     <row r="812" spans="1:1" ht="13.2">
-      <c r="A812" s="35"/>
+      <c r="A812" s="34"/>
     </row>
     <row r="813" spans="1:1" ht="13.2">
-      <c r="A813" s="35"/>
+      <c r="A813" s="34"/>
     </row>
     <row r="814" spans="1:1" ht="13.2">
-      <c r="A814" s="35"/>
+      <c r="A814" s="34"/>
     </row>
     <row r="815" spans="1:1" ht="13.2">
-      <c r="A815" s="35"/>
+      <c r="A815" s="34"/>
     </row>
     <row r="816" spans="1:1" ht="13.2">
-      <c r="A816" s="35"/>
+      <c r="A816" s="34"/>
     </row>
     <row r="817" spans="1:1" ht="13.2">
-      <c r="A817" s="35"/>
+      <c r="A817" s="34"/>
     </row>
     <row r="818" spans="1:1" ht="13.2">
-      <c r="A818" s="35"/>
+      <c r="A818" s="34"/>
     </row>
     <row r="819" spans="1:1" ht="13.2">
-      <c r="A819" s="35"/>
+      <c r="A819" s="34"/>
     </row>
     <row r="820" spans="1:1" ht="13.2">
-      <c r="A820" s="35"/>
+      <c r="A820" s="34"/>
     </row>
     <row r="821" spans="1:1" ht="13.2">
-      <c r="A821" s="35"/>
+      <c r="A821" s="34"/>
     </row>
     <row r="822" spans="1:1" ht="13.2">
-      <c r="A822" s="35"/>
+      <c r="A822" s="34"/>
     </row>
     <row r="823" spans="1:1" ht="13.2">
-      <c r="A823" s="35"/>
+      <c r="A823" s="34"/>
     </row>
     <row r="824" spans="1:1" ht="13.2">
-      <c r="A824" s="35"/>
+      <c r="A824" s="34"/>
     </row>
     <row r="825" spans="1:1" ht="13.2">
-      <c r="A825" s="35"/>
+      <c r="A825" s="34"/>
     </row>
     <row r="826" spans="1:1" ht="13.2">
-      <c r="A826" s="35"/>
+      <c r="A826" s="34"/>
     </row>
     <row r="827" spans="1:1" ht="13.2">
-      <c r="A827" s="35"/>
+      <c r="A827" s="34"/>
     </row>
     <row r="828" spans="1:1" ht="13.2">
-      <c r="A828" s="35"/>
+      <c r="A828" s="34"/>
     </row>
     <row r="829" spans="1:1" ht="13.2">
-      <c r="A829" s="35"/>
+      <c r="A829" s="34"/>
     </row>
     <row r="830" spans="1:1" ht="13.2">
-      <c r="A830" s="35"/>
+      <c r="A830" s="34"/>
     </row>
     <row r="831" spans="1:1" ht="13.2">
-      <c r="A831" s="35"/>
+      <c r="A831" s="34"/>
     </row>
     <row r="832" spans="1:1" ht="13.2">
-      <c r="A832" s="35"/>
+      <c r="A832" s="34"/>
     </row>
     <row r="833" spans="1:1" ht="13.2">
-      <c r="A833" s="35"/>
+      <c r="A833" s="34"/>
     </row>
     <row r="834" spans="1:1" ht="13.2">
-      <c r="A834" s="35"/>
+      <c r="A834" s="34"/>
     </row>
     <row r="835" spans="1:1" ht="13.2">
-      <c r="A835" s="35"/>
+      <c r="A835" s="34"/>
     </row>
     <row r="836" spans="1:1" ht="13.2">
-      <c r="A836" s="35"/>
+      <c r="A836" s="34"/>
     </row>
     <row r="837" spans="1:1" ht="13.2">
-      <c r="A837" s="35"/>
+      <c r="A837" s="34"/>
     </row>
     <row r="838" spans="1:1" ht="13.2">
-      <c r="A838" s="35"/>
+      <c r="A838" s="34"/>
     </row>
     <row r="839" spans="1:1" ht="13.2">
-      <c r="A839" s="35"/>
+      <c r="A839" s="34"/>
     </row>
     <row r="840" spans="1:1" ht="13.2">
-      <c r="A840" s="35"/>
+      <c r="A840" s="34"/>
     </row>
     <row r="841" spans="1:1" ht="13.2">
-      <c r="A841" s="35"/>
+      <c r="A841" s="34"/>
     </row>
     <row r="842" spans="1:1" ht="13.2">
-      <c r="A842" s="35"/>
+      <c r="A842" s="34"/>
     </row>
     <row r="843" spans="1:1" ht="13.2">
-      <c r="A843" s="35"/>
+      <c r="A843" s="34"/>
     </row>
     <row r="844" spans="1:1" ht="13.2">
-      <c r="A844" s="35"/>
+      <c r="A844" s="34"/>
     </row>
     <row r="845" spans="1:1" ht="13.2">
-      <c r="A845" s="35"/>
+      <c r="A845" s="34"/>
     </row>
     <row r="846" spans="1:1" ht="13.2">
-      <c r="A846" s="35"/>
+      <c r="A846" s="34"/>
     </row>
     <row r="847" spans="1:1" ht="13.2">
-      <c r="A847" s="35"/>
+      <c r="A847" s="34"/>
     </row>
     <row r="848" spans="1:1" ht="13.2">
-      <c r="A848" s="35"/>
+      <c r="A848" s="34"/>
     </row>
     <row r="849" spans="1:1" ht="13.2">
-      <c r="A849" s="35"/>
+      <c r="A849" s="34"/>
     </row>
     <row r="850" spans="1:1" ht="13.2">
-      <c r="A850" s="35"/>
+      <c r="A850" s="34"/>
     </row>
     <row r="851" spans="1:1" ht="13.2">
-      <c r="A851" s="35"/>
+      <c r="A851" s="34"/>
     </row>
     <row r="852" spans="1:1" ht="13.2">
-      <c r="A852" s="35"/>
+      <c r="A852" s="34"/>
     </row>
     <row r="853" spans="1:1" ht="13.2">
-      <c r="A853" s="35"/>
+      <c r="A853" s="34"/>
     </row>
     <row r="854" spans="1:1" ht="13.2">
-      <c r="A854" s="35"/>
+      <c r="A854" s="34"/>
     </row>
     <row r="855" spans="1:1" ht="13.2">
-      <c r="A855" s="35"/>
+      <c r="A855" s="34"/>
     </row>
     <row r="856" spans="1:1" ht="13.2">
-      <c r="A856" s="35"/>
+      <c r="A856" s="34"/>
     </row>
     <row r="857" spans="1:1" ht="13.2">
-      <c r="A857" s="35"/>
+      <c r="A857" s="34"/>
     </row>
     <row r="858" spans="1:1" ht="13.2">
-      <c r="A858" s="35"/>
+      <c r="A858" s="34"/>
     </row>
     <row r="859" spans="1:1" ht="13.2">
-      <c r="A859" s="35"/>
+      <c r="A859" s="34"/>
     </row>
     <row r="860" spans="1:1" ht="13.2">
-      <c r="A860" s="35"/>
+      <c r="A860" s="34"/>
     </row>
     <row r="861" spans="1:1" ht="13.2">
-      <c r="A861" s="35"/>
+      <c r="A861" s="34"/>
     </row>
     <row r="862" spans="1:1" ht="13.2">
-      <c r="A862" s="35"/>
+      <c r="A862" s="34"/>
     </row>
     <row r="863" spans="1:1" ht="13.2">
-      <c r="A863" s="35"/>
+      <c r="A863" s="34"/>
     </row>
     <row r="864" spans="1:1" ht="13.2">
-      <c r="A864" s="35"/>
+      <c r="A864" s="34"/>
     </row>
     <row r="865" spans="1:1" ht="13.2">
-      <c r="A865" s="35"/>
+      <c r="A865" s="34"/>
     </row>
     <row r="866" spans="1:1" ht="13.2">
-      <c r="A866" s="35"/>
+      <c r="A866" s="34"/>
     </row>
     <row r="867" spans="1:1" ht="13.2">
-      <c r="A867" s="35"/>
+      <c r="A867" s="34"/>
     </row>
     <row r="868" spans="1:1" ht="13.2">
-      <c r="A868" s="35"/>
+      <c r="A868" s="34"/>
     </row>
     <row r="869" spans="1:1" ht="13.2">
-      <c r="A869" s="35"/>
+      <c r="A869" s="34"/>
     </row>
     <row r="870" spans="1:1" ht="13.2">
-      <c r="A870" s="35"/>
+      <c r="A870" s="34"/>
     </row>
     <row r="871" spans="1:1" ht="13.2">
-      <c r="A871" s="35"/>
+      <c r="A871" s="34"/>
     </row>
     <row r="872" spans="1:1" ht="13.2">
-      <c r="A872" s="35"/>
+      <c r="A872" s="34"/>
     </row>
     <row r="873" spans="1:1" ht="13.2">
-      <c r="A873" s="35"/>
+      <c r="A873" s="34"/>
     </row>
     <row r="874" spans="1:1" ht="13.2">
-      <c r="A874" s="35"/>
+      <c r="A874" s="34"/>
     </row>
     <row r="875" spans="1:1" ht="13.2">
-      <c r="A875" s="35"/>
+      <c r="A875" s="34"/>
     </row>
     <row r="876" spans="1:1" ht="13.2">
-      <c r="A876" s="35"/>
+      <c r="A876" s="34"/>
     </row>
     <row r="877" spans="1:1" ht="13.2">
-      <c r="A877" s="35"/>
+      <c r="A877" s="34"/>
     </row>
     <row r="878" spans="1:1" ht="13.2">
-      <c r="A878" s="35"/>
+      <c r="A878" s="34"/>
     </row>
     <row r="879" spans="1:1" ht="13.2">
-      <c r="A879" s="35"/>
+      <c r="A879" s="34"/>
     </row>
     <row r="880" spans="1:1" ht="13.2">
-      <c r="A880" s="35"/>
+      <c r="A880" s="34"/>
     </row>
     <row r="881" spans="1:1" ht="13.2">
-      <c r="A881" s="35"/>
+      <c r="A881" s="34"/>
     </row>
     <row r="882" spans="1:1" ht="13.2">
-      <c r="A882" s="35"/>
+      <c r="A882" s="34"/>
     </row>
     <row r="883" spans="1:1" ht="13.2">
-      <c r="A883" s="35"/>
+      <c r="A883" s="34"/>
     </row>
     <row r="884" spans="1:1" ht="13.2">
-      <c r="A884" s="35"/>
+      <c r="A884" s="34"/>
     </row>
     <row r="885" spans="1:1" ht="13.2">
-      <c r="A885" s="35"/>
+      <c r="A885" s="34"/>
     </row>
     <row r="886" spans="1:1" ht="13.2">
-      <c r="A886" s="35"/>
+      <c r="A886" s="34"/>
     </row>
     <row r="887" spans="1:1" ht="13.2">
-      <c r="A887" s="35"/>
+      <c r="A887" s="34"/>
     </row>
     <row r="888" spans="1:1" ht="13.2">
-      <c r="A888" s="35"/>
+      <c r="A888" s="34"/>
     </row>
     <row r="889" spans="1:1" ht="13.2">
-      <c r="A889" s="35"/>
+      <c r="A889" s="34"/>
     </row>
     <row r="890" spans="1:1" ht="13.2">
-      <c r="A890" s="35"/>
+      <c r="A890" s="34"/>
     </row>
     <row r="891" spans="1:1" ht="13.2">
-      <c r="A891" s="35"/>
+      <c r="A891" s="34"/>
     </row>
     <row r="892" spans="1:1" ht="13.2">
-      <c r="A892" s="35"/>
+      <c r="A892" s="34"/>
     </row>
     <row r="893" spans="1:1" ht="13.2">
-      <c r="A893" s="35"/>
+      <c r="A893" s="34"/>
     </row>
     <row r="894" spans="1:1" ht="13.2">
-      <c r="A894" s="35"/>
+      <c r="A894" s="34"/>
     </row>
     <row r="895" spans="1:1" ht="13.2">
-      <c r="A895" s="35"/>
+      <c r="A895" s="34"/>
     </row>
     <row r="896" spans="1:1" ht="13.2">
-      <c r="A896" s="35"/>
+      <c r="A896" s="34"/>
     </row>
     <row r="897" spans="1:1" ht="13.2">
-      <c r="A897" s="35"/>
+      <c r="A897" s="34"/>
     </row>
     <row r="898" spans="1:1" ht="13.2">
-      <c r="A898" s="35"/>
+      <c r="A898" s="34"/>
     </row>
     <row r="899" spans="1:1" ht="13.2">
-      <c r="A899" s="35"/>
+      <c r="A899" s="34"/>
     </row>
     <row r="900" spans="1:1" ht="13.2">
-      <c r="A900" s="35"/>
+      <c r="A900" s="34"/>
     </row>
     <row r="901" spans="1:1" ht="13.2">
-      <c r="A901" s="35"/>
+      <c r="A901" s="34"/>
     </row>
     <row r="902" spans="1:1" ht="13.2">
-      <c r="A902" s="35"/>
+      <c r="A902" s="34"/>
     </row>
     <row r="903" spans="1:1" ht="13.2">
-      <c r="A903" s="35"/>
+      <c r="A903" s="34"/>
     </row>
     <row r="904" spans="1:1" ht="13.2">
-      <c r="A904" s="35"/>
+      <c r="A904" s="34"/>
     </row>
     <row r="905" spans="1:1" ht="13.2">
-      <c r="A905" s="35"/>
+      <c r="A905" s="34"/>
     </row>
     <row r="906" spans="1:1" ht="13.2">
-      <c r="A906" s="35"/>
+      <c r="A906" s="34"/>
     </row>
     <row r="907" spans="1:1" ht="13.2">
-      <c r="A907" s="35"/>
+      <c r="A907" s="34"/>
     </row>
     <row r="908" spans="1:1" ht="13.2">
-      <c r="A908" s="35"/>
+      <c r="A908" s="34"/>
     </row>
     <row r="909" spans="1:1" ht="13.2">
-      <c r="A909" s="35"/>
+      <c r="A909" s="34"/>
     </row>
     <row r="910" spans="1:1" ht="13.2">
-      <c r="A910" s="35"/>
+      <c r="A910" s="34"/>
     </row>
     <row r="911" spans="1:1" ht="13.2">
-      <c r="A911" s="35"/>
+      <c r="A911" s="34"/>
     </row>
     <row r="912" spans="1:1" ht="13.2">
-      <c r="A912" s="35"/>
+      <c r="A912" s="34"/>
     </row>
     <row r="913" spans="1:1" ht="13.2">
-      <c r="A913" s="35"/>
+      <c r="A913" s="34"/>
     </row>
     <row r="914" spans="1:1" ht="13.2">
-      <c r="A914" s="35"/>
+      <c r="A914" s="34"/>
     </row>
     <row r="915" spans="1:1" ht="13.2">
-      <c r="A915" s="35"/>
+      <c r="A915" s="34"/>
     </row>
     <row r="916" spans="1:1" ht="13.2">
-      <c r="A916" s="35"/>
+      <c r="A916" s="34"/>
     </row>
     <row r="917" spans="1:1" ht="13.2">
-      <c r="A917" s="35"/>
+      <c r="A917" s="34"/>
     </row>
     <row r="918" spans="1:1" ht="13.2">
-      <c r="A918" s="35"/>
+      <c r="A918" s="34"/>
     </row>
     <row r="919" spans="1:1" ht="13.2">
-      <c r="A919" s="35"/>
+      <c r="A919" s="34"/>
     </row>
     <row r="920" spans="1:1" ht="13.2">
-      <c r="A920" s="35"/>
+      <c r="A920" s="34"/>
     </row>
     <row r="921" spans="1:1" ht="13.2">
-      <c r="A921" s="35"/>
+      <c r="A921" s="34"/>
     </row>
     <row r="922" spans="1:1" ht="13.2">
-      <c r="A922" s="35"/>
+      <c r="A922" s="34"/>
     </row>
     <row r="923" spans="1:1" ht="13.2">
-      <c r="A923" s="35"/>
+      <c r="A923" s="34"/>
     </row>
     <row r="924" spans="1:1" ht="13.2">
-      <c r="A924" s="35"/>
+      <c r="A924" s="34"/>
     </row>
     <row r="925" spans="1:1" ht="13.2">
-      <c r="A925" s="35"/>
+      <c r="A925" s="34"/>
     </row>
     <row r="926" spans="1:1" ht="13.2">
-      <c r="A926" s="35"/>
+      <c r="A926" s="34"/>
     </row>
     <row r="927" spans="1:1" ht="13.2">
-      <c r="A927" s="35"/>
+      <c r="A927" s="34"/>
     </row>
     <row r="928" spans="1:1" ht="13.2">
-      <c r="A928" s="35"/>
+      <c r="A928" s="34"/>
     </row>
     <row r="929" spans="1:1" ht="13.2">
-      <c r="A929" s="35"/>
+      <c r="A929" s="34"/>
     </row>
     <row r="930" spans="1:1" ht="13.2">
-      <c r="A930" s="35"/>
+      <c r="A930" s="34"/>
     </row>
     <row r="931" spans="1:1" ht="13.2">
-      <c r="A931" s="35"/>
+      <c r="A931" s="34"/>
     </row>
     <row r="932" spans="1:1" ht="13.2">
-      <c r="A932" s="35"/>
+      <c r="A932" s="34"/>
     </row>
     <row r="933" spans="1:1" ht="13.2">
-      <c r="A933" s="35"/>
+      <c r="A933" s="34"/>
     </row>
     <row r="934" spans="1:1" ht="13.2">
-      <c r="A934" s="35"/>
+      <c r="A934" s="34"/>
     </row>
     <row r="935" spans="1:1" ht="13.2">
-      <c r="A935" s="35"/>
+      <c r="A935" s="34"/>
     </row>
     <row r="936" spans="1:1" ht="13.2">
-      <c r="A936" s="35"/>
+      <c r="A936" s="34"/>
     </row>
     <row r="937" spans="1:1" ht="13.2">
-      <c r="A937" s="35"/>
+      <c r="A937" s="34"/>
     </row>
     <row r="938" spans="1:1" ht="13.2">
-      <c r="A938" s="35"/>
+      <c r="A938" s="34"/>
     </row>
     <row r="939" spans="1:1" ht="13.2">
-      <c r="A939" s="35"/>
+      <c r="A939" s="34"/>
     </row>
     <row r="940" spans="1:1" ht="13.2">
-      <c r="A940" s="35"/>
+      <c r="A940" s="34"/>
     </row>
     <row r="941" spans="1:1" ht="13.2">
-      <c r="A941" s="35"/>
+      <c r="A941" s="34"/>
     </row>
     <row r="942" spans="1:1" ht="13.2">
-      <c r="A942" s="35"/>
+      <c r="A942" s="34"/>
     </row>
     <row r="943" spans="1:1" ht="13.2">
-      <c r="A943" s="35"/>
+      <c r="A943" s="34"/>
     </row>
     <row r="944" spans="1:1" ht="13.2">
-      <c r="A944" s="35"/>
+      <c r="A944" s="34"/>
     </row>
     <row r="945" spans="1:1" ht="13.2">
-      <c r="A945" s="35"/>
+      <c r="A945" s="34"/>
     </row>
     <row r="946" spans="1:1" ht="13.2">
-      <c r="A946" s="35"/>
+      <c r="A946" s="34"/>
     </row>
     <row r="947" spans="1:1" ht="13.2">
-      <c r="A947" s="35"/>
+      <c r="A947" s="34"/>
     </row>
     <row r="948" spans="1:1" ht="13.2">
-      <c r="A948" s="35"/>
+      <c r="A948" s="34"/>
     </row>
     <row r="949" spans="1:1" ht="13.2">
-      <c r="A949" s="35"/>
+      <c r="A949" s="34"/>
     </row>
     <row r="950" spans="1:1" ht="13.2">
-      <c r="A950" s="35"/>
+      <c r="A950" s="34"/>
     </row>
     <row r="951" spans="1:1" ht="13.2">
-      <c r="A951" s="35"/>
+      <c r="A951" s="34"/>
     </row>
     <row r="952" spans="1:1" ht="13.2">
-      <c r="A952" s="35"/>
+      <c r="A952" s="34"/>
     </row>
     <row r="953" spans="1:1" ht="13.2">
-      <c r="A953" s="35"/>
+      <c r="A953" s="34"/>
     </row>
     <row r="954" spans="1:1" ht="13.2">
-      <c r="A954" s="35"/>
+      <c r="A954" s="34"/>
     </row>
     <row r="955" spans="1:1" ht="13.2">
-      <c r="A955" s="35"/>
+      <c r="A955" s="34"/>
     </row>
     <row r="956" spans="1:1" ht="13.2">
-      <c r="A956" s="35"/>
+      <c r="A956" s="34"/>
     </row>
     <row r="957" spans="1:1" ht="13.2">
-      <c r="A957" s="35"/>
+      <c r="A957" s="34"/>
     </row>
     <row r="958" spans="1:1" ht="13.2">
-      <c r="A958" s="35"/>
+      <c r="A958" s="34"/>
     </row>
     <row r="959" spans="1:1" ht="13.2">
-      <c r="A959" s="35"/>
+      <c r="A959" s="34"/>
     </row>
     <row r="960" spans="1:1" ht="13.2">
-      <c r="A960" s="35"/>
+      <c r="A960" s="34"/>
     </row>
     <row r="961" spans="1:1" ht="13.2">
-      <c r="A961" s="35"/>
+      <c r="A961" s="34"/>
     </row>
     <row r="962" spans="1:1" ht="13.2">
-      <c r="A962" s="35"/>
+      <c r="A962" s="34"/>
     </row>
     <row r="963" spans="1:1" ht="13.2">
-      <c r="A963" s="35"/>
+      <c r="A963" s="34"/>
     </row>
     <row r="964" spans="1:1" ht="13.2">
-      <c r="A964" s="35"/>
+      <c r="A964" s="34"/>
     </row>
     <row r="965" spans="1:1" ht="13.2">
-      <c r="A965" s="35"/>
+      <c r="A965" s="34"/>
     </row>
     <row r="966" spans="1:1" ht="13.2">
-      <c r="A966" s="35"/>
+      <c r="A966" s="34"/>
     </row>
     <row r="967" spans="1:1" ht="13.2">
-      <c r="A967" s="35"/>
+      <c r="A967" s="34"/>
     </row>
     <row r="968" spans="1:1" ht="13.2">
-      <c r="A968" s="35"/>
+      <c r="A968" s="34"/>
     </row>
     <row r="969" spans="1:1" ht="13.2">
-      <c r="A969" s="35"/>
+      <c r="A969" s="34"/>
     </row>
     <row r="970" spans="1:1" ht="13.2">
-      <c r="A970" s="35"/>
+      <c r="A970" s="34"/>
     </row>
     <row r="971" spans="1:1" ht="13.2">
-      <c r="A971" s="35"/>
+      <c r="A971" s="34"/>
     </row>
     <row r="972" spans="1:1" ht="13.2">
-      <c r="A972" s="35"/>
+      <c r="A972" s="34"/>
     </row>
     <row r="973" spans="1:1" ht="13.2">
-      <c r="A973" s="35"/>
+      <c r="A973" s="34"/>
     </row>
     <row r="974" spans="1:1" ht="13.2">
-      <c r="A974" s="35"/>
+      <c r="A974" s="34"/>
     </row>
     <row r="975" spans="1:1" ht="13.2">
-      <c r="A975" s="35"/>
+      <c r="A975" s="34"/>
     </row>
     <row r="976" spans="1:1" ht="13.2">
-      <c r="A976" s="35"/>
+      <c r="A976" s="34"/>
     </row>
     <row r="977" spans="1:1" ht="13.2">
-      <c r="A977" s="35"/>
+      <c r="A977" s="34"/>
     </row>
     <row r="978" spans="1:1" ht="13.2">
-      <c r="A978" s="35"/>
+      <c r="A978" s="34"/>
     </row>
     <row r="979" spans="1:1" ht="13.2">
-      <c r="A979" s="35"/>
+      <c r="A979" s="34"/>
     </row>
     <row r="980" spans="1:1" ht="13.2">
-      <c r="A980" s="35"/>
+      <c r="A980" s="34"/>
     </row>
     <row r="981" spans="1:1" ht="13.2">
-      <c r="A981" s="35"/>
+      <c r="A981" s="34"/>
     </row>
     <row r="982" spans="1:1" ht="13.2">
-      <c r="A982" s="35"/>
+      <c r="A982" s="34"/>
     </row>
     <row r="983" spans="1:1" ht="13.2">
-      <c r="A983" s="35"/>
+      <c r="A983" s="34"/>
     </row>
     <row r="984" spans="1:1" ht="13.2">
-      <c r="A984" s="35"/>
+      <c r="A984" s="34"/>
     </row>
     <row r="985" spans="1:1" ht="13.2">
-      <c r="A985" s="35"/>
+      <c r="A985" s="34"/>
     </row>
     <row r="986" spans="1:1" ht="13.2">
-      <c r="A986" s="35"/>
+      <c r="A986" s="34"/>
     </row>
     <row r="987" spans="1:1" ht="13.2">
-      <c r="A987" s="35"/>
+      <c r="A987" s="34"/>
     </row>
     <row r="988" spans="1:1" ht="13.2">
-      <c r="A988" s="35"/>
+      <c r="A988" s="34"/>
     </row>
     <row r="989" spans="1:1" ht="13.2">
-      <c r="A989" s="35"/>
+      <c r="A989" s="34"/>
     </row>
     <row r="990" spans="1:1" ht="13.2">
-      <c r="A990" s="35"/>
+      <c r="A990" s="34"/>
     </row>
     <row r="991" spans="1:1" ht="13.2">
-      <c r="A991" s="35"/>
+      <c r="A991" s="34"/>
     </row>
     <row r="992" spans="1:1" ht="13.2">
-      <c r="A992" s="35"/>
+      <c r="A992" s="34"/>
     </row>
     <row r="993" spans="1:1" ht="13.2">
-      <c r="A993" s="35"/>
+      <c r="A993" s="34"/>
     </row>
     <row r="994" spans="1:1" ht="13.2">
-      <c r="A994" s="35"/>
+      <c r="A994" s="34"/>
     </row>
     <row r="995" spans="1:1" ht="13.2">
-      <c r="A995" s="35"/>
+      <c r="A995" s="34"/>
     </row>
     <row r="996" spans="1:1" ht="13.2">
-      <c r="A996" s="35"/>
+      <c r="A996" s="34"/>
     </row>
     <row r="997" spans="1:1" ht="13.2">
-      <c r="A997" s="35"/>
+      <c r="A997" s="34"/>
     </row>
     <row r="998" spans="1:1" ht="13.2">
-      <c r="A998" s="35"/>
+      <c r="A998" s="34"/>
     </row>
     <row r="999" spans="1:1" ht="13.2">
-      <c r="A999" s="35"/>
+      <c r="A999" s="34"/>
     </row>
     <row r="1000" spans="1:1" ht="13.2">
-      <c r="A1000" s="35"/>
+      <c r="A1000" s="34"/>
     </row>
     <row r="1001" spans="1:1" ht="13.2">
-      <c r="A1001" s="35"/>
+      <c r="A1001" s="34"/>
     </row>
     <row r="1002" spans="1:1" ht="13.2">
-      <c r="A1002" s="35"/>
+      <c r="A1002" s="34"/>
     </row>
     <row r="1003" spans="1:1" ht="13.2">
-      <c r="A1003" s="35"/>
+      <c r="A1003" s="34"/>
     </row>
     <row r="1004" spans="1:1" ht="13.2">
-      <c r="A1004" s="35"/>
+      <c r="A1004" s="34"/>
     </row>
     <row r="1005" spans="1:1" ht="13.2">
-      <c r="A1005" s="35"/>
+      <c r="A1005" s="34"/>
     </row>
     <row r="1006" spans="1:1" ht="13.2">
-      <c r="A1006" s="35"/>
+      <c r="A1006" s="34"/>
     </row>
     <row r="1007" spans="1:1" ht="13.2">
-      <c r="A1007" s="35"/>
+      <c r="A1007" s="34"/>
     </row>
   </sheetData>
   <mergeCells count="7">
@@ -20756,13 +20800,13 @@
     <mergeCell ref="A7:J7"/>
   </mergeCells>
   <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" sqref="I8:I12 I14:I23 I25:I59" xr:uid="{00000000-0002-0000-0000-000000000000}">
+    <dataValidation type="list" allowBlank="1" sqref="I8:I12 I25:I59 I14:I23" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>"STILL,ON GOING,DELIVERED,DELIVERED (LATE)"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" sqref="B8:B12 B14:B23 B25:B59" xr:uid="{00000000-0002-0000-0000-000001000000}">
+    <dataValidation type="list" allowBlank="1" sqref="B8:B12 B25:B59 B14:B23" xr:uid="{00000000-0002-0000-0000-000001000000}">
       <formula1>"Technical,Non -Technical"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" sqref="C8:C12 C14:C23 C25:C59" xr:uid="{00000000-0002-0000-0000-000002000000}">
+    <dataValidation type="list" allowBlank="1" sqref="C8:C12 C25:C59 C14:C23" xr:uid="{00000000-0002-0000-0000-000002000000}">
       <formula1>"Hazem Mekawy,Esraa Awad,Nada Mohamed,Mina Helmi,Alzahraa El-Sallakh"</formula1>
     </dataValidation>
   </dataValidations>
@@ -20770,5 +20814,6 @@
     <hyperlink ref="B4" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Updating the CYRS > Released Updating the PP >> Latest updates Updating the SRS >> Reviewing Mina
Signed-off-by: Hazemmekawy <dextermekawy@gmail.com>
</commit_message>
<xml_diff>
--- a/SW deliveries log/PP.xlsx
+++ b/SW deliveries log/PP.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hazem Mekawy\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\ITI COURSES\Software Engineering\SWE_WORKSPACE\SW deliveries log\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{275079F4-0308-4DC3-9677-6C50192D10FB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C624C182-2E75-458D-8072-6C7A41A0EBDF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="106" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="55">
   <si>
     <t>Sovy - Digital Calculator PO1_DGC_PROJECT PLAN</t>
   </si>
@@ -154,9 +154,6 @@
     <t>SIQ Document Update</t>
   </si>
   <si>
-    <t>STILL</t>
-  </si>
-  <si>
     <t>CYRS Document Update</t>
   </si>
   <si>
@@ -185,6 +182,9 @@
   </si>
   <si>
     <t>WEEK 3</t>
+  </si>
+  <si>
+    <t>Except the lastest review that was on 6/2/2020</t>
   </si>
 </sst>
 </file>
@@ -487,7 +487,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -615,6 +615,21 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -835,8 +850,8 @@
   </sheetPr>
   <dimension ref="A1:KA1007"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C15" workbookViewId="0">
-      <selection activeCell="H25" sqref="H25"/>
+    <sheetView tabSelected="1" topLeftCell="F16" workbookViewId="0">
+      <selection activeCell="J18" sqref="J18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1"/>
@@ -848,7 +863,7 @@
     <col min="5" max="5" width="26.44140625" customWidth="1"/>
     <col min="6" max="8" width="30.44140625" customWidth="1"/>
     <col min="9" max="9" width="29.5546875" customWidth="1"/>
-    <col min="10" max="10" width="37.88671875" customWidth="1"/>
+    <col min="10" max="10" width="58.109375" style="49" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:287" ht="28.2">
@@ -863,7 +878,7 @@
       <c r="G1" s="1"/>
       <c r="H1" s="1"/>
       <c r="I1" s="1"/>
-      <c r="J1" s="1"/>
+      <c r="J1" s="45"/>
       <c r="K1" s="2"/>
       <c r="L1" s="2"/>
       <c r="M1" s="2"/>
@@ -1164,7 +1179,7 @@
       <c r="G2" s="41"/>
       <c r="H2" s="41"/>
       <c r="I2" s="8"/>
-      <c r="J2" s="8"/>
+      <c r="J2" s="46"/>
       <c r="K2" s="8"/>
       <c r="L2" s="8"/>
       <c r="M2" s="8"/>
@@ -1788,7 +1803,7 @@
       <c r="I5" s="27" t="s">
         <v>23</v>
       </c>
-      <c r="J5" s="27" t="s">
+      <c r="J5" s="47" t="s">
         <v>24</v>
       </c>
       <c r="K5" s="9"/>
@@ -2679,7 +2694,7 @@
       <c r="I8" s="29" t="s">
         <v>30</v>
       </c>
-      <c r="J8" s="28"/>
+      <c r="J8" s="48"/>
       <c r="K8" s="28"/>
       <c r="L8" s="28"/>
       <c r="M8" s="28"/>
@@ -2986,7 +3001,7 @@
       <c r="I9" s="29" t="s">
         <v>33</v>
       </c>
-      <c r="J9" s="30" t="s">
+      <c r="J9" s="48" t="s">
         <v>34</v>
       </c>
       <c r="K9" s="28"/>
@@ -3295,7 +3310,7 @@
       <c r="I10" s="29" t="s">
         <v>33</v>
       </c>
-      <c r="J10" s="30" t="s">
+      <c r="J10" s="48" t="s">
         <v>37</v>
       </c>
       <c r="K10" s="28"/>
@@ -3604,7 +3619,7 @@
       <c r="I11" s="29" t="s">
         <v>33</v>
       </c>
-      <c r="J11" s="30" t="s">
+      <c r="J11" s="48" t="s">
         <v>37</v>
       </c>
       <c r="K11" s="28"/>
@@ -3913,7 +3928,7 @@
       <c r="I12" s="29" t="s">
         <v>33</v>
       </c>
-      <c r="J12" s="30" t="s">
+      <c r="J12" s="48" t="s">
         <v>41</v>
       </c>
       <c r="K12" s="28"/>
@@ -4513,7 +4528,7 @@
       <c r="I14" s="29" t="s">
         <v>33</v>
       </c>
-      <c r="J14" s="28"/>
+      <c r="J14" s="48"/>
       <c r="K14" s="28"/>
       <c r="L14" s="28"/>
       <c r="M14" s="28"/>
@@ -4794,7 +4809,7 @@
     </row>
     <row r="15" spans="1:287" ht="30.75" customHeight="1">
       <c r="A15" s="29" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B15" s="30" t="s">
         <v>28</v>
@@ -4820,7 +4835,7 @@
       <c r="I15" s="29" t="s">
         <v>33</v>
       </c>
-      <c r="J15" s="28"/>
+      <c r="J15" s="48"/>
       <c r="K15" s="28"/>
       <c r="L15" s="28"/>
       <c r="M15" s="28"/>
@@ -5101,7 +5116,7 @@
     </row>
     <row r="16" spans="1:287" ht="30.75" customHeight="1">
       <c r="A16" s="29" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B16" s="30" t="s">
         <v>28</v>
@@ -5127,7 +5142,7 @@
       <c r="I16" s="29" t="s">
         <v>33</v>
       </c>
-      <c r="J16" s="28"/>
+      <c r="J16" s="48"/>
       <c r="K16" s="28"/>
       <c r="L16" s="28"/>
       <c r="M16" s="28"/>
@@ -5408,7 +5423,7 @@
     </row>
     <row r="17" spans="1:287" ht="30.75" customHeight="1">
       <c r="A17" s="29" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B17" s="30" t="s">
         <v>28</v>
@@ -5434,7 +5449,7 @@
       <c r="I17" s="29" t="s">
         <v>33</v>
       </c>
-      <c r="J17" s="28"/>
+      <c r="J17" s="48"/>
       <c r="K17" s="28"/>
       <c r="L17" s="28"/>
       <c r="M17" s="28"/>
@@ -5715,7 +5730,7 @@
     </row>
     <row r="18" spans="1:287" ht="30.75" customHeight="1">
       <c r="A18" s="29" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B18" s="30" t="s">
         <v>28</v>
@@ -5741,7 +5756,7 @@
       <c r="I18" s="29" t="s">
         <v>33</v>
       </c>
-      <c r="J18" s="28"/>
+      <c r="J18" s="48"/>
       <c r="K18" s="28"/>
       <c r="L18" s="28"/>
       <c r="M18" s="28"/>
@@ -6022,7 +6037,7 @@
     </row>
     <row r="19" spans="1:287" ht="30.75" customHeight="1">
       <c r="A19" s="32" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B19" s="30" t="s">
         <v>28</v>
@@ -6048,7 +6063,7 @@
       <c r="I19" s="29" t="s">
         <v>33</v>
       </c>
-      <c r="J19" s="28"/>
+      <c r="J19" s="48"/>
       <c r="K19" s="28"/>
       <c r="L19" s="28"/>
       <c r="M19" s="28"/>
@@ -6329,7 +6344,7 @@
     </row>
     <row r="20" spans="1:287" ht="30.75" customHeight="1">
       <c r="A20" s="32" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B20" s="30" t="s">
         <v>28</v>
@@ -6343,13 +6358,19 @@
       <c r="E20" s="36">
         <v>43867</v>
       </c>
-      <c r="F20" s="28"/>
-      <c r="G20" s="28"/>
-      <c r="H20" s="28"/>
+      <c r="F20" s="36">
+        <v>43867</v>
+      </c>
+      <c r="G20" s="36">
+        <v>43867</v>
+      </c>
+      <c r="H20" s="28">
+        <v>1</v>
+      </c>
       <c r="I20" s="29" t="s">
-        <v>44</v>
+        <v>33</v>
       </c>
-      <c r="J20" s="28"/>
+      <c r="J20" s="48"/>
       <c r="K20" s="28"/>
       <c r="L20" s="28"/>
       <c r="M20" s="28"/>
@@ -6630,7 +6651,7 @@
     </row>
     <row r="21" spans="1:287" ht="30.75" customHeight="1">
       <c r="A21" s="29" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B21" s="30" t="s">
         <v>28</v>
@@ -6656,7 +6677,7 @@
       <c r="I21" s="29" t="s">
         <v>33</v>
       </c>
-      <c r="J21" s="28"/>
+      <c r="J21" s="48"/>
       <c r="K21" s="28"/>
       <c r="L21" s="28"/>
       <c r="M21" s="28"/>
@@ -6937,7 +6958,7 @@
     </row>
     <row r="22" spans="1:287" ht="30.75" customHeight="1">
       <c r="A22" s="29" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B22" s="30" t="s">
         <v>28</v>
@@ -6954,12 +6975,16 @@
       <c r="F22" s="35">
         <v>43866</v>
       </c>
-      <c r="G22" s="28"/>
-      <c r="H22" s="28"/>
+      <c r="G22" s="36">
+        <v>43867</v>
+      </c>
+      <c r="H22" s="28">
+        <v>2</v>
+      </c>
       <c r="I22" s="29" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
-      <c r="J22" s="28"/>
+      <c r="J22" s="48"/>
       <c r="K22" s="28"/>
       <c r="L22" s="28"/>
       <c r="M22" s="28"/>
@@ -7240,7 +7265,7 @@
     </row>
     <row r="23" spans="1:287" ht="30.75" customHeight="1">
       <c r="A23" s="29" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B23" s="30" t="s">
         <v>28</v>
@@ -7254,13 +7279,21 @@
       <c r="E23" s="36">
         <v>43868</v>
       </c>
-      <c r="F23" s="28"/>
-      <c r="G23" s="28"/>
-      <c r="H23" s="28"/>
+      <c r="F23" s="36">
+        <v>43868</v>
+      </c>
+      <c r="G23" s="36">
+        <v>43868</v>
+      </c>
+      <c r="H23" s="28">
+        <v>1</v>
+      </c>
       <c r="I23" s="29" t="s">
-        <v>44</v>
+        <v>33</v>
       </c>
-      <c r="J23" s="28"/>
+      <c r="J23" s="48" t="s">
+        <v>54</v>
+      </c>
       <c r="K23" s="28"/>
       <c r="L23" s="28"/>
       <c r="M23" s="28"/>
@@ -7541,7 +7574,7 @@
     </row>
     <row r="24" spans="1:287" ht="30.75" customHeight="1">
       <c r="A24" s="37" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B24" s="38"/>
       <c r="C24" s="38"/>
@@ -7840,7 +7873,7 @@
       <c r="G25" s="28"/>
       <c r="H25" s="28"/>
       <c r="I25" s="29"/>
-      <c r="J25" s="28"/>
+      <c r="J25" s="48"/>
       <c r="K25" s="28"/>
       <c r="L25" s="28"/>
       <c r="M25" s="28"/>
@@ -8129,7 +8162,7 @@
       <c r="G26" s="28"/>
       <c r="H26" s="28"/>
       <c r="I26" s="29"/>
-      <c r="J26" s="28"/>
+      <c r="J26" s="48"/>
       <c r="K26" s="28"/>
       <c r="L26" s="28"/>
       <c r="M26" s="28"/>
@@ -8418,7 +8451,7 @@
       <c r="G27" s="28"/>
       <c r="H27" s="28"/>
       <c r="I27" s="29"/>
-      <c r="J27" s="28"/>
+      <c r="J27" s="48"/>
       <c r="K27" s="28"/>
       <c r="L27" s="28"/>
       <c r="M27" s="28"/>
@@ -8707,7 +8740,7 @@
       <c r="G28" s="28"/>
       <c r="H28" s="28"/>
       <c r="I28" s="29"/>
-      <c r="J28" s="28"/>
+      <c r="J28" s="48"/>
       <c r="K28" s="28"/>
       <c r="L28" s="28"/>
       <c r="M28" s="28"/>
@@ -8996,7 +9029,7 @@
       <c r="G29" s="28"/>
       <c r="H29" s="28"/>
       <c r="I29" s="29"/>
-      <c r="J29" s="28"/>
+      <c r="J29" s="48"/>
       <c r="K29" s="28"/>
       <c r="L29" s="28"/>
       <c r="M29" s="28"/>
@@ -9285,7 +9318,7 @@
       <c r="G30" s="28"/>
       <c r="H30" s="28"/>
       <c r="I30" s="29"/>
-      <c r="J30" s="28"/>
+      <c r="J30" s="48"/>
       <c r="K30" s="28"/>
       <c r="L30" s="28"/>
       <c r="M30" s="28"/>
@@ -9574,7 +9607,7 @@
       <c r="G31" s="28"/>
       <c r="H31" s="28"/>
       <c r="I31" s="29"/>
-      <c r="J31" s="28"/>
+      <c r="J31" s="48"/>
       <c r="K31" s="28"/>
       <c r="L31" s="28"/>
       <c r="M31" s="28"/>
@@ -9863,7 +9896,7 @@
       <c r="G32" s="28"/>
       <c r="H32" s="28"/>
       <c r="I32" s="29"/>
-      <c r="J32" s="28"/>
+      <c r="J32" s="48"/>
       <c r="K32" s="28"/>
       <c r="L32" s="28"/>
       <c r="M32" s="28"/>
@@ -10152,7 +10185,7 @@
       <c r="G33" s="28"/>
       <c r="H33" s="28"/>
       <c r="I33" s="29"/>
-      <c r="J33" s="28"/>
+      <c r="J33" s="48"/>
       <c r="K33" s="28"/>
       <c r="L33" s="28"/>
       <c r="M33" s="28"/>
@@ -10441,7 +10474,7 @@
       <c r="G34" s="28"/>
       <c r="H34" s="28"/>
       <c r="I34" s="29"/>
-      <c r="J34" s="28"/>
+      <c r="J34" s="48"/>
       <c r="K34" s="28"/>
       <c r="L34" s="28"/>
       <c r="M34" s="28"/>
@@ -10730,7 +10763,7 @@
       <c r="G35" s="28"/>
       <c r="H35" s="28"/>
       <c r="I35" s="29"/>
-      <c r="J35" s="28"/>
+      <c r="J35" s="48"/>
       <c r="K35" s="28"/>
       <c r="L35" s="28"/>
       <c r="M35" s="28"/>
@@ -11019,7 +11052,7 @@
       <c r="G36" s="28"/>
       <c r="H36" s="28"/>
       <c r="I36" s="29"/>
-      <c r="J36" s="28"/>
+      <c r="J36" s="48"/>
       <c r="K36" s="28"/>
       <c r="L36" s="28"/>
       <c r="M36" s="28"/>
@@ -11308,7 +11341,7 @@
       <c r="G37" s="28"/>
       <c r="H37" s="28"/>
       <c r="I37" s="29"/>
-      <c r="J37" s="28"/>
+      <c r="J37" s="48"/>
       <c r="K37" s="28"/>
       <c r="L37" s="28"/>
       <c r="M37" s="28"/>
@@ -11597,7 +11630,7 @@
       <c r="G38" s="28"/>
       <c r="H38" s="28"/>
       <c r="I38" s="29"/>
-      <c r="J38" s="28"/>
+      <c r="J38" s="48"/>
       <c r="K38" s="28"/>
       <c r="L38" s="28"/>
       <c r="M38" s="28"/>
@@ -11886,7 +11919,7 @@
       <c r="G39" s="28"/>
       <c r="H39" s="28"/>
       <c r="I39" s="29"/>
-      <c r="J39" s="28"/>
+      <c r="J39" s="48"/>
       <c r="K39" s="28"/>
       <c r="L39" s="28"/>
       <c r="M39" s="28"/>
@@ -12175,7 +12208,7 @@
       <c r="G40" s="28"/>
       <c r="H40" s="28"/>
       <c r="I40" s="29"/>
-      <c r="J40" s="28"/>
+      <c r="J40" s="48"/>
       <c r="K40" s="28"/>
       <c r="L40" s="28"/>
       <c r="M40" s="28"/>
@@ -12464,7 +12497,7 @@
       <c r="G41" s="28"/>
       <c r="H41" s="28"/>
       <c r="I41" s="29"/>
-      <c r="J41" s="28"/>
+      <c r="J41" s="48"/>
       <c r="K41" s="28"/>
       <c r="L41" s="28"/>
       <c r="M41" s="28"/>
@@ -12753,7 +12786,7 @@
       <c r="G42" s="28"/>
       <c r="H42" s="28"/>
       <c r="I42" s="29"/>
-      <c r="J42" s="28"/>
+      <c r="J42" s="48"/>
       <c r="K42" s="28"/>
       <c r="L42" s="28"/>
       <c r="M42" s="28"/>
@@ -13042,7 +13075,7 @@
       <c r="G43" s="28"/>
       <c r="H43" s="28"/>
       <c r="I43" s="29"/>
-      <c r="J43" s="28"/>
+      <c r="J43" s="48"/>
       <c r="K43" s="28"/>
       <c r="L43" s="28"/>
       <c r="M43" s="28"/>
@@ -13331,7 +13364,7 @@
       <c r="G44" s="28"/>
       <c r="H44" s="28"/>
       <c r="I44" s="29"/>
-      <c r="J44" s="28"/>
+      <c r="J44" s="48"/>
       <c r="K44" s="28"/>
       <c r="L44" s="28"/>
       <c r="M44" s="28"/>
@@ -13620,7 +13653,7 @@
       <c r="G45" s="28"/>
       <c r="H45" s="28"/>
       <c r="I45" s="29"/>
-      <c r="J45" s="28"/>
+      <c r="J45" s="48"/>
       <c r="K45" s="28"/>
       <c r="L45" s="28"/>
       <c r="M45" s="28"/>
@@ -13909,7 +13942,7 @@
       <c r="G46" s="28"/>
       <c r="H46" s="28"/>
       <c r="I46" s="29"/>
-      <c r="J46" s="28"/>
+      <c r="J46" s="48"/>
       <c r="K46" s="28"/>
       <c r="L46" s="28"/>
       <c r="M46" s="28"/>
@@ -14198,7 +14231,7 @@
       <c r="G47" s="28"/>
       <c r="H47" s="28"/>
       <c r="I47" s="29"/>
-      <c r="J47" s="28"/>
+      <c r="J47" s="48"/>
       <c r="K47" s="28"/>
       <c r="L47" s="28"/>
       <c r="M47" s="28"/>
@@ -14487,7 +14520,7 @@
       <c r="G48" s="28"/>
       <c r="H48" s="28"/>
       <c r="I48" s="29"/>
-      <c r="J48" s="28"/>
+      <c r="J48" s="48"/>
       <c r="K48" s="28"/>
       <c r="L48" s="28"/>
       <c r="M48" s="28"/>
@@ -14776,7 +14809,7 @@
       <c r="G49" s="28"/>
       <c r="H49" s="28"/>
       <c r="I49" s="29"/>
-      <c r="J49" s="28"/>
+      <c r="J49" s="48"/>
       <c r="K49" s="28"/>
       <c r="L49" s="28"/>
       <c r="M49" s="28"/>
@@ -15065,7 +15098,7 @@
       <c r="G50" s="28"/>
       <c r="H50" s="28"/>
       <c r="I50" s="29"/>
-      <c r="J50" s="28"/>
+      <c r="J50" s="48"/>
       <c r="K50" s="28"/>
       <c r="L50" s="28"/>
       <c r="M50" s="28"/>
@@ -15354,7 +15387,7 @@
       <c r="G51" s="28"/>
       <c r="H51" s="28"/>
       <c r="I51" s="29"/>
-      <c r="J51" s="28"/>
+      <c r="J51" s="48"/>
       <c r="K51" s="28"/>
       <c r="L51" s="28"/>
       <c r="M51" s="28"/>
@@ -15643,7 +15676,7 @@
       <c r="G52" s="28"/>
       <c r="H52" s="28"/>
       <c r="I52" s="29"/>
-      <c r="J52" s="28"/>
+      <c r="J52" s="48"/>
       <c r="K52" s="28"/>
       <c r="L52" s="28"/>
       <c r="M52" s="28"/>
@@ -15932,7 +15965,7 @@
       <c r="G53" s="28"/>
       <c r="H53" s="28"/>
       <c r="I53" s="29"/>
-      <c r="J53" s="28"/>
+      <c r="J53" s="48"/>
       <c r="K53" s="28"/>
       <c r="L53" s="28"/>
       <c r="M53" s="28"/>
@@ -16221,7 +16254,7 @@
       <c r="G54" s="28"/>
       <c r="H54" s="28"/>
       <c r="I54" s="29"/>
-      <c r="J54" s="28"/>
+      <c r="J54" s="48"/>
       <c r="K54" s="28"/>
       <c r="L54" s="28"/>
       <c r="M54" s="28"/>
@@ -16510,7 +16543,7 @@
       <c r="G55" s="28"/>
       <c r="H55" s="28"/>
       <c r="I55" s="29"/>
-      <c r="J55" s="28"/>
+      <c r="J55" s="48"/>
       <c r="K55" s="28"/>
       <c r="L55" s="28"/>
       <c r="M55" s="28"/>
@@ -16799,7 +16832,7 @@
       <c r="G56" s="28"/>
       <c r="H56" s="28"/>
       <c r="I56" s="29"/>
-      <c r="J56" s="28"/>
+      <c r="J56" s="48"/>
       <c r="K56" s="28"/>
       <c r="L56" s="28"/>
       <c r="M56" s="28"/>
@@ -17088,7 +17121,7 @@
       <c r="G57" s="28"/>
       <c r="H57" s="28"/>
       <c r="I57" s="29"/>
-      <c r="J57" s="28"/>
+      <c r="J57" s="48"/>
       <c r="K57" s="28"/>
       <c r="L57" s="28"/>
       <c r="M57" s="28"/>
@@ -17377,7 +17410,7 @@
       <c r="G58" s="28"/>
       <c r="H58" s="28"/>
       <c r="I58" s="29"/>
-      <c r="J58" s="28"/>
+      <c r="J58" s="48"/>
       <c r="K58" s="28"/>
       <c r="L58" s="28"/>
       <c r="M58" s="28"/>
@@ -17666,7 +17699,7 @@
       <c r="G59" s="28"/>
       <c r="H59" s="28"/>
       <c r="I59" s="29"/>
-      <c r="J59" s="28"/>
+      <c r="J59" s="48"/>
       <c r="K59" s="28"/>
       <c r="L59" s="28"/>
       <c r="M59" s="28"/>

</xml_diff>

<commit_message>
update_PP - Updating the PP for WEEK3 - Added new Tasks to Mina & Nada
Signed-off-by: Hazemmekawy <dextermekawy@gmail.com>
</commit_message>
<xml_diff>
--- a/SW deliveries log/PP.xlsx
+++ b/SW deliveries log/PP.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\ITI COURSES\Software Engineering\SWE_WORKSPACE\SW deliveries log\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C624C182-2E75-458D-8072-6C7A41A0EBDF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F636B8D3-6689-4D65-8E2A-38D34F5BFBBF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="106" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="57">
   <si>
     <t>Sovy - Digital Calculator PO1_DGC_PROJECT PLAN</t>
   </si>
@@ -185,6 +185,12 @@
   </si>
   <si>
     <t>Except the lastest review that was on 6/2/2020</t>
+  </si>
+  <si>
+    <t>Releasing CYRS/HIS Documents</t>
+  </si>
+  <si>
+    <t>SRS Document Update</t>
   </si>
 </sst>
 </file>
@@ -597,6 +603,21 @@
     <xf numFmtId="164" fontId="21" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="16" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -615,21 +636,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -850,8 +856,8 @@
   </sheetPr>
   <dimension ref="A1:KA1007"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F16" workbookViewId="0">
-      <selection activeCell="J18" sqref="J18"/>
+    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1"/>
@@ -863,22 +869,22 @@
     <col min="5" max="5" width="26.44140625" customWidth="1"/>
     <col min="6" max="8" width="30.44140625" customWidth="1"/>
     <col min="9" max="9" width="29.5546875" customWidth="1"/>
-    <col min="10" max="10" width="58.109375" style="49" customWidth="1"/>
+    <col min="10" max="10" width="58.109375" style="41" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:287" ht="28.2">
-      <c r="A1" s="39" t="s">
+      <c r="A1" s="44" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="38"/>
-      <c r="C1" s="38"/>
-      <c r="D1" s="38"/>
-      <c r="E1" s="38"/>
+      <c r="B1" s="43"/>
+      <c r="C1" s="43"/>
+      <c r="D1" s="43"/>
+      <c r="E1" s="43"/>
       <c r="F1" s="1"/>
       <c r="G1" s="1"/>
       <c r="H1" s="1"/>
       <c r="I1" s="1"/>
-      <c r="J1" s="45"/>
+      <c r="J1" s="37"/>
       <c r="K1" s="2"/>
       <c r="L1" s="2"/>
       <c r="M1" s="2"/>
@@ -1173,13 +1179,13 @@
       <c r="E2" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="40" t="s">
+      <c r="F2" s="45" t="s">
         <v>6</v>
       </c>
-      <c r="G2" s="41"/>
-      <c r="H2" s="41"/>
+      <c r="G2" s="46"/>
+      <c r="H2" s="46"/>
       <c r="I2" s="8"/>
-      <c r="J2" s="46"/>
+      <c r="J2" s="38"/>
       <c r="K2" s="8"/>
       <c r="L2" s="8"/>
       <c r="M2" s="8"/>
@@ -1761,12 +1767,12 @@
       <c r="A4" s="20" t="s">
         <v>12</v>
       </c>
-      <c r="B4" s="42" t="s">
+      <c r="B4" s="47" t="s">
         <v>13</v>
       </c>
-      <c r="C4" s="38"/>
-      <c r="D4" s="38"/>
-      <c r="E4" s="38"/>
+      <c r="C4" s="43"/>
+      <c r="D4" s="43"/>
+      <c r="E4" s="43"/>
       <c r="F4" s="21"/>
       <c r="G4" s="21"/>
       <c r="H4" s="22"/>
@@ -1803,7 +1809,7 @@
       <c r="I5" s="27" t="s">
         <v>23</v>
       </c>
-      <c r="J5" s="47" t="s">
+      <c r="J5" s="39" t="s">
         <v>24</v>
       </c>
       <c r="K5" s="9"/>
@@ -2085,18 +2091,18 @@
       <c r="KA5" s="19"/>
     </row>
     <row r="6" spans="1:287" ht="30.75" customHeight="1">
-      <c r="A6" s="43" t="s">
+      <c r="A6" s="48" t="s">
         <v>25</v>
       </c>
-      <c r="B6" s="44"/>
-      <c r="C6" s="44"/>
-      <c r="D6" s="44"/>
-      <c r="E6" s="44"/>
-      <c r="F6" s="44"/>
-      <c r="G6" s="44"/>
-      <c r="H6" s="44"/>
-      <c r="I6" s="44"/>
-      <c r="J6" s="44"/>
+      <c r="B6" s="49"/>
+      <c r="C6" s="49"/>
+      <c r="D6" s="49"/>
+      <c r="E6" s="49"/>
+      <c r="F6" s="49"/>
+      <c r="G6" s="49"/>
+      <c r="H6" s="49"/>
+      <c r="I6" s="49"/>
+      <c r="J6" s="49"/>
       <c r="K6" s="28"/>
       <c r="L6" s="28"/>
       <c r="M6" s="28"/>
@@ -2376,18 +2382,18 @@
       <c r="KA6" s="28"/>
     </row>
     <row r="7" spans="1:287" ht="30.75" customHeight="1">
-      <c r="A7" s="37" t="s">
+      <c r="A7" s="42" t="s">
         <v>26</v>
       </c>
-      <c r="B7" s="38"/>
-      <c r="C7" s="38"/>
-      <c r="D7" s="38"/>
-      <c r="E7" s="38"/>
-      <c r="F7" s="38"/>
-      <c r="G7" s="38"/>
-      <c r="H7" s="38"/>
-      <c r="I7" s="38"/>
-      <c r="J7" s="38"/>
+      <c r="B7" s="43"/>
+      <c r="C7" s="43"/>
+      <c r="D7" s="43"/>
+      <c r="E7" s="43"/>
+      <c r="F7" s="43"/>
+      <c r="G7" s="43"/>
+      <c r="H7" s="43"/>
+      <c r="I7" s="43"/>
+      <c r="J7" s="43"/>
       <c r="K7" s="28"/>
       <c r="L7" s="28"/>
       <c r="M7" s="28"/>
@@ -2694,7 +2700,7 @@
       <c r="I8" s="29" t="s">
         <v>30</v>
       </c>
-      <c r="J8" s="48"/>
+      <c r="J8" s="40"/>
       <c r="K8" s="28"/>
       <c r="L8" s="28"/>
       <c r="M8" s="28"/>
@@ -3001,7 +3007,7 @@
       <c r="I9" s="29" t="s">
         <v>33</v>
       </c>
-      <c r="J9" s="48" t="s">
+      <c r="J9" s="40" t="s">
         <v>34</v>
       </c>
       <c r="K9" s="28"/>
@@ -3310,7 +3316,7 @@
       <c r="I10" s="29" t="s">
         <v>33</v>
       </c>
-      <c r="J10" s="48" t="s">
+      <c r="J10" s="40" t="s">
         <v>37</v>
       </c>
       <c r="K10" s="28"/>
@@ -3619,7 +3625,7 @@
       <c r="I11" s="29" t="s">
         <v>33</v>
       </c>
-      <c r="J11" s="48" t="s">
+      <c r="J11" s="40" t="s">
         <v>37</v>
       </c>
       <c r="K11" s="28"/>
@@ -3928,7 +3934,7 @@
       <c r="I12" s="29" t="s">
         <v>33</v>
       </c>
-      <c r="J12" s="48" t="s">
+      <c r="J12" s="40" t="s">
         <v>41</v>
       </c>
       <c r="K12" s="28"/>
@@ -4210,18 +4216,18 @@
       <c r="KA12" s="28"/>
     </row>
     <row r="13" spans="1:287" ht="30.75" customHeight="1">
-      <c r="A13" s="37" t="s">
+      <c r="A13" s="42" t="s">
         <v>42</v>
       </c>
-      <c r="B13" s="38"/>
-      <c r="C13" s="38"/>
-      <c r="D13" s="38"/>
-      <c r="E13" s="38"/>
-      <c r="F13" s="38"/>
-      <c r="G13" s="38"/>
-      <c r="H13" s="38"/>
-      <c r="I13" s="38"/>
-      <c r="J13" s="38"/>
+      <c r="B13" s="43"/>
+      <c r="C13" s="43"/>
+      <c r="D13" s="43"/>
+      <c r="E13" s="43"/>
+      <c r="F13" s="43"/>
+      <c r="G13" s="43"/>
+      <c r="H13" s="43"/>
+      <c r="I13" s="43"/>
+      <c r="J13" s="43"/>
       <c r="K13" s="28"/>
       <c r="L13" s="28"/>
       <c r="M13" s="28"/>
@@ -4528,7 +4534,7 @@
       <c r="I14" s="29" t="s">
         <v>33</v>
       </c>
-      <c r="J14" s="48"/>
+      <c r="J14" s="40"/>
       <c r="K14" s="28"/>
       <c r="L14" s="28"/>
       <c r="M14" s="28"/>
@@ -4835,7 +4841,7 @@
       <c r="I15" s="29" t="s">
         <v>33</v>
       </c>
-      <c r="J15" s="48"/>
+      <c r="J15" s="40"/>
       <c r="K15" s="28"/>
       <c r="L15" s="28"/>
       <c r="M15" s="28"/>
@@ -5142,7 +5148,7 @@
       <c r="I16" s="29" t="s">
         <v>33</v>
       </c>
-      <c r="J16" s="48"/>
+      <c r="J16" s="40"/>
       <c r="K16" s="28"/>
       <c r="L16" s="28"/>
       <c r="M16" s="28"/>
@@ -5449,7 +5455,7 @@
       <c r="I17" s="29" t="s">
         <v>33</v>
       </c>
-      <c r="J17" s="48"/>
+      <c r="J17" s="40"/>
       <c r="K17" s="28"/>
       <c r="L17" s="28"/>
       <c r="M17" s="28"/>
@@ -5756,7 +5762,7 @@
       <c r="I18" s="29" t="s">
         <v>33</v>
       </c>
-      <c r="J18" s="48"/>
+      <c r="J18" s="40"/>
       <c r="K18" s="28"/>
       <c r="L18" s="28"/>
       <c r="M18" s="28"/>
@@ -6063,7 +6069,7 @@
       <c r="I19" s="29" t="s">
         <v>33</v>
       </c>
-      <c r="J19" s="48"/>
+      <c r="J19" s="40"/>
       <c r="K19" s="28"/>
       <c r="L19" s="28"/>
       <c r="M19" s="28"/>
@@ -6370,7 +6376,7 @@
       <c r="I20" s="29" t="s">
         <v>33</v>
       </c>
-      <c r="J20" s="48"/>
+      <c r="J20" s="40"/>
       <c r="K20" s="28"/>
       <c r="L20" s="28"/>
       <c r="M20" s="28"/>
@@ -6677,7 +6683,7 @@
       <c r="I21" s="29" t="s">
         <v>33</v>
       </c>
-      <c r="J21" s="48"/>
+      <c r="J21" s="40"/>
       <c r="K21" s="28"/>
       <c r="L21" s="28"/>
       <c r="M21" s="28"/>
@@ -6984,7 +6990,7 @@
       <c r="I22" s="29" t="s">
         <v>33</v>
       </c>
-      <c r="J22" s="48"/>
+      <c r="J22" s="40"/>
       <c r="K22" s="28"/>
       <c r="L22" s="28"/>
       <c r="M22" s="28"/>
@@ -7291,7 +7297,7 @@
       <c r="I23" s="29" t="s">
         <v>33</v>
       </c>
-      <c r="J23" s="48" t="s">
+      <c r="J23" s="40" t="s">
         <v>54</v>
       </c>
       <c r="K23" s="28"/>
@@ -7573,18 +7579,18 @@
       <c r="KA23" s="28"/>
     </row>
     <row r="24" spans="1:287" ht="30.75" customHeight="1">
-      <c r="A24" s="37" t="s">
+      <c r="A24" s="42" t="s">
         <v>53</v>
       </c>
-      <c r="B24" s="38"/>
-      <c r="C24" s="38"/>
-      <c r="D24" s="38"/>
-      <c r="E24" s="38"/>
-      <c r="F24" s="38"/>
-      <c r="G24" s="38"/>
-      <c r="H24" s="38"/>
-      <c r="I24" s="38"/>
-      <c r="J24" s="38"/>
+      <c r="B24" s="43"/>
+      <c r="C24" s="43"/>
+      <c r="D24" s="43"/>
+      <c r="E24" s="43"/>
+      <c r="F24" s="43"/>
+      <c r="G24" s="43"/>
+      <c r="H24" s="43"/>
+      <c r="I24" s="43"/>
+      <c r="J24" s="43"/>
       <c r="K24" s="28"/>
       <c r="L24" s="28"/>
       <c r="M24" s="28"/>
@@ -7864,16 +7870,34 @@
       <c r="KA24" s="28"/>
     </row>
     <row r="25" spans="1:287" ht="30.75" customHeight="1">
-      <c r="A25" s="33"/>
-      <c r="B25" s="28"/>
-      <c r="C25" s="30"/>
-      <c r="D25" s="28"/>
-      <c r="E25" s="28"/>
-      <c r="F25" s="28"/>
-      <c r="G25" s="28"/>
-      <c r="H25" s="28"/>
-      <c r="I25" s="29"/>
-      <c r="J25" s="48"/>
+      <c r="A25" s="33" t="s">
+        <v>43</v>
+      </c>
+      <c r="B25" s="28" t="s">
+        <v>28</v>
+      </c>
+      <c r="C25" s="30" t="s">
+        <v>36</v>
+      </c>
+      <c r="D25" s="35">
+        <v>43869</v>
+      </c>
+      <c r="E25" s="35">
+        <v>43869</v>
+      </c>
+      <c r="F25" s="35">
+        <v>43869</v>
+      </c>
+      <c r="G25" s="35">
+        <v>43869</v>
+      </c>
+      <c r="H25" s="28">
+        <v>1</v>
+      </c>
+      <c r="I25" s="29" t="s">
+        <v>30</v>
+      </c>
+      <c r="J25" s="40"/>
       <c r="K25" s="28"/>
       <c r="L25" s="28"/>
       <c r="M25" s="28"/>
@@ -8153,16 +8177,34 @@
       <c r="KA25" s="28"/>
     </row>
     <row r="26" spans="1:287" ht="30.75" customHeight="1">
-      <c r="A26" s="33"/>
-      <c r="B26" s="28"/>
-      <c r="C26" s="30"/>
-      <c r="D26" s="28"/>
-      <c r="E26" s="28"/>
-      <c r="F26" s="28"/>
-      <c r="G26" s="28"/>
-      <c r="H26" s="28"/>
-      <c r="I26" s="29"/>
-      <c r="J26" s="48"/>
+      <c r="A26" s="33" t="s">
+        <v>50</v>
+      </c>
+      <c r="B26" s="30" t="s">
+        <v>28</v>
+      </c>
+      <c r="C26" s="30" t="s">
+        <v>36</v>
+      </c>
+      <c r="D26" s="35">
+        <v>43869</v>
+      </c>
+      <c r="E26" s="35">
+        <v>43869</v>
+      </c>
+      <c r="F26" s="35">
+        <v>43869</v>
+      </c>
+      <c r="G26" s="35">
+        <v>43869</v>
+      </c>
+      <c r="H26" s="28">
+        <v>1</v>
+      </c>
+      <c r="I26" s="29" t="s">
+        <v>30</v>
+      </c>
+      <c r="J26" s="40"/>
       <c r="K26" s="28"/>
       <c r="L26" s="28"/>
       <c r="M26" s="28"/>
@@ -8442,16 +8484,34 @@
       <c r="KA26" s="28"/>
     </row>
     <row r="27" spans="1:287" ht="30.75" customHeight="1">
-      <c r="A27" s="33"/>
-      <c r="B27" s="28"/>
-      <c r="C27" s="30"/>
-      <c r="D27" s="28"/>
-      <c r="E27" s="28"/>
-      <c r="F27" s="28"/>
-      <c r="G27" s="28"/>
-      <c r="H27" s="28"/>
-      <c r="I27" s="29"/>
-      <c r="J27" s="48"/>
+      <c r="A27" s="33" t="s">
+        <v>55</v>
+      </c>
+      <c r="B27" s="30" t="s">
+        <v>28</v>
+      </c>
+      <c r="C27" s="30" t="s">
+        <v>8</v>
+      </c>
+      <c r="D27" s="35">
+        <v>43869</v>
+      </c>
+      <c r="E27" s="35">
+        <v>43869</v>
+      </c>
+      <c r="F27" s="35">
+        <v>43869</v>
+      </c>
+      <c r="G27" s="35">
+        <v>43869</v>
+      </c>
+      <c r="H27" s="28">
+        <v>1</v>
+      </c>
+      <c r="I27" s="29" t="s">
+        <v>30</v>
+      </c>
+      <c r="J27" s="40"/>
       <c r="K27" s="28"/>
       <c r="L27" s="28"/>
       <c r="M27" s="28"/>
@@ -8731,16 +8791,32 @@
       <c r="KA27" s="28"/>
     </row>
     <row r="28" spans="1:287" ht="30.75" customHeight="1">
-      <c r="A28" s="33"/>
-      <c r="B28" s="28"/>
-      <c r="C28" s="30"/>
-      <c r="D28" s="28"/>
-      <c r="E28" s="28"/>
-      <c r="F28" s="28"/>
+      <c r="A28" s="33" t="s">
+        <v>56</v>
+      </c>
+      <c r="B28" s="28" t="s">
+        <v>28</v>
+      </c>
+      <c r="C28" s="30" t="s">
+        <v>32</v>
+      </c>
+      <c r="D28" s="35">
+        <v>43869</v>
+      </c>
+      <c r="E28" s="35">
+        <v>43869</v>
+      </c>
+      <c r="F28" s="35">
+        <v>43869</v>
+      </c>
       <c r="G28" s="28"/>
-      <c r="H28" s="28"/>
-      <c r="I28" s="29"/>
-      <c r="J28" s="48"/>
+      <c r="H28" s="28">
+        <v>1</v>
+      </c>
+      <c r="I28" s="29" t="s">
+        <v>30</v>
+      </c>
+      <c r="J28" s="40"/>
       <c r="K28" s="28"/>
       <c r="L28" s="28"/>
       <c r="M28" s="28"/>
@@ -9029,7 +9105,7 @@
       <c r="G29" s="28"/>
       <c r="H29" s="28"/>
       <c r="I29" s="29"/>
-      <c r="J29" s="48"/>
+      <c r="J29" s="40"/>
       <c r="K29" s="28"/>
       <c r="L29" s="28"/>
       <c r="M29" s="28"/>
@@ -9318,7 +9394,7 @@
       <c r="G30" s="28"/>
       <c r="H30" s="28"/>
       <c r="I30" s="29"/>
-      <c r="J30" s="48"/>
+      <c r="J30" s="40"/>
       <c r="K30" s="28"/>
       <c r="L30" s="28"/>
       <c r="M30" s="28"/>
@@ -9607,7 +9683,7 @@
       <c r="G31" s="28"/>
       <c r="H31" s="28"/>
       <c r="I31" s="29"/>
-      <c r="J31" s="48"/>
+      <c r="J31" s="40"/>
       <c r="K31" s="28"/>
       <c r="L31" s="28"/>
       <c r="M31" s="28"/>
@@ -9896,7 +9972,7 @@
       <c r="G32" s="28"/>
       <c r="H32" s="28"/>
       <c r="I32" s="29"/>
-      <c r="J32" s="48"/>
+      <c r="J32" s="40"/>
       <c r="K32" s="28"/>
       <c r="L32" s="28"/>
       <c r="M32" s="28"/>
@@ -10185,7 +10261,7 @@
       <c r="G33" s="28"/>
       <c r="H33" s="28"/>
       <c r="I33" s="29"/>
-      <c r="J33" s="48"/>
+      <c r="J33" s="40"/>
       <c r="K33" s="28"/>
       <c r="L33" s="28"/>
       <c r="M33" s="28"/>
@@ -10474,7 +10550,7 @@
       <c r="G34" s="28"/>
       <c r="H34" s="28"/>
       <c r="I34" s="29"/>
-      <c r="J34" s="48"/>
+      <c r="J34" s="40"/>
       <c r="K34" s="28"/>
       <c r="L34" s="28"/>
       <c r="M34" s="28"/>
@@ -10763,7 +10839,7 @@
       <c r="G35" s="28"/>
       <c r="H35" s="28"/>
       <c r="I35" s="29"/>
-      <c r="J35" s="48"/>
+      <c r="J35" s="40"/>
       <c r="K35" s="28"/>
       <c r="L35" s="28"/>
       <c r="M35" s="28"/>
@@ -11052,7 +11128,7 @@
       <c r="G36" s="28"/>
       <c r="H36" s="28"/>
       <c r="I36" s="29"/>
-      <c r="J36" s="48"/>
+      <c r="J36" s="40"/>
       <c r="K36" s="28"/>
       <c r="L36" s="28"/>
       <c r="M36" s="28"/>
@@ -11341,7 +11417,7 @@
       <c r="G37" s="28"/>
       <c r="H37" s="28"/>
       <c r="I37" s="29"/>
-      <c r="J37" s="48"/>
+      <c r="J37" s="40"/>
       <c r="K37" s="28"/>
       <c r="L37" s="28"/>
       <c r="M37" s="28"/>
@@ -11630,7 +11706,7 @@
       <c r="G38" s="28"/>
       <c r="H38" s="28"/>
       <c r="I38" s="29"/>
-      <c r="J38" s="48"/>
+      <c r="J38" s="40"/>
       <c r="K38" s="28"/>
       <c r="L38" s="28"/>
       <c r="M38" s="28"/>
@@ -11919,7 +11995,7 @@
       <c r="G39" s="28"/>
       <c r="H39" s="28"/>
       <c r="I39" s="29"/>
-      <c r="J39" s="48"/>
+      <c r="J39" s="40"/>
       <c r="K39" s="28"/>
       <c r="L39" s="28"/>
       <c r="M39" s="28"/>
@@ -12208,7 +12284,7 @@
       <c r="G40" s="28"/>
       <c r="H40" s="28"/>
       <c r="I40" s="29"/>
-      <c r="J40" s="48"/>
+      <c r="J40" s="40"/>
       <c r="K40" s="28"/>
       <c r="L40" s="28"/>
       <c r="M40" s="28"/>
@@ -12497,7 +12573,7 @@
       <c r="G41" s="28"/>
       <c r="H41" s="28"/>
       <c r="I41" s="29"/>
-      <c r="J41" s="48"/>
+      <c r="J41" s="40"/>
       <c r="K41" s="28"/>
       <c r="L41" s="28"/>
       <c r="M41" s="28"/>
@@ -12786,7 +12862,7 @@
       <c r="G42" s="28"/>
       <c r="H42" s="28"/>
       <c r="I42" s="29"/>
-      <c r="J42" s="48"/>
+      <c r="J42" s="40"/>
       <c r="K42" s="28"/>
       <c r="L42" s="28"/>
       <c r="M42" s="28"/>
@@ -13075,7 +13151,7 @@
       <c r="G43" s="28"/>
       <c r="H43" s="28"/>
       <c r="I43" s="29"/>
-      <c r="J43" s="48"/>
+      <c r="J43" s="40"/>
       <c r="K43" s="28"/>
       <c r="L43" s="28"/>
       <c r="M43" s="28"/>
@@ -13364,7 +13440,7 @@
       <c r="G44" s="28"/>
       <c r="H44" s="28"/>
       <c r="I44" s="29"/>
-      <c r="J44" s="48"/>
+      <c r="J44" s="40"/>
       <c r="K44" s="28"/>
       <c r="L44" s="28"/>
       <c r="M44" s="28"/>
@@ -13653,7 +13729,7 @@
       <c r="G45" s="28"/>
       <c r="H45" s="28"/>
       <c r="I45" s="29"/>
-      <c r="J45" s="48"/>
+      <c r="J45" s="40"/>
       <c r="K45" s="28"/>
       <c r="L45" s="28"/>
       <c r="M45" s="28"/>
@@ -13942,7 +14018,7 @@
       <c r="G46" s="28"/>
       <c r="H46" s="28"/>
       <c r="I46" s="29"/>
-      <c r="J46" s="48"/>
+      <c r="J46" s="40"/>
       <c r="K46" s="28"/>
       <c r="L46" s="28"/>
       <c r="M46" s="28"/>
@@ -14231,7 +14307,7 @@
       <c r="G47" s="28"/>
       <c r="H47" s="28"/>
       <c r="I47" s="29"/>
-      <c r="J47" s="48"/>
+      <c r="J47" s="40"/>
       <c r="K47" s="28"/>
       <c r="L47" s="28"/>
       <c r="M47" s="28"/>
@@ -14520,7 +14596,7 @@
       <c r="G48" s="28"/>
       <c r="H48" s="28"/>
       <c r="I48" s="29"/>
-      <c r="J48" s="48"/>
+      <c r="J48" s="40"/>
       <c r="K48" s="28"/>
       <c r="L48" s="28"/>
       <c r="M48" s="28"/>
@@ -14809,7 +14885,7 @@
       <c r="G49" s="28"/>
       <c r="H49" s="28"/>
       <c r="I49" s="29"/>
-      <c r="J49" s="48"/>
+      <c r="J49" s="40"/>
       <c r="K49" s="28"/>
       <c r="L49" s="28"/>
       <c r="M49" s="28"/>
@@ -15098,7 +15174,7 @@
       <c r="G50" s="28"/>
       <c r="H50" s="28"/>
       <c r="I50" s="29"/>
-      <c r="J50" s="48"/>
+      <c r="J50" s="40"/>
       <c r="K50" s="28"/>
       <c r="L50" s="28"/>
       <c r="M50" s="28"/>
@@ -15387,7 +15463,7 @@
       <c r="G51" s="28"/>
       <c r="H51" s="28"/>
       <c r="I51" s="29"/>
-      <c r="J51" s="48"/>
+      <c r="J51" s="40"/>
       <c r="K51" s="28"/>
       <c r="L51" s="28"/>
       <c r="M51" s="28"/>
@@ -15676,7 +15752,7 @@
       <c r="G52" s="28"/>
       <c r="H52" s="28"/>
       <c r="I52" s="29"/>
-      <c r="J52" s="48"/>
+      <c r="J52" s="40"/>
       <c r="K52" s="28"/>
       <c r="L52" s="28"/>
       <c r="M52" s="28"/>
@@ -15965,7 +16041,7 @@
       <c r="G53" s="28"/>
       <c r="H53" s="28"/>
       <c r="I53" s="29"/>
-      <c r="J53" s="48"/>
+      <c r="J53" s="40"/>
       <c r="K53" s="28"/>
       <c r="L53" s="28"/>
       <c r="M53" s="28"/>
@@ -16254,7 +16330,7 @@
       <c r="G54" s="28"/>
       <c r="H54" s="28"/>
       <c r="I54" s="29"/>
-      <c r="J54" s="48"/>
+      <c r="J54" s="40"/>
       <c r="K54" s="28"/>
       <c r="L54" s="28"/>
       <c r="M54" s="28"/>
@@ -16543,7 +16619,7 @@
       <c r="G55" s="28"/>
       <c r="H55" s="28"/>
       <c r="I55" s="29"/>
-      <c r="J55" s="48"/>
+      <c r="J55" s="40"/>
       <c r="K55" s="28"/>
       <c r="L55" s="28"/>
       <c r="M55" s="28"/>
@@ -16832,7 +16908,7 @@
       <c r="G56" s="28"/>
       <c r="H56" s="28"/>
       <c r="I56" s="29"/>
-      <c r="J56" s="48"/>
+      <c r="J56" s="40"/>
       <c r="K56" s="28"/>
       <c r="L56" s="28"/>
       <c r="M56" s="28"/>
@@ -17121,7 +17197,7 @@
       <c r="G57" s="28"/>
       <c r="H57" s="28"/>
       <c r="I57" s="29"/>
-      <c r="J57" s="48"/>
+      <c r="J57" s="40"/>
       <c r="K57" s="28"/>
       <c r="L57" s="28"/>
       <c r="M57" s="28"/>
@@ -17410,7 +17486,7 @@
       <c r="G58" s="28"/>
       <c r="H58" s="28"/>
       <c r="I58" s="29"/>
-      <c r="J58" s="48"/>
+      <c r="J58" s="40"/>
       <c r="K58" s="28"/>
       <c r="L58" s="28"/>
       <c r="M58" s="28"/>
@@ -17699,7 +17775,7 @@
       <c r="G59" s="28"/>
       <c r="H59" s="28"/>
       <c r="I59" s="29"/>
-      <c r="J59" s="48"/>
+      <c r="J59" s="40"/>
       <c r="K59" s="28"/>
       <c r="L59" s="28"/>
       <c r="M59" s="28"/>
@@ -20836,7 +20912,7 @@
     <dataValidation type="list" allowBlank="1" sqref="I8:I12 I25:I59 I14:I23" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>"STILL,ON GOING,DELIVERED,DELIVERED (LATE)"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" sqref="B8:B12 B25:B59 B14:B23" xr:uid="{00000000-0002-0000-0000-000001000000}">
+    <dataValidation type="list" allowBlank="1" sqref="B8:B12 B14:B23 B25:B59" xr:uid="{00000000-0002-0000-0000-000001000000}">
       <formula1>"Technical,Non -Technical"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" sqref="C8:C12 C25:C59 C14:C23" xr:uid="{00000000-0002-0000-0000-000002000000}">

</xml_diff>

<commit_message>
Updated PP -Delivery status Signed-off-by: Hazemmekawy <dextermekawy@gmail.com>
</commit_message>
<xml_diff>
--- a/SW deliveries log/PP.xlsx
+++ b/SW deliveries log/PP.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\ITI COURSES\Software Engineering\SWE_WORKSPACE\SW deliveries log\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F636B8D3-6689-4D65-8E2A-38D34F5BFBBF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1ECD568-1586-4F40-A150-EB464319C1AB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="106" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -856,8 +856,8 @@
   </sheetPr>
   <dimension ref="A1:KA1007"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
-      <selection activeCell="C28" sqref="C28"/>
+    <sheetView tabSelected="1" topLeftCell="F21" workbookViewId="0">
+      <selection activeCell="H29" sqref="H29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1"/>
@@ -7895,7 +7895,7 @@
         <v>1</v>
       </c>
       <c r="I25" s="29" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="J25" s="40"/>
       <c r="K25" s="28"/>
@@ -8202,7 +8202,7 @@
         <v>1</v>
       </c>
       <c r="I26" s="29" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="J26" s="40"/>
       <c r="K26" s="28"/>
@@ -8509,7 +8509,7 @@
         <v>1</v>
       </c>
       <c r="I27" s="29" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="J27" s="40"/>
       <c r="K27" s="28"/>
@@ -8809,12 +8809,14 @@
       <c r="F28" s="35">
         <v>43869</v>
       </c>
-      <c r="G28" s="28"/>
+      <c r="G28" s="35">
+        <v>43869</v>
+      </c>
       <c r="H28" s="28">
         <v>1</v>
       </c>
       <c r="I28" s="29" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="J28" s="40"/>
       <c r="K28" s="28"/>

</xml_diff>

<commit_message>
Check the project plan according to the the latest changes in CRS Signed-off-by: Hazemmekawy <dextermekawy@gmail.com>
</commit_message>
<xml_diff>
--- a/SW deliveries log/PP.xlsx
+++ b/SW deliveries log/PP.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\ITI COURSES\Software Engineering\SWE_WORKSPACE\SW deliveries log\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCE26BD6-ACD0-4037-B01C-6859465CF00E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D57DEC64-0A7A-46DF-9E51-B48BD23F000C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="106" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="65">
   <si>
     <t>Sovy - Digital Calculator PO1_DGC_PROJECT PLAN</t>
   </si>
@@ -181,9 +181,6 @@
     <t>Except the lastest review that was on 6/2/2020</t>
   </si>
   <si>
-    <t>Releasing CYRS/HIS Documents</t>
-  </si>
-  <si>
     <t>SRS Document Update</t>
   </si>
   <si>
@@ -204,6 +201,23 @@
   <si>
     <t>Documentation</t>
   </si>
+  <si>
+    <t>WEEK 4 (CRS Update Cycle)</t>
+  </si>
+  <si>
+    <t>Releasing CYRS/HSI Documents</t>
+  </si>
+  <si>
+    <t>CYRS Documuent Update</t>
+  </si>
+  <si>
+    <t>Updating the CYRS according to these changes:
+- Adding the clear switch separate from the keypad
+- Adding the new opearands limits</t>
+  </si>
+  <si>
+    <t>GDD Document Update</t>
+  </si>
 </sst>
 </file>
 
@@ -212,7 +226,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="mmmm\ d\,\ yyyy"/>
   </numFmts>
-  <fonts count="22">
+  <fonts count="23">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -338,8 +352,15 @@
       <name val="Georgia"/>
       <family val="1"/>
     </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="7">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -373,6 +394,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="8"/>
+        <bgColor theme="8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
         <bgColor theme="8"/>
       </patternFill>
     </fill>
@@ -505,7 +538,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="51">
+  <cellXfs count="57">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -649,6 +682,22 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="22" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="20" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -867,10 +916,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:KA1001"/>
+  <dimension ref="A1:KA999"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="F33" sqref="F33"/>
+    <sheetView tabSelected="1" topLeftCell="B28" workbookViewId="0">
+      <selection activeCell="J38" sqref="J38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1"/>
@@ -1799,7 +1848,7 @@
         <v>15</v>
       </c>
       <c r="B5" s="24" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C5" s="24" t="s">
         <v>16</v>
@@ -2690,7 +2739,7 @@
         <v>26</v>
       </c>
       <c r="B8" s="30" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C8" s="30" t="s">
         <v>8</v>
@@ -2997,7 +3046,7 @@
         <v>29</v>
       </c>
       <c r="B9" s="30" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C9" s="30" t="s">
         <v>30</v>
@@ -3306,7 +3355,7 @@
         <v>33</v>
       </c>
       <c r="B10" s="30" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C10" s="30" t="s">
         <v>34</v>
@@ -3615,7 +3664,7 @@
         <v>33</v>
       </c>
       <c r="B11" s="30" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C11" s="30" t="s">
         <v>36</v>
@@ -3924,7 +3973,7 @@
         <v>37</v>
       </c>
       <c r="B12" s="30" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C12" s="30" t="s">
         <v>38</v>
@@ -4524,7 +4573,7 @@
         <v>41</v>
       </c>
       <c r="B14" s="30" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C14" s="30" t="s">
         <v>38</v>
@@ -4831,7 +4880,7 @@
         <v>42</v>
       </c>
       <c r="B15" s="30" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C15" s="30" t="s">
         <v>36</v>
@@ -5138,7 +5187,7 @@
         <v>43</v>
       </c>
       <c r="B16" s="30" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C16" s="30" t="s">
         <v>34</v>
@@ -5445,7 +5494,7 @@
         <v>44</v>
       </c>
       <c r="B17" s="30" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C17" s="30" t="s">
         <v>30</v>
@@ -5752,7 +5801,7 @@
         <v>47</v>
       </c>
       <c r="B18" s="30" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C18" s="30" t="s">
         <v>8</v>
@@ -6059,7 +6108,7 @@
         <v>45</v>
       </c>
       <c r="B19" s="30" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C19" s="30" t="s">
         <v>8</v>
@@ -6366,7 +6415,7 @@
         <v>46</v>
       </c>
       <c r="B20" s="30" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C20" s="30" t="s">
         <v>36</v>
@@ -6673,7 +6722,7 @@
         <v>48</v>
       </c>
       <c r="B21" s="30" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C21" s="30" t="s">
         <v>38</v>
@@ -6980,7 +7029,7 @@
         <v>49</v>
       </c>
       <c r="B22" s="30" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C22" s="30" t="s">
         <v>34</v>
@@ -7287,7 +7336,7 @@
         <v>50</v>
       </c>
       <c r="B23" s="30" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C23" s="30" t="s">
         <v>8</v>
@@ -7887,7 +7936,7 @@
         <v>41</v>
       </c>
       <c r="B25" s="30" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C25" s="30" t="s">
         <v>34</v>
@@ -8194,7 +8243,7 @@
         <v>48</v>
       </c>
       <c r="B26" s="30" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C26" s="30" t="s">
         <v>34</v>
@@ -8498,10 +8547,10 @@
     </row>
     <row r="27" spans="1:287" ht="30.75" customHeight="1">
       <c r="A27" s="33" t="s">
-        <v>53</v>
+        <v>61</v>
       </c>
       <c r="B27" s="30" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C27" s="30" t="s">
         <v>8</v>
@@ -8805,10 +8854,10 @@
     </row>
     <row r="28" spans="1:287" ht="30.75" customHeight="1">
       <c r="A28" s="33" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B28" s="30" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C28" s="30" t="s">
         <v>30</v>
@@ -9111,8 +9160,8 @@
       <c r="KA28" s="28"/>
     </row>
     <row r="29" spans="1:287" s="42" customFormat="1" ht="30.75" customHeight="1">
-      <c r="A29" s="43" t="s">
-        <v>55</v>
+      <c r="A29" s="51" t="s">
+        <v>54</v>
       </c>
       <c r="B29" s="44"/>
       <c r="C29" s="44"/>
@@ -9403,10 +9452,10 @@
     </row>
     <row r="30" spans="1:287" s="42" customFormat="1" ht="30.75" customHeight="1">
       <c r="A30" s="33" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B30" s="30" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C30" s="30" t="s">
         <v>30</v>
@@ -9420,8 +9469,12 @@
       <c r="F30" s="35">
         <v>43883</v>
       </c>
-      <c r="G30" s="35"/>
-      <c r="H30" s="30"/>
+      <c r="G30" s="35">
+        <v>43885</v>
+      </c>
+      <c r="H30" s="30">
+        <v>3</v>
+      </c>
       <c r="I30" s="33" t="s">
         <v>28</v>
       </c>
@@ -9709,7 +9762,7 @@
         <v>47</v>
       </c>
       <c r="B31" s="30" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C31" s="30" t="s">
         <v>38</v>
@@ -9720,11 +9773,17 @@
       <c r="E31" s="35">
         <v>43884</v>
       </c>
-      <c r="F31" s="35"/>
-      <c r="G31" s="35"/>
-      <c r="H31" s="30"/>
+      <c r="F31" s="35">
+        <v>43885</v>
+      </c>
+      <c r="G31" s="35">
+        <v>43885</v>
+      </c>
+      <c r="H31" s="30">
+        <v>1</v>
+      </c>
       <c r="I31" s="33" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="J31" s="40"/>
       <c r="K31" s="30"/>
@@ -10007,10 +10066,10 @@
     </row>
     <row r="32" spans="1:287" ht="30.75" customHeight="1">
       <c r="A32" s="33" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B32" s="30" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C32" s="30" t="s">
         <v>36</v>
@@ -10021,11 +10080,17 @@
       <c r="E32" s="35">
         <v>43886</v>
       </c>
-      <c r="F32" s="28"/>
-      <c r="G32" s="28"/>
-      <c r="H32" s="28"/>
+      <c r="F32" s="35">
+        <v>43885</v>
+      </c>
+      <c r="G32" s="35">
+        <v>43887</v>
+      </c>
+      <c r="H32" s="28">
+        <v>3</v>
+      </c>
       <c r="I32" s="33" t="s">
-        <v>58</v>
+        <v>31</v>
       </c>
       <c r="J32" s="40"/>
       <c r="K32" s="28"/>
@@ -10306,606 +10371,622 @@
       <c r="JZ32" s="28"/>
       <c r="KA32" s="28"/>
     </row>
-    <row r="33" spans="1:287" s="42" customFormat="1" ht="30.75" customHeight="1">
-      <c r="A33" s="32" t="s">
+    <row r="33" spans="1:287" ht="30.75" customHeight="1">
+      <c r="A33" s="52" t="s">
+        <v>60</v>
+      </c>
+      <c r="B33" s="53"/>
+      <c r="C33" s="53"/>
+      <c r="D33" s="53"/>
+      <c r="E33" s="53"/>
+      <c r="F33" s="53"/>
+      <c r="G33" s="53"/>
+      <c r="H33" s="53"/>
+      <c r="I33" s="53"/>
+      <c r="J33" s="53"/>
+      <c r="K33" s="28"/>
+      <c r="L33" s="28"/>
+      <c r="M33" s="28"/>
+      <c r="N33" s="28"/>
+      <c r="O33" s="28"/>
+      <c r="P33" s="28"/>
+      <c r="Q33" s="28"/>
+      <c r="R33" s="28"/>
+      <c r="S33" s="28"/>
+      <c r="T33" s="28"/>
+      <c r="U33" s="28"/>
+      <c r="V33" s="28"/>
+      <c r="W33" s="28"/>
+      <c r="X33" s="28"/>
+      <c r="Y33" s="28"/>
+      <c r="Z33" s="28"/>
+      <c r="AA33" s="28"/>
+      <c r="AB33" s="28"/>
+      <c r="AC33" s="28"/>
+      <c r="AD33" s="28"/>
+      <c r="AE33" s="28"/>
+      <c r="AF33" s="28"/>
+      <c r="AG33" s="28"/>
+      <c r="AH33" s="28"/>
+      <c r="AI33" s="28"/>
+      <c r="AJ33" s="28"/>
+      <c r="AK33" s="28"/>
+      <c r="AL33" s="28"/>
+      <c r="AM33" s="28"/>
+      <c r="AN33" s="28"/>
+      <c r="AO33" s="28"/>
+      <c r="AP33" s="28"/>
+      <c r="AQ33" s="28"/>
+      <c r="AR33" s="28"/>
+      <c r="AS33" s="28"/>
+      <c r="AT33" s="28"/>
+      <c r="AU33" s="28"/>
+      <c r="AV33" s="28"/>
+      <c r="AW33" s="28"/>
+      <c r="AX33" s="28"/>
+      <c r="AY33" s="28"/>
+      <c r="AZ33" s="28"/>
+      <c r="BA33" s="28"/>
+      <c r="BB33" s="28"/>
+      <c r="BC33" s="28"/>
+      <c r="BD33" s="28"/>
+      <c r="BE33" s="28"/>
+      <c r="BF33" s="28"/>
+      <c r="BG33" s="28"/>
+      <c r="BH33" s="28"/>
+      <c r="BI33" s="28"/>
+      <c r="BJ33" s="28"/>
+      <c r="BK33" s="28"/>
+      <c r="BL33" s="28"/>
+      <c r="BM33" s="28"/>
+      <c r="BN33" s="28"/>
+      <c r="BO33" s="28"/>
+      <c r="BP33" s="28"/>
+      <c r="BQ33" s="28"/>
+      <c r="BR33" s="28"/>
+      <c r="BS33" s="28"/>
+      <c r="BT33" s="28"/>
+      <c r="BU33" s="28"/>
+      <c r="BV33" s="28"/>
+      <c r="BW33" s="28"/>
+      <c r="BX33" s="28"/>
+      <c r="BY33" s="28"/>
+      <c r="BZ33" s="28"/>
+      <c r="CA33" s="28"/>
+      <c r="CB33" s="28"/>
+      <c r="CC33" s="28"/>
+      <c r="CD33" s="28"/>
+      <c r="CE33" s="28"/>
+      <c r="CF33" s="28"/>
+      <c r="CG33" s="28"/>
+      <c r="CH33" s="28"/>
+      <c r="CI33" s="28"/>
+      <c r="CJ33" s="28"/>
+      <c r="CK33" s="28"/>
+      <c r="CL33" s="28"/>
+      <c r="CM33" s="28"/>
+      <c r="CN33" s="28"/>
+      <c r="CO33" s="28"/>
+      <c r="CP33" s="28"/>
+      <c r="CQ33" s="28"/>
+      <c r="CR33" s="28"/>
+      <c r="CS33" s="28"/>
+      <c r="CT33" s="28"/>
+      <c r="CU33" s="28"/>
+      <c r="CV33" s="28"/>
+      <c r="CW33" s="28"/>
+      <c r="CX33" s="28"/>
+      <c r="CY33" s="28"/>
+      <c r="CZ33" s="28"/>
+      <c r="DA33" s="28"/>
+      <c r="DB33" s="28"/>
+      <c r="DC33" s="28"/>
+      <c r="DD33" s="28"/>
+      <c r="DE33" s="28"/>
+      <c r="DF33" s="28"/>
+      <c r="DG33" s="28"/>
+      <c r="DH33" s="28"/>
+      <c r="DI33" s="28"/>
+      <c r="DJ33" s="28"/>
+      <c r="DK33" s="28"/>
+      <c r="DL33" s="28"/>
+      <c r="DM33" s="28"/>
+      <c r="DN33" s="28"/>
+      <c r="DO33" s="28"/>
+      <c r="DP33" s="28"/>
+      <c r="DQ33" s="28"/>
+      <c r="DR33" s="28"/>
+      <c r="DS33" s="28"/>
+      <c r="DT33" s="28"/>
+      <c r="DU33" s="28"/>
+      <c r="DV33" s="28"/>
+      <c r="DW33" s="28"/>
+      <c r="DX33" s="28"/>
+      <c r="DY33" s="28"/>
+      <c r="DZ33" s="28"/>
+      <c r="EA33" s="28"/>
+      <c r="EB33" s="28"/>
+      <c r="EC33" s="28"/>
+      <c r="ED33" s="28"/>
+      <c r="EE33" s="28"/>
+      <c r="EF33" s="28"/>
+      <c r="EG33" s="28"/>
+      <c r="EH33" s="28"/>
+      <c r="EI33" s="28"/>
+      <c r="EJ33" s="28"/>
+      <c r="EK33" s="28"/>
+      <c r="EL33" s="28"/>
+      <c r="EM33" s="28"/>
+      <c r="EN33" s="28"/>
+      <c r="EO33" s="28"/>
+      <c r="EP33" s="28"/>
+      <c r="EQ33" s="28"/>
+      <c r="ER33" s="28"/>
+      <c r="ES33" s="28"/>
+      <c r="ET33" s="28"/>
+      <c r="EU33" s="28"/>
+      <c r="EV33" s="28"/>
+      <c r="EW33" s="28"/>
+      <c r="EX33" s="28"/>
+      <c r="EY33" s="28"/>
+      <c r="EZ33" s="28"/>
+      <c r="FA33" s="28"/>
+      <c r="FB33" s="28"/>
+      <c r="FC33" s="28"/>
+      <c r="FD33" s="28"/>
+      <c r="FE33" s="28"/>
+      <c r="FF33" s="28"/>
+      <c r="FG33" s="28"/>
+      <c r="FH33" s="28"/>
+      <c r="FI33" s="28"/>
+      <c r="FJ33" s="28"/>
+      <c r="FK33" s="28"/>
+      <c r="FL33" s="28"/>
+      <c r="FM33" s="28"/>
+      <c r="FN33" s="28"/>
+      <c r="FO33" s="28"/>
+      <c r="FP33" s="28"/>
+      <c r="FQ33" s="28"/>
+      <c r="FR33" s="28"/>
+      <c r="FS33" s="28"/>
+      <c r="FT33" s="28"/>
+      <c r="FU33" s="28"/>
+      <c r="FV33" s="28"/>
+      <c r="FW33" s="28"/>
+      <c r="FX33" s="28"/>
+      <c r="FY33" s="28"/>
+      <c r="FZ33" s="28"/>
+      <c r="GA33" s="28"/>
+      <c r="GB33" s="28"/>
+      <c r="GC33" s="28"/>
+      <c r="GD33" s="28"/>
+      <c r="GE33" s="28"/>
+      <c r="GF33" s="28"/>
+      <c r="GG33" s="28"/>
+      <c r="GH33" s="28"/>
+      <c r="GI33" s="28"/>
+      <c r="GJ33" s="28"/>
+      <c r="GK33" s="28"/>
+      <c r="GL33" s="28"/>
+      <c r="GM33" s="28"/>
+      <c r="GN33" s="28"/>
+      <c r="GO33" s="28"/>
+      <c r="GP33" s="28"/>
+      <c r="GQ33" s="28"/>
+      <c r="GR33" s="28"/>
+      <c r="GS33" s="28"/>
+      <c r="GT33" s="28"/>
+      <c r="GU33" s="28"/>
+      <c r="GV33" s="28"/>
+      <c r="GW33" s="28"/>
+      <c r="GX33" s="28"/>
+      <c r="GY33" s="28"/>
+      <c r="GZ33" s="28"/>
+      <c r="HA33" s="28"/>
+      <c r="HB33" s="28"/>
+      <c r="HC33" s="28"/>
+      <c r="HD33" s="28"/>
+      <c r="HE33" s="28"/>
+      <c r="HF33" s="28"/>
+      <c r="HG33" s="28"/>
+      <c r="HH33" s="28"/>
+      <c r="HI33" s="28"/>
+      <c r="HJ33" s="28"/>
+      <c r="HK33" s="28"/>
+      <c r="HL33" s="28"/>
+      <c r="HM33" s="28"/>
+      <c r="HN33" s="28"/>
+      <c r="HO33" s="28"/>
+      <c r="HP33" s="28"/>
+      <c r="HQ33" s="28"/>
+      <c r="HR33" s="28"/>
+      <c r="HS33" s="28"/>
+      <c r="HT33" s="28"/>
+      <c r="HU33" s="28"/>
+      <c r="HV33" s="28"/>
+      <c r="HW33" s="28"/>
+      <c r="HX33" s="28"/>
+      <c r="HY33" s="28"/>
+      <c r="HZ33" s="28"/>
+      <c r="IA33" s="28"/>
+      <c r="IB33" s="28"/>
+      <c r="IC33" s="28"/>
+      <c r="ID33" s="28"/>
+      <c r="IE33" s="28"/>
+      <c r="IF33" s="28"/>
+      <c r="IG33" s="28"/>
+      <c r="IH33" s="28"/>
+      <c r="II33" s="28"/>
+      <c r="IJ33" s="28"/>
+      <c r="IK33" s="28"/>
+      <c r="IL33" s="28"/>
+      <c r="IM33" s="28"/>
+      <c r="IN33" s="28"/>
+      <c r="IO33" s="28"/>
+      <c r="IP33" s="28"/>
+      <c r="IQ33" s="28"/>
+      <c r="IR33" s="28"/>
+      <c r="IS33" s="28"/>
+      <c r="IT33" s="28"/>
+      <c r="IU33" s="28"/>
+      <c r="IV33" s="28"/>
+      <c r="IW33" s="28"/>
+      <c r="IX33" s="28"/>
+      <c r="IY33" s="28"/>
+      <c r="IZ33" s="28"/>
+      <c r="JA33" s="28"/>
+      <c r="JB33" s="28"/>
+      <c r="JC33" s="28"/>
+      <c r="JD33" s="28"/>
+      <c r="JE33" s="28"/>
+      <c r="JF33" s="28"/>
+      <c r="JG33" s="28"/>
+      <c r="JH33" s="28"/>
+      <c r="JI33" s="28"/>
+      <c r="JJ33" s="28"/>
+      <c r="JK33" s="28"/>
+      <c r="JL33" s="28"/>
+      <c r="JM33" s="28"/>
+      <c r="JN33" s="28"/>
+      <c r="JO33" s="28"/>
+      <c r="JP33" s="28"/>
+      <c r="JQ33" s="28"/>
+      <c r="JR33" s="28"/>
+      <c r="JS33" s="28"/>
+      <c r="JT33" s="28"/>
+      <c r="JU33" s="28"/>
+      <c r="JV33" s="28"/>
+      <c r="JW33" s="28"/>
+      <c r="JX33" s="28"/>
+      <c r="JY33" s="28"/>
+      <c r="JZ33" s="28"/>
+      <c r="KA33" s="28"/>
+    </row>
+    <row r="34" spans="1:287" s="41" customFormat="1" ht="56.4" customHeight="1">
+      <c r="A34" s="55" t="s">
+        <v>62</v>
+      </c>
+      <c r="B34" s="40" t="s">
+        <v>59</v>
+      </c>
+      <c r="C34" s="40" t="s">
+        <v>8</v>
+      </c>
+      <c r="D34" s="56">
+        <v>43885</v>
+      </c>
+      <c r="E34" s="56">
+        <v>43886</v>
+      </c>
+      <c r="F34" s="40"/>
+      <c r="G34" s="40"/>
+      <c r="H34" s="40"/>
+      <c r="I34" s="55" t="s">
         <v>57</v>
       </c>
-      <c r="B33" s="30" t="s">
-        <v>60</v>
-      </c>
-      <c r="C33" s="30" t="s">
-        <v>8</v>
-      </c>
-      <c r="D33" s="35">
-        <v>43885</v>
-      </c>
-      <c r="E33" s="35">
+      <c r="J34" s="54" t="s">
+        <v>63</v>
+      </c>
+      <c r="K34" s="40"/>
+      <c r="L34" s="40"/>
+      <c r="M34" s="40"/>
+      <c r="N34" s="40"/>
+      <c r="O34" s="40"/>
+      <c r="P34" s="40"/>
+      <c r="Q34" s="40"/>
+      <c r="R34" s="40"/>
+      <c r="S34" s="40"/>
+      <c r="T34" s="40"/>
+      <c r="U34" s="40"/>
+      <c r="V34" s="40"/>
+      <c r="W34" s="40"/>
+      <c r="X34" s="40"/>
+      <c r="Y34" s="40"/>
+      <c r="Z34" s="40"/>
+      <c r="AA34" s="40"/>
+      <c r="AB34" s="40"/>
+      <c r="AC34" s="40"/>
+      <c r="AD34" s="40"/>
+      <c r="AE34" s="40"/>
+      <c r="AF34" s="40"/>
+      <c r="AG34" s="40"/>
+      <c r="AH34" s="40"/>
+      <c r="AI34" s="40"/>
+      <c r="AJ34" s="40"/>
+      <c r="AK34" s="40"/>
+      <c r="AL34" s="40"/>
+      <c r="AM34" s="40"/>
+      <c r="AN34" s="40"/>
+      <c r="AO34" s="40"/>
+      <c r="AP34" s="40"/>
+      <c r="AQ34" s="40"/>
+      <c r="AR34" s="40"/>
+      <c r="AS34" s="40"/>
+      <c r="AT34" s="40"/>
+      <c r="AU34" s="40"/>
+      <c r="AV34" s="40"/>
+      <c r="AW34" s="40"/>
+      <c r="AX34" s="40"/>
+      <c r="AY34" s="40"/>
+      <c r="AZ34" s="40"/>
+      <c r="BA34" s="40"/>
+      <c r="BB34" s="40"/>
+      <c r="BC34" s="40"/>
+      <c r="BD34" s="40"/>
+      <c r="BE34" s="40"/>
+      <c r="BF34" s="40"/>
+      <c r="BG34" s="40"/>
+      <c r="BH34" s="40"/>
+      <c r="BI34" s="40"/>
+      <c r="BJ34" s="40"/>
+      <c r="BK34" s="40"/>
+      <c r="BL34" s="40"/>
+      <c r="BM34" s="40"/>
+      <c r="BN34" s="40"/>
+      <c r="BO34" s="40"/>
+      <c r="BP34" s="40"/>
+      <c r="BQ34" s="40"/>
+      <c r="BR34" s="40"/>
+      <c r="BS34" s="40"/>
+      <c r="BT34" s="40"/>
+      <c r="BU34" s="40"/>
+      <c r="BV34" s="40"/>
+      <c r="BW34" s="40"/>
+      <c r="BX34" s="40"/>
+      <c r="BY34" s="40"/>
+      <c r="BZ34" s="40"/>
+      <c r="CA34" s="40"/>
+      <c r="CB34" s="40"/>
+      <c r="CC34" s="40"/>
+      <c r="CD34" s="40"/>
+      <c r="CE34" s="40"/>
+      <c r="CF34" s="40"/>
+      <c r="CG34" s="40"/>
+      <c r="CH34" s="40"/>
+      <c r="CI34" s="40"/>
+      <c r="CJ34" s="40"/>
+      <c r="CK34" s="40"/>
+      <c r="CL34" s="40"/>
+      <c r="CM34" s="40"/>
+      <c r="CN34" s="40"/>
+      <c r="CO34" s="40"/>
+      <c r="CP34" s="40"/>
+      <c r="CQ34" s="40"/>
+      <c r="CR34" s="40"/>
+      <c r="CS34" s="40"/>
+      <c r="CT34" s="40"/>
+      <c r="CU34" s="40"/>
+      <c r="CV34" s="40"/>
+      <c r="CW34" s="40"/>
+      <c r="CX34" s="40"/>
+      <c r="CY34" s="40"/>
+      <c r="CZ34" s="40"/>
+      <c r="DA34" s="40"/>
+      <c r="DB34" s="40"/>
+      <c r="DC34" s="40"/>
+      <c r="DD34" s="40"/>
+      <c r="DE34" s="40"/>
+      <c r="DF34" s="40"/>
+      <c r="DG34" s="40"/>
+      <c r="DH34" s="40"/>
+      <c r="DI34" s="40"/>
+      <c r="DJ34" s="40"/>
+      <c r="DK34" s="40"/>
+      <c r="DL34" s="40"/>
+      <c r="DM34" s="40"/>
+      <c r="DN34" s="40"/>
+      <c r="DO34" s="40"/>
+      <c r="DP34" s="40"/>
+      <c r="DQ34" s="40"/>
+      <c r="DR34" s="40"/>
+      <c r="DS34" s="40"/>
+      <c r="DT34" s="40"/>
+      <c r="DU34" s="40"/>
+      <c r="DV34" s="40"/>
+      <c r="DW34" s="40"/>
+      <c r="DX34" s="40"/>
+      <c r="DY34" s="40"/>
+      <c r="DZ34" s="40"/>
+      <c r="EA34" s="40"/>
+      <c r="EB34" s="40"/>
+      <c r="EC34" s="40"/>
+      <c r="ED34" s="40"/>
+      <c r="EE34" s="40"/>
+      <c r="EF34" s="40"/>
+      <c r="EG34" s="40"/>
+      <c r="EH34" s="40"/>
+      <c r="EI34" s="40"/>
+      <c r="EJ34" s="40"/>
+      <c r="EK34" s="40"/>
+      <c r="EL34" s="40"/>
+      <c r="EM34" s="40"/>
+      <c r="EN34" s="40"/>
+      <c r="EO34" s="40"/>
+      <c r="EP34" s="40"/>
+      <c r="EQ34" s="40"/>
+      <c r="ER34" s="40"/>
+      <c r="ES34" s="40"/>
+      <c r="ET34" s="40"/>
+      <c r="EU34" s="40"/>
+      <c r="EV34" s="40"/>
+      <c r="EW34" s="40"/>
+      <c r="EX34" s="40"/>
+      <c r="EY34" s="40"/>
+      <c r="EZ34" s="40"/>
+      <c r="FA34" s="40"/>
+      <c r="FB34" s="40"/>
+      <c r="FC34" s="40"/>
+      <c r="FD34" s="40"/>
+      <c r="FE34" s="40"/>
+      <c r="FF34" s="40"/>
+      <c r="FG34" s="40"/>
+      <c r="FH34" s="40"/>
+      <c r="FI34" s="40"/>
+      <c r="FJ34" s="40"/>
+      <c r="FK34" s="40"/>
+      <c r="FL34" s="40"/>
+      <c r="FM34" s="40"/>
+      <c r="FN34" s="40"/>
+      <c r="FO34" s="40"/>
+      <c r="FP34" s="40"/>
+      <c r="FQ34" s="40"/>
+      <c r="FR34" s="40"/>
+      <c r="FS34" s="40"/>
+      <c r="FT34" s="40"/>
+      <c r="FU34" s="40"/>
+      <c r="FV34" s="40"/>
+      <c r="FW34" s="40"/>
+      <c r="FX34" s="40"/>
+      <c r="FY34" s="40"/>
+      <c r="FZ34" s="40"/>
+      <c r="GA34" s="40"/>
+      <c r="GB34" s="40"/>
+      <c r="GC34" s="40"/>
+      <c r="GD34" s="40"/>
+      <c r="GE34" s="40"/>
+      <c r="GF34" s="40"/>
+      <c r="GG34" s="40"/>
+      <c r="GH34" s="40"/>
+      <c r="GI34" s="40"/>
+      <c r="GJ34" s="40"/>
+      <c r="GK34" s="40"/>
+      <c r="GL34" s="40"/>
+      <c r="GM34" s="40"/>
+      <c r="GN34" s="40"/>
+      <c r="GO34" s="40"/>
+      <c r="GP34" s="40"/>
+      <c r="GQ34" s="40"/>
+      <c r="GR34" s="40"/>
+      <c r="GS34" s="40"/>
+      <c r="GT34" s="40"/>
+      <c r="GU34" s="40"/>
+      <c r="GV34" s="40"/>
+      <c r="GW34" s="40"/>
+      <c r="GX34" s="40"/>
+      <c r="GY34" s="40"/>
+      <c r="GZ34" s="40"/>
+      <c r="HA34" s="40"/>
+      <c r="HB34" s="40"/>
+      <c r="HC34" s="40"/>
+      <c r="HD34" s="40"/>
+      <c r="HE34" s="40"/>
+      <c r="HF34" s="40"/>
+      <c r="HG34" s="40"/>
+      <c r="HH34" s="40"/>
+      <c r="HI34" s="40"/>
+      <c r="HJ34" s="40"/>
+      <c r="HK34" s="40"/>
+      <c r="HL34" s="40"/>
+      <c r="HM34" s="40"/>
+      <c r="HN34" s="40"/>
+      <c r="HO34" s="40"/>
+      <c r="HP34" s="40"/>
+      <c r="HQ34" s="40"/>
+      <c r="HR34" s="40"/>
+      <c r="HS34" s="40"/>
+      <c r="HT34" s="40"/>
+      <c r="HU34" s="40"/>
+      <c r="HV34" s="40"/>
+      <c r="HW34" s="40"/>
+      <c r="HX34" s="40"/>
+      <c r="HY34" s="40"/>
+      <c r="HZ34" s="40"/>
+      <c r="IA34" s="40"/>
+      <c r="IB34" s="40"/>
+      <c r="IC34" s="40"/>
+      <c r="ID34" s="40"/>
+      <c r="IE34" s="40"/>
+      <c r="IF34" s="40"/>
+      <c r="IG34" s="40"/>
+      <c r="IH34" s="40"/>
+      <c r="II34" s="40"/>
+      <c r="IJ34" s="40"/>
+      <c r="IK34" s="40"/>
+      <c r="IL34" s="40"/>
+      <c r="IM34" s="40"/>
+      <c r="IN34" s="40"/>
+      <c r="IO34" s="40"/>
+      <c r="IP34" s="40"/>
+      <c r="IQ34" s="40"/>
+      <c r="IR34" s="40"/>
+      <c r="IS34" s="40"/>
+      <c r="IT34" s="40"/>
+      <c r="IU34" s="40"/>
+      <c r="IV34" s="40"/>
+      <c r="IW34" s="40"/>
+      <c r="IX34" s="40"/>
+      <c r="IY34" s="40"/>
+      <c r="IZ34" s="40"/>
+      <c r="JA34" s="40"/>
+      <c r="JB34" s="40"/>
+      <c r="JC34" s="40"/>
+      <c r="JD34" s="40"/>
+      <c r="JE34" s="40"/>
+      <c r="JF34" s="40"/>
+      <c r="JG34" s="40"/>
+      <c r="JH34" s="40"/>
+      <c r="JI34" s="40"/>
+      <c r="JJ34" s="40"/>
+      <c r="JK34" s="40"/>
+      <c r="JL34" s="40"/>
+      <c r="JM34" s="40"/>
+      <c r="JN34" s="40"/>
+      <c r="JO34" s="40"/>
+      <c r="JP34" s="40"/>
+      <c r="JQ34" s="40"/>
+      <c r="JR34" s="40"/>
+      <c r="JS34" s="40"/>
+      <c r="JT34" s="40"/>
+      <c r="JU34" s="40"/>
+      <c r="JV34" s="40"/>
+      <c r="JW34" s="40"/>
+      <c r="JX34" s="40"/>
+      <c r="JY34" s="40"/>
+      <c r="JZ34" s="40"/>
+      <c r="KA34" s="40"/>
+    </row>
+    <row r="35" spans="1:287" ht="30.75" customHeight="1">
+      <c r="A35" s="33" t="s">
+        <v>48</v>
+      </c>
+      <c r="B35" s="40" t="s">
+        <v>59</v>
+      </c>
+      <c r="C35" s="30" t="s">
+        <v>38</v>
+      </c>
+      <c r="D35" s="56">
+        <v>43886</v>
+      </c>
+      <c r="E35" s="56">
         <v>43887</v>
       </c>
-      <c r="F33" s="36"/>
-      <c r="G33" s="36"/>
-      <c r="H33" s="30"/>
-      <c r="I33" s="33" t="s">
-        <v>58</v>
-      </c>
-      <c r="J33" s="40"/>
-      <c r="K33" s="30"/>
-      <c r="L33" s="30"/>
-      <c r="M33" s="30"/>
-      <c r="N33" s="30"/>
-      <c r="O33" s="30"/>
-      <c r="P33" s="30"/>
-      <c r="Q33" s="30"/>
-      <c r="R33" s="30"/>
-      <c r="S33" s="30"/>
-      <c r="T33" s="30"/>
-      <c r="U33" s="30"/>
-      <c r="V33" s="30"/>
-      <c r="W33" s="30"/>
-      <c r="X33" s="30"/>
-      <c r="Y33" s="30"/>
-      <c r="Z33" s="30"/>
-      <c r="AA33" s="30"/>
-      <c r="AB33" s="30"/>
-      <c r="AC33" s="30"/>
-      <c r="AD33" s="30"/>
-      <c r="AE33" s="30"/>
-      <c r="AF33" s="30"/>
-      <c r="AG33" s="30"/>
-      <c r="AH33" s="30"/>
-      <c r="AI33" s="30"/>
-      <c r="AJ33" s="30"/>
-      <c r="AK33" s="30"/>
-      <c r="AL33" s="30"/>
-      <c r="AM33" s="30"/>
-      <c r="AN33" s="30"/>
-      <c r="AO33" s="30"/>
-      <c r="AP33" s="30"/>
-      <c r="AQ33" s="30"/>
-      <c r="AR33" s="30"/>
-      <c r="AS33" s="30"/>
-      <c r="AT33" s="30"/>
-      <c r="AU33" s="30"/>
-      <c r="AV33" s="30"/>
-      <c r="AW33" s="30"/>
-      <c r="AX33" s="30"/>
-      <c r="AY33" s="30"/>
-      <c r="AZ33" s="30"/>
-      <c r="BA33" s="30"/>
-      <c r="BB33" s="30"/>
-      <c r="BC33" s="30"/>
-      <c r="BD33" s="30"/>
-      <c r="BE33" s="30"/>
-      <c r="BF33" s="30"/>
-      <c r="BG33" s="30"/>
-      <c r="BH33" s="30"/>
-      <c r="BI33" s="30"/>
-      <c r="BJ33" s="30"/>
-      <c r="BK33" s="30"/>
-      <c r="BL33" s="30"/>
-      <c r="BM33" s="30"/>
-      <c r="BN33" s="30"/>
-      <c r="BO33" s="30"/>
-      <c r="BP33" s="30"/>
-      <c r="BQ33" s="30"/>
-      <c r="BR33" s="30"/>
-      <c r="BS33" s="30"/>
-      <c r="BT33" s="30"/>
-      <c r="BU33" s="30"/>
-      <c r="BV33" s="30"/>
-      <c r="BW33" s="30"/>
-      <c r="BX33" s="30"/>
-      <c r="BY33" s="30"/>
-      <c r="BZ33" s="30"/>
-      <c r="CA33" s="30"/>
-      <c r="CB33" s="30"/>
-      <c r="CC33" s="30"/>
-      <c r="CD33" s="30"/>
-      <c r="CE33" s="30"/>
-      <c r="CF33" s="30"/>
-      <c r="CG33" s="30"/>
-      <c r="CH33" s="30"/>
-      <c r="CI33" s="30"/>
-      <c r="CJ33" s="30"/>
-      <c r="CK33" s="30"/>
-      <c r="CL33" s="30"/>
-      <c r="CM33" s="30"/>
-      <c r="CN33" s="30"/>
-      <c r="CO33" s="30"/>
-      <c r="CP33" s="30"/>
-      <c r="CQ33" s="30"/>
-      <c r="CR33" s="30"/>
-      <c r="CS33" s="30"/>
-      <c r="CT33" s="30"/>
-      <c r="CU33" s="30"/>
-      <c r="CV33" s="30"/>
-      <c r="CW33" s="30"/>
-      <c r="CX33" s="30"/>
-      <c r="CY33" s="30"/>
-      <c r="CZ33" s="30"/>
-      <c r="DA33" s="30"/>
-      <c r="DB33" s="30"/>
-      <c r="DC33" s="30"/>
-      <c r="DD33" s="30"/>
-      <c r="DE33" s="30"/>
-      <c r="DF33" s="30"/>
-      <c r="DG33" s="30"/>
-      <c r="DH33" s="30"/>
-      <c r="DI33" s="30"/>
-      <c r="DJ33" s="30"/>
-      <c r="DK33" s="30"/>
-      <c r="DL33" s="30"/>
-      <c r="DM33" s="30"/>
-      <c r="DN33" s="30"/>
-      <c r="DO33" s="30"/>
-      <c r="DP33" s="30"/>
-      <c r="DQ33" s="30"/>
-      <c r="DR33" s="30"/>
-      <c r="DS33" s="30"/>
-      <c r="DT33" s="30"/>
-      <c r="DU33" s="30"/>
-      <c r="DV33" s="30"/>
-      <c r="DW33" s="30"/>
-      <c r="DX33" s="30"/>
-      <c r="DY33" s="30"/>
-      <c r="DZ33" s="30"/>
-      <c r="EA33" s="30"/>
-      <c r="EB33" s="30"/>
-      <c r="EC33" s="30"/>
-      <c r="ED33" s="30"/>
-      <c r="EE33" s="30"/>
-      <c r="EF33" s="30"/>
-      <c r="EG33" s="30"/>
-      <c r="EH33" s="30"/>
-      <c r="EI33" s="30"/>
-      <c r="EJ33" s="30"/>
-      <c r="EK33" s="30"/>
-      <c r="EL33" s="30"/>
-      <c r="EM33" s="30"/>
-      <c r="EN33" s="30"/>
-      <c r="EO33" s="30"/>
-      <c r="EP33" s="30"/>
-      <c r="EQ33" s="30"/>
-      <c r="ER33" s="30"/>
-      <c r="ES33" s="30"/>
-      <c r="ET33" s="30"/>
-      <c r="EU33" s="30"/>
-      <c r="EV33" s="30"/>
-      <c r="EW33" s="30"/>
-      <c r="EX33" s="30"/>
-      <c r="EY33" s="30"/>
-      <c r="EZ33" s="30"/>
-      <c r="FA33" s="30"/>
-      <c r="FB33" s="30"/>
-      <c r="FC33" s="30"/>
-      <c r="FD33" s="30"/>
-      <c r="FE33" s="30"/>
-      <c r="FF33" s="30"/>
-      <c r="FG33" s="30"/>
-      <c r="FH33" s="30"/>
-      <c r="FI33" s="30"/>
-      <c r="FJ33" s="30"/>
-      <c r="FK33" s="30"/>
-      <c r="FL33" s="30"/>
-      <c r="FM33" s="30"/>
-      <c r="FN33" s="30"/>
-      <c r="FO33" s="30"/>
-      <c r="FP33" s="30"/>
-      <c r="FQ33" s="30"/>
-      <c r="FR33" s="30"/>
-      <c r="FS33" s="30"/>
-      <c r="FT33" s="30"/>
-      <c r="FU33" s="30"/>
-      <c r="FV33" s="30"/>
-      <c r="FW33" s="30"/>
-      <c r="FX33" s="30"/>
-      <c r="FY33" s="30"/>
-      <c r="FZ33" s="30"/>
-      <c r="GA33" s="30"/>
-      <c r="GB33" s="30"/>
-      <c r="GC33" s="30"/>
-      <c r="GD33" s="30"/>
-      <c r="GE33" s="30"/>
-      <c r="GF33" s="30"/>
-      <c r="GG33" s="30"/>
-      <c r="GH33" s="30"/>
-      <c r="GI33" s="30"/>
-      <c r="GJ33" s="30"/>
-      <c r="GK33" s="30"/>
-      <c r="GL33" s="30"/>
-      <c r="GM33" s="30"/>
-      <c r="GN33" s="30"/>
-      <c r="GO33" s="30"/>
-      <c r="GP33" s="30"/>
-      <c r="GQ33" s="30"/>
-      <c r="GR33" s="30"/>
-      <c r="GS33" s="30"/>
-      <c r="GT33" s="30"/>
-      <c r="GU33" s="30"/>
-      <c r="GV33" s="30"/>
-      <c r="GW33" s="30"/>
-      <c r="GX33" s="30"/>
-      <c r="GY33" s="30"/>
-      <c r="GZ33" s="30"/>
-      <c r="HA33" s="30"/>
-      <c r="HB33" s="30"/>
-      <c r="HC33" s="30"/>
-      <c r="HD33" s="30"/>
-      <c r="HE33" s="30"/>
-      <c r="HF33" s="30"/>
-      <c r="HG33" s="30"/>
-      <c r="HH33" s="30"/>
-      <c r="HI33" s="30"/>
-      <c r="HJ33" s="30"/>
-      <c r="HK33" s="30"/>
-      <c r="HL33" s="30"/>
-      <c r="HM33" s="30"/>
-      <c r="HN33" s="30"/>
-      <c r="HO33" s="30"/>
-      <c r="HP33" s="30"/>
-      <c r="HQ33" s="30"/>
-      <c r="HR33" s="30"/>
-      <c r="HS33" s="30"/>
-      <c r="HT33" s="30"/>
-      <c r="HU33" s="30"/>
-      <c r="HV33" s="30"/>
-      <c r="HW33" s="30"/>
-      <c r="HX33" s="30"/>
-      <c r="HY33" s="30"/>
-      <c r="HZ33" s="30"/>
-      <c r="IA33" s="30"/>
-      <c r="IB33" s="30"/>
-      <c r="IC33" s="30"/>
-      <c r="ID33" s="30"/>
-      <c r="IE33" s="30"/>
-      <c r="IF33" s="30"/>
-      <c r="IG33" s="30"/>
-      <c r="IH33" s="30"/>
-      <c r="II33" s="30"/>
-      <c r="IJ33" s="30"/>
-      <c r="IK33" s="30"/>
-      <c r="IL33" s="30"/>
-      <c r="IM33" s="30"/>
-      <c r="IN33" s="30"/>
-      <c r="IO33" s="30"/>
-      <c r="IP33" s="30"/>
-      <c r="IQ33" s="30"/>
-      <c r="IR33" s="30"/>
-      <c r="IS33" s="30"/>
-      <c r="IT33" s="30"/>
-      <c r="IU33" s="30"/>
-      <c r="IV33" s="30"/>
-      <c r="IW33" s="30"/>
-      <c r="IX33" s="30"/>
-      <c r="IY33" s="30"/>
-      <c r="IZ33" s="30"/>
-      <c r="JA33" s="30"/>
-      <c r="JB33" s="30"/>
-      <c r="JC33" s="30"/>
-      <c r="JD33" s="30"/>
-      <c r="JE33" s="30"/>
-      <c r="JF33" s="30"/>
-      <c r="JG33" s="30"/>
-      <c r="JH33" s="30"/>
-      <c r="JI33" s="30"/>
-      <c r="JJ33" s="30"/>
-      <c r="JK33" s="30"/>
-      <c r="JL33" s="30"/>
-      <c r="JM33" s="30"/>
-      <c r="JN33" s="30"/>
-      <c r="JO33" s="30"/>
-      <c r="JP33" s="30"/>
-      <c r="JQ33" s="30"/>
-      <c r="JR33" s="30"/>
-      <c r="JS33" s="30"/>
-      <c r="JT33" s="30"/>
-      <c r="JU33" s="30"/>
-      <c r="JV33" s="30"/>
-      <c r="JW33" s="30"/>
-      <c r="JX33" s="30"/>
-      <c r="JY33" s="30"/>
-      <c r="JZ33" s="30"/>
-      <c r="KA33" s="30"/>
-    </row>
-    <row r="34" spans="1:287" ht="30.75" customHeight="1">
-      <c r="A34" s="33"/>
-      <c r="B34" s="28"/>
-      <c r="C34" s="30"/>
-      <c r="D34" s="28"/>
-      <c r="E34" s="28"/>
-      <c r="F34" s="28"/>
-      <c r="G34" s="28"/>
-      <c r="H34" s="28"/>
-      <c r="I34" s="29"/>
-      <c r="J34" s="40"/>
-      <c r="K34" s="28"/>
-      <c r="L34" s="28"/>
-      <c r="M34" s="28"/>
-      <c r="N34" s="28"/>
-      <c r="O34" s="28"/>
-      <c r="P34" s="28"/>
-      <c r="Q34" s="28"/>
-      <c r="R34" s="28"/>
-      <c r="S34" s="28"/>
-      <c r="T34" s="28"/>
-      <c r="U34" s="28"/>
-      <c r="V34" s="28"/>
-      <c r="W34" s="28"/>
-      <c r="X34" s="28"/>
-      <c r="Y34" s="28"/>
-      <c r="Z34" s="28"/>
-      <c r="AA34" s="28"/>
-      <c r="AB34" s="28"/>
-      <c r="AC34" s="28"/>
-      <c r="AD34" s="28"/>
-      <c r="AE34" s="28"/>
-      <c r="AF34" s="28"/>
-      <c r="AG34" s="28"/>
-      <c r="AH34" s="28"/>
-      <c r="AI34" s="28"/>
-      <c r="AJ34" s="28"/>
-      <c r="AK34" s="28"/>
-      <c r="AL34" s="28"/>
-      <c r="AM34" s="28"/>
-      <c r="AN34" s="28"/>
-      <c r="AO34" s="28"/>
-      <c r="AP34" s="28"/>
-      <c r="AQ34" s="28"/>
-      <c r="AR34" s="28"/>
-      <c r="AS34" s="28"/>
-      <c r="AT34" s="28"/>
-      <c r="AU34" s="28"/>
-      <c r="AV34" s="28"/>
-      <c r="AW34" s="28"/>
-      <c r="AX34" s="28"/>
-      <c r="AY34" s="28"/>
-      <c r="AZ34" s="28"/>
-      <c r="BA34" s="28"/>
-      <c r="BB34" s="28"/>
-      <c r="BC34" s="28"/>
-      <c r="BD34" s="28"/>
-      <c r="BE34" s="28"/>
-      <c r="BF34" s="28"/>
-      <c r="BG34" s="28"/>
-      <c r="BH34" s="28"/>
-      <c r="BI34" s="28"/>
-      <c r="BJ34" s="28"/>
-      <c r="BK34" s="28"/>
-      <c r="BL34" s="28"/>
-      <c r="BM34" s="28"/>
-      <c r="BN34" s="28"/>
-      <c r="BO34" s="28"/>
-      <c r="BP34" s="28"/>
-      <c r="BQ34" s="28"/>
-      <c r="BR34" s="28"/>
-      <c r="BS34" s="28"/>
-      <c r="BT34" s="28"/>
-      <c r="BU34" s="28"/>
-      <c r="BV34" s="28"/>
-      <c r="BW34" s="28"/>
-      <c r="BX34" s="28"/>
-      <c r="BY34" s="28"/>
-      <c r="BZ34" s="28"/>
-      <c r="CA34" s="28"/>
-      <c r="CB34" s="28"/>
-      <c r="CC34" s="28"/>
-      <c r="CD34" s="28"/>
-      <c r="CE34" s="28"/>
-      <c r="CF34" s="28"/>
-      <c r="CG34" s="28"/>
-      <c r="CH34" s="28"/>
-      <c r="CI34" s="28"/>
-      <c r="CJ34" s="28"/>
-      <c r="CK34" s="28"/>
-      <c r="CL34" s="28"/>
-      <c r="CM34" s="28"/>
-      <c r="CN34" s="28"/>
-      <c r="CO34" s="28"/>
-      <c r="CP34" s="28"/>
-      <c r="CQ34" s="28"/>
-      <c r="CR34" s="28"/>
-      <c r="CS34" s="28"/>
-      <c r="CT34" s="28"/>
-      <c r="CU34" s="28"/>
-      <c r="CV34" s="28"/>
-      <c r="CW34" s="28"/>
-      <c r="CX34" s="28"/>
-      <c r="CY34" s="28"/>
-      <c r="CZ34" s="28"/>
-      <c r="DA34" s="28"/>
-      <c r="DB34" s="28"/>
-      <c r="DC34" s="28"/>
-      <c r="DD34" s="28"/>
-      <c r="DE34" s="28"/>
-      <c r="DF34" s="28"/>
-      <c r="DG34" s="28"/>
-      <c r="DH34" s="28"/>
-      <c r="DI34" s="28"/>
-      <c r="DJ34" s="28"/>
-      <c r="DK34" s="28"/>
-      <c r="DL34" s="28"/>
-      <c r="DM34" s="28"/>
-      <c r="DN34" s="28"/>
-      <c r="DO34" s="28"/>
-      <c r="DP34" s="28"/>
-      <c r="DQ34" s="28"/>
-      <c r="DR34" s="28"/>
-      <c r="DS34" s="28"/>
-      <c r="DT34" s="28"/>
-      <c r="DU34" s="28"/>
-      <c r="DV34" s="28"/>
-      <c r="DW34" s="28"/>
-      <c r="DX34" s="28"/>
-      <c r="DY34" s="28"/>
-      <c r="DZ34" s="28"/>
-      <c r="EA34" s="28"/>
-      <c r="EB34" s="28"/>
-      <c r="EC34" s="28"/>
-      <c r="ED34" s="28"/>
-      <c r="EE34" s="28"/>
-      <c r="EF34" s="28"/>
-      <c r="EG34" s="28"/>
-      <c r="EH34" s="28"/>
-      <c r="EI34" s="28"/>
-      <c r="EJ34" s="28"/>
-      <c r="EK34" s="28"/>
-      <c r="EL34" s="28"/>
-      <c r="EM34" s="28"/>
-      <c r="EN34" s="28"/>
-      <c r="EO34" s="28"/>
-      <c r="EP34" s="28"/>
-      <c r="EQ34" s="28"/>
-      <c r="ER34" s="28"/>
-      <c r="ES34" s="28"/>
-      <c r="ET34" s="28"/>
-      <c r="EU34" s="28"/>
-      <c r="EV34" s="28"/>
-      <c r="EW34" s="28"/>
-      <c r="EX34" s="28"/>
-      <c r="EY34" s="28"/>
-      <c r="EZ34" s="28"/>
-      <c r="FA34" s="28"/>
-      <c r="FB34" s="28"/>
-      <c r="FC34" s="28"/>
-      <c r="FD34" s="28"/>
-      <c r="FE34" s="28"/>
-      <c r="FF34" s="28"/>
-      <c r="FG34" s="28"/>
-      <c r="FH34" s="28"/>
-      <c r="FI34" s="28"/>
-      <c r="FJ34" s="28"/>
-      <c r="FK34" s="28"/>
-      <c r="FL34" s="28"/>
-      <c r="FM34" s="28"/>
-      <c r="FN34" s="28"/>
-      <c r="FO34" s="28"/>
-      <c r="FP34" s="28"/>
-      <c r="FQ34" s="28"/>
-      <c r="FR34" s="28"/>
-      <c r="FS34" s="28"/>
-      <c r="FT34" s="28"/>
-      <c r="FU34" s="28"/>
-      <c r="FV34" s="28"/>
-      <c r="FW34" s="28"/>
-      <c r="FX34" s="28"/>
-      <c r="FY34" s="28"/>
-      <c r="FZ34" s="28"/>
-      <c r="GA34" s="28"/>
-      <c r="GB34" s="28"/>
-      <c r="GC34" s="28"/>
-      <c r="GD34" s="28"/>
-      <c r="GE34" s="28"/>
-      <c r="GF34" s="28"/>
-      <c r="GG34" s="28"/>
-      <c r="GH34" s="28"/>
-      <c r="GI34" s="28"/>
-      <c r="GJ34" s="28"/>
-      <c r="GK34" s="28"/>
-      <c r="GL34" s="28"/>
-      <c r="GM34" s="28"/>
-      <c r="GN34" s="28"/>
-      <c r="GO34" s="28"/>
-      <c r="GP34" s="28"/>
-      <c r="GQ34" s="28"/>
-      <c r="GR34" s="28"/>
-      <c r="GS34" s="28"/>
-      <c r="GT34" s="28"/>
-      <c r="GU34" s="28"/>
-      <c r="GV34" s="28"/>
-      <c r="GW34" s="28"/>
-      <c r="GX34" s="28"/>
-      <c r="GY34" s="28"/>
-      <c r="GZ34" s="28"/>
-      <c r="HA34" s="28"/>
-      <c r="HB34" s="28"/>
-      <c r="HC34" s="28"/>
-      <c r="HD34" s="28"/>
-      <c r="HE34" s="28"/>
-      <c r="HF34" s="28"/>
-      <c r="HG34" s="28"/>
-      <c r="HH34" s="28"/>
-      <c r="HI34" s="28"/>
-      <c r="HJ34" s="28"/>
-      <c r="HK34" s="28"/>
-      <c r="HL34" s="28"/>
-      <c r="HM34" s="28"/>
-      <c r="HN34" s="28"/>
-      <c r="HO34" s="28"/>
-      <c r="HP34" s="28"/>
-      <c r="HQ34" s="28"/>
-      <c r="HR34" s="28"/>
-      <c r="HS34" s="28"/>
-      <c r="HT34" s="28"/>
-      <c r="HU34" s="28"/>
-      <c r="HV34" s="28"/>
-      <c r="HW34" s="28"/>
-      <c r="HX34" s="28"/>
-      <c r="HY34" s="28"/>
-      <c r="HZ34" s="28"/>
-      <c r="IA34" s="28"/>
-      <c r="IB34" s="28"/>
-      <c r="IC34" s="28"/>
-      <c r="ID34" s="28"/>
-      <c r="IE34" s="28"/>
-      <c r="IF34" s="28"/>
-      <c r="IG34" s="28"/>
-      <c r="IH34" s="28"/>
-      <c r="II34" s="28"/>
-      <c r="IJ34" s="28"/>
-      <c r="IK34" s="28"/>
-      <c r="IL34" s="28"/>
-      <c r="IM34" s="28"/>
-      <c r="IN34" s="28"/>
-      <c r="IO34" s="28"/>
-      <c r="IP34" s="28"/>
-      <c r="IQ34" s="28"/>
-      <c r="IR34" s="28"/>
-      <c r="IS34" s="28"/>
-      <c r="IT34" s="28"/>
-      <c r="IU34" s="28"/>
-      <c r="IV34" s="28"/>
-      <c r="IW34" s="28"/>
-      <c r="IX34" s="28"/>
-      <c r="IY34" s="28"/>
-      <c r="IZ34" s="28"/>
-      <c r="JA34" s="28"/>
-      <c r="JB34" s="28"/>
-      <c r="JC34" s="28"/>
-      <c r="JD34" s="28"/>
-      <c r="JE34" s="28"/>
-      <c r="JF34" s="28"/>
-      <c r="JG34" s="28"/>
-      <c r="JH34" s="28"/>
-      <c r="JI34" s="28"/>
-      <c r="JJ34" s="28"/>
-      <c r="JK34" s="28"/>
-      <c r="JL34" s="28"/>
-      <c r="JM34" s="28"/>
-      <c r="JN34" s="28"/>
-      <c r="JO34" s="28"/>
-      <c r="JP34" s="28"/>
-      <c r="JQ34" s="28"/>
-      <c r="JR34" s="28"/>
-      <c r="JS34" s="28"/>
-      <c r="JT34" s="28"/>
-      <c r="JU34" s="28"/>
-      <c r="JV34" s="28"/>
-      <c r="JW34" s="28"/>
-      <c r="JX34" s="28"/>
-      <c r="JY34" s="28"/>
-      <c r="JZ34" s="28"/>
-      <c r="KA34" s="28"/>
-    </row>
-    <row r="35" spans="1:287" ht="30.75" customHeight="1">
-      <c r="A35" s="33"/>
-      <c r="B35" s="28"/>
-      <c r="C35" s="30"/>
-      <c r="D35" s="28"/>
-      <c r="E35" s="28"/>
       <c r="F35" s="28"/>
       <c r="G35" s="28"/>
       <c r="H35" s="28"/>
-      <c r="I35" s="29"/>
+      <c r="I35" s="55" t="s">
+        <v>57</v>
+      </c>
       <c r="J35" s="40"/>
       <c r="K35" s="28"/>
       <c r="L35" s="28"/>
@@ -11186,15 +11267,27 @@
       <c r="KA35" s="28"/>
     </row>
     <row r="36" spans="1:287" ht="30.75" customHeight="1">
-      <c r="A36" s="33"/>
-      <c r="B36" s="28"/>
-      <c r="C36" s="30"/>
-      <c r="D36" s="28"/>
-      <c r="E36" s="28"/>
+      <c r="A36" s="33" t="s">
+        <v>53</v>
+      </c>
+      <c r="B36" s="40" t="s">
+        <v>59</v>
+      </c>
+      <c r="C36" s="30" t="s">
+        <v>30</v>
+      </c>
+      <c r="D36" s="56">
+        <v>43887</v>
+      </c>
+      <c r="E36" s="56">
+        <v>43888</v>
+      </c>
       <c r="F36" s="28"/>
       <c r="G36" s="28"/>
       <c r="H36" s="28"/>
-      <c r="I36" s="29"/>
+      <c r="I36" s="55" t="s">
+        <v>57</v>
+      </c>
       <c r="J36" s="40"/>
       <c r="K36" s="28"/>
       <c r="L36" s="28"/>
@@ -11475,15 +11568,27 @@
       <c r="KA36" s="28"/>
     </row>
     <row r="37" spans="1:287" ht="30.75" customHeight="1">
-      <c r="A37" s="33"/>
-      <c r="B37" s="28"/>
-      <c r="C37" s="30"/>
-      <c r="D37" s="28"/>
-      <c r="E37" s="28"/>
+      <c r="A37" s="33" t="s">
+        <v>64</v>
+      </c>
+      <c r="B37" s="40" t="s">
+        <v>59</v>
+      </c>
+      <c r="C37" s="30" t="s">
+        <v>34</v>
+      </c>
+      <c r="D37" s="56">
+        <v>43889</v>
+      </c>
+      <c r="E37" s="56">
+        <v>43889</v>
+      </c>
       <c r="F37" s="28"/>
       <c r="G37" s="28"/>
       <c r="H37" s="28"/>
-      <c r="I37" s="29"/>
+      <c r="I37" s="55" t="s">
+        <v>57</v>
+      </c>
       <c r="J37" s="40"/>
       <c r="K37" s="28"/>
       <c r="L37" s="28"/>
@@ -11764,15 +11869,27 @@
       <c r="KA37" s="28"/>
     </row>
     <row r="38" spans="1:287" ht="30.75" customHeight="1">
-      <c r="A38" s="33"/>
-      <c r="B38" s="28"/>
-      <c r="C38" s="30"/>
-      <c r="D38" s="28"/>
-      <c r="E38" s="28"/>
+      <c r="A38" s="33" t="s">
+        <v>56</v>
+      </c>
+      <c r="B38" s="40" t="s">
+        <v>59</v>
+      </c>
+      <c r="C38" s="30" t="s">
+        <v>8</v>
+      </c>
+      <c r="D38" s="56">
+        <v>43889</v>
+      </c>
+      <c r="E38" s="56">
+        <v>43889</v>
+      </c>
       <c r="F38" s="28"/>
       <c r="G38" s="28"/>
       <c r="H38" s="28"/>
-      <c r="I38" s="29"/>
+      <c r="I38" s="55" t="s">
+        <v>57</v>
+      </c>
       <c r="J38" s="40"/>
       <c r="K38" s="28"/>
       <c r="L38" s="28"/>
@@ -12061,7 +12178,7 @@
       <c r="F39" s="28"/>
       <c r="G39" s="28"/>
       <c r="H39" s="28"/>
-      <c r="I39" s="29"/>
+      <c r="I39" s="55"/>
       <c r="J39" s="40"/>
       <c r="K39" s="28"/>
       <c r="L39" s="28"/>
@@ -15809,583 +15926,11 @@
       <c r="JZ51" s="28"/>
       <c r="KA51" s="28"/>
     </row>
-    <row r="52" spans="1:287" ht="30.75" customHeight="1">
-      <c r="A52" s="33"/>
-      <c r="B52" s="28"/>
-      <c r="C52" s="30"/>
-      <c r="D52" s="28"/>
-      <c r="E52" s="28"/>
-      <c r="F52" s="28"/>
-      <c r="G52" s="28"/>
-      <c r="H52" s="28"/>
-      <c r="I52" s="29"/>
-      <c r="J52" s="40"/>
-      <c r="K52" s="28"/>
-      <c r="L52" s="28"/>
-      <c r="M52" s="28"/>
-      <c r="N52" s="28"/>
-      <c r="O52" s="28"/>
-      <c r="P52" s="28"/>
-      <c r="Q52" s="28"/>
-      <c r="R52" s="28"/>
-      <c r="S52" s="28"/>
-      <c r="T52" s="28"/>
-      <c r="U52" s="28"/>
-      <c r="V52" s="28"/>
-      <c r="W52" s="28"/>
-      <c r="X52" s="28"/>
-      <c r="Y52" s="28"/>
-      <c r="Z52" s="28"/>
-      <c r="AA52" s="28"/>
-      <c r="AB52" s="28"/>
-      <c r="AC52" s="28"/>
-      <c r="AD52" s="28"/>
-      <c r="AE52" s="28"/>
-      <c r="AF52" s="28"/>
-      <c r="AG52" s="28"/>
-      <c r="AH52" s="28"/>
-      <c r="AI52" s="28"/>
-      <c r="AJ52" s="28"/>
-      <c r="AK52" s="28"/>
-      <c r="AL52" s="28"/>
-      <c r="AM52" s="28"/>
-      <c r="AN52" s="28"/>
-      <c r="AO52" s="28"/>
-      <c r="AP52" s="28"/>
-      <c r="AQ52" s="28"/>
-      <c r="AR52" s="28"/>
-      <c r="AS52" s="28"/>
-      <c r="AT52" s="28"/>
-      <c r="AU52" s="28"/>
-      <c r="AV52" s="28"/>
-      <c r="AW52" s="28"/>
-      <c r="AX52" s="28"/>
-      <c r="AY52" s="28"/>
-      <c r="AZ52" s="28"/>
-      <c r="BA52" s="28"/>
-      <c r="BB52" s="28"/>
-      <c r="BC52" s="28"/>
-      <c r="BD52" s="28"/>
-      <c r="BE52" s="28"/>
-      <c r="BF52" s="28"/>
-      <c r="BG52" s="28"/>
-      <c r="BH52" s="28"/>
-      <c r="BI52" s="28"/>
-      <c r="BJ52" s="28"/>
-      <c r="BK52" s="28"/>
-      <c r="BL52" s="28"/>
-      <c r="BM52" s="28"/>
-      <c r="BN52" s="28"/>
-      <c r="BO52" s="28"/>
-      <c r="BP52" s="28"/>
-      <c r="BQ52" s="28"/>
-      <c r="BR52" s="28"/>
-      <c r="BS52" s="28"/>
-      <c r="BT52" s="28"/>
-      <c r="BU52" s="28"/>
-      <c r="BV52" s="28"/>
-      <c r="BW52" s="28"/>
-      <c r="BX52" s="28"/>
-      <c r="BY52" s="28"/>
-      <c r="BZ52" s="28"/>
-      <c r="CA52" s="28"/>
-      <c r="CB52" s="28"/>
-      <c r="CC52" s="28"/>
-      <c r="CD52" s="28"/>
-      <c r="CE52" s="28"/>
-      <c r="CF52" s="28"/>
-      <c r="CG52" s="28"/>
-      <c r="CH52" s="28"/>
-      <c r="CI52" s="28"/>
-      <c r="CJ52" s="28"/>
-      <c r="CK52" s="28"/>
-      <c r="CL52" s="28"/>
-      <c r="CM52" s="28"/>
-      <c r="CN52" s="28"/>
-      <c r="CO52" s="28"/>
-      <c r="CP52" s="28"/>
-      <c r="CQ52" s="28"/>
-      <c r="CR52" s="28"/>
-      <c r="CS52" s="28"/>
-      <c r="CT52" s="28"/>
-      <c r="CU52" s="28"/>
-      <c r="CV52" s="28"/>
-      <c r="CW52" s="28"/>
-      <c r="CX52" s="28"/>
-      <c r="CY52" s="28"/>
-      <c r="CZ52" s="28"/>
-      <c r="DA52" s="28"/>
-      <c r="DB52" s="28"/>
-      <c r="DC52" s="28"/>
-      <c r="DD52" s="28"/>
-      <c r="DE52" s="28"/>
-      <c r="DF52" s="28"/>
-      <c r="DG52" s="28"/>
-      <c r="DH52" s="28"/>
-      <c r="DI52" s="28"/>
-      <c r="DJ52" s="28"/>
-      <c r="DK52" s="28"/>
-      <c r="DL52" s="28"/>
-      <c r="DM52" s="28"/>
-      <c r="DN52" s="28"/>
-      <c r="DO52" s="28"/>
-      <c r="DP52" s="28"/>
-      <c r="DQ52" s="28"/>
-      <c r="DR52" s="28"/>
-      <c r="DS52" s="28"/>
-      <c r="DT52" s="28"/>
-      <c r="DU52" s="28"/>
-      <c r="DV52" s="28"/>
-      <c r="DW52" s="28"/>
-      <c r="DX52" s="28"/>
-      <c r="DY52" s="28"/>
-      <c r="DZ52" s="28"/>
-      <c r="EA52" s="28"/>
-      <c r="EB52" s="28"/>
-      <c r="EC52" s="28"/>
-      <c r="ED52" s="28"/>
-      <c r="EE52" s="28"/>
-      <c r="EF52" s="28"/>
-      <c r="EG52" s="28"/>
-      <c r="EH52" s="28"/>
-      <c r="EI52" s="28"/>
-      <c r="EJ52" s="28"/>
-      <c r="EK52" s="28"/>
-      <c r="EL52" s="28"/>
-      <c r="EM52" s="28"/>
-      <c r="EN52" s="28"/>
-      <c r="EO52" s="28"/>
-      <c r="EP52" s="28"/>
-      <c r="EQ52" s="28"/>
-      <c r="ER52" s="28"/>
-      <c r="ES52" s="28"/>
-      <c r="ET52" s="28"/>
-      <c r="EU52" s="28"/>
-      <c r="EV52" s="28"/>
-      <c r="EW52" s="28"/>
-      <c r="EX52" s="28"/>
-      <c r="EY52" s="28"/>
-      <c r="EZ52" s="28"/>
-      <c r="FA52" s="28"/>
-      <c r="FB52" s="28"/>
-      <c r="FC52" s="28"/>
-      <c r="FD52" s="28"/>
-      <c r="FE52" s="28"/>
-      <c r="FF52" s="28"/>
-      <c r="FG52" s="28"/>
-      <c r="FH52" s="28"/>
-      <c r="FI52" s="28"/>
-      <c r="FJ52" s="28"/>
-      <c r="FK52" s="28"/>
-      <c r="FL52" s="28"/>
-      <c r="FM52" s="28"/>
-      <c r="FN52" s="28"/>
-      <c r="FO52" s="28"/>
-      <c r="FP52" s="28"/>
-      <c r="FQ52" s="28"/>
-      <c r="FR52" s="28"/>
-      <c r="FS52" s="28"/>
-      <c r="FT52" s="28"/>
-      <c r="FU52" s="28"/>
-      <c r="FV52" s="28"/>
-      <c r="FW52" s="28"/>
-      <c r="FX52" s="28"/>
-      <c r="FY52" s="28"/>
-      <c r="FZ52" s="28"/>
-      <c r="GA52" s="28"/>
-      <c r="GB52" s="28"/>
-      <c r="GC52" s="28"/>
-      <c r="GD52" s="28"/>
-      <c r="GE52" s="28"/>
-      <c r="GF52" s="28"/>
-      <c r="GG52" s="28"/>
-      <c r="GH52" s="28"/>
-      <c r="GI52" s="28"/>
-      <c r="GJ52" s="28"/>
-      <c r="GK52" s="28"/>
-      <c r="GL52" s="28"/>
-      <c r="GM52" s="28"/>
-      <c r="GN52" s="28"/>
-      <c r="GO52" s="28"/>
-      <c r="GP52" s="28"/>
-      <c r="GQ52" s="28"/>
-      <c r="GR52" s="28"/>
-      <c r="GS52" s="28"/>
-      <c r="GT52" s="28"/>
-      <c r="GU52" s="28"/>
-      <c r="GV52" s="28"/>
-      <c r="GW52" s="28"/>
-      <c r="GX52" s="28"/>
-      <c r="GY52" s="28"/>
-      <c r="GZ52" s="28"/>
-      <c r="HA52" s="28"/>
-      <c r="HB52" s="28"/>
-      <c r="HC52" s="28"/>
-      <c r="HD52" s="28"/>
-      <c r="HE52" s="28"/>
-      <c r="HF52" s="28"/>
-      <c r="HG52" s="28"/>
-      <c r="HH52" s="28"/>
-      <c r="HI52" s="28"/>
-      <c r="HJ52" s="28"/>
-      <c r="HK52" s="28"/>
-      <c r="HL52" s="28"/>
-      <c r="HM52" s="28"/>
-      <c r="HN52" s="28"/>
-      <c r="HO52" s="28"/>
-      <c r="HP52" s="28"/>
-      <c r="HQ52" s="28"/>
-      <c r="HR52" s="28"/>
-      <c r="HS52" s="28"/>
-      <c r="HT52" s="28"/>
-      <c r="HU52" s="28"/>
-      <c r="HV52" s="28"/>
-      <c r="HW52" s="28"/>
-      <c r="HX52" s="28"/>
-      <c r="HY52" s="28"/>
-      <c r="HZ52" s="28"/>
-      <c r="IA52" s="28"/>
-      <c r="IB52" s="28"/>
-      <c r="IC52" s="28"/>
-      <c r="ID52" s="28"/>
-      <c r="IE52" s="28"/>
-      <c r="IF52" s="28"/>
-      <c r="IG52" s="28"/>
-      <c r="IH52" s="28"/>
-      <c r="II52" s="28"/>
-      <c r="IJ52" s="28"/>
-      <c r="IK52" s="28"/>
-      <c r="IL52" s="28"/>
-      <c r="IM52" s="28"/>
-      <c r="IN52" s="28"/>
-      <c r="IO52" s="28"/>
-      <c r="IP52" s="28"/>
-      <c r="IQ52" s="28"/>
-      <c r="IR52" s="28"/>
-      <c r="IS52" s="28"/>
-      <c r="IT52" s="28"/>
-      <c r="IU52" s="28"/>
-      <c r="IV52" s="28"/>
-      <c r="IW52" s="28"/>
-      <c r="IX52" s="28"/>
-      <c r="IY52" s="28"/>
-      <c r="IZ52" s="28"/>
-      <c r="JA52" s="28"/>
-      <c r="JB52" s="28"/>
-      <c r="JC52" s="28"/>
-      <c r="JD52" s="28"/>
-      <c r="JE52" s="28"/>
-      <c r="JF52" s="28"/>
-      <c r="JG52" s="28"/>
-      <c r="JH52" s="28"/>
-      <c r="JI52" s="28"/>
-      <c r="JJ52" s="28"/>
-      <c r="JK52" s="28"/>
-      <c r="JL52" s="28"/>
-      <c r="JM52" s="28"/>
-      <c r="JN52" s="28"/>
-      <c r="JO52" s="28"/>
-      <c r="JP52" s="28"/>
-      <c r="JQ52" s="28"/>
-      <c r="JR52" s="28"/>
-      <c r="JS52" s="28"/>
-      <c r="JT52" s="28"/>
-      <c r="JU52" s="28"/>
-      <c r="JV52" s="28"/>
-      <c r="JW52" s="28"/>
-      <c r="JX52" s="28"/>
-      <c r="JY52" s="28"/>
-      <c r="JZ52" s="28"/>
-      <c r="KA52" s="28"/>
-    </row>
-    <row r="53" spans="1:287" ht="30.75" customHeight="1">
-      <c r="A53" s="33"/>
-      <c r="B53" s="28"/>
-      <c r="C53" s="30"/>
-      <c r="D53" s="28"/>
-      <c r="E53" s="28"/>
-      <c r="F53" s="28"/>
-      <c r="G53" s="28"/>
-      <c r="H53" s="28"/>
-      <c r="I53" s="29"/>
-      <c r="J53" s="40"/>
-      <c r="K53" s="28"/>
-      <c r="L53" s="28"/>
-      <c r="M53" s="28"/>
-      <c r="N53" s="28"/>
-      <c r="O53" s="28"/>
-      <c r="P53" s="28"/>
-      <c r="Q53" s="28"/>
-      <c r="R53" s="28"/>
-      <c r="S53" s="28"/>
-      <c r="T53" s="28"/>
-      <c r="U53" s="28"/>
-      <c r="V53" s="28"/>
-      <c r="W53" s="28"/>
-      <c r="X53" s="28"/>
-      <c r="Y53" s="28"/>
-      <c r="Z53" s="28"/>
-      <c r="AA53" s="28"/>
-      <c r="AB53" s="28"/>
-      <c r="AC53" s="28"/>
-      <c r="AD53" s="28"/>
-      <c r="AE53" s="28"/>
-      <c r="AF53" s="28"/>
-      <c r="AG53" s="28"/>
-      <c r="AH53" s="28"/>
-      <c r="AI53" s="28"/>
-      <c r="AJ53" s="28"/>
-      <c r="AK53" s="28"/>
-      <c r="AL53" s="28"/>
-      <c r="AM53" s="28"/>
-      <c r="AN53" s="28"/>
-      <c r="AO53" s="28"/>
-      <c r="AP53" s="28"/>
-      <c r="AQ53" s="28"/>
-      <c r="AR53" s="28"/>
-      <c r="AS53" s="28"/>
-      <c r="AT53" s="28"/>
-      <c r="AU53" s="28"/>
-      <c r="AV53" s="28"/>
-      <c r="AW53" s="28"/>
-      <c r="AX53" s="28"/>
-      <c r="AY53" s="28"/>
-      <c r="AZ53" s="28"/>
-      <c r="BA53" s="28"/>
-      <c r="BB53" s="28"/>
-      <c r="BC53" s="28"/>
-      <c r="BD53" s="28"/>
-      <c r="BE53" s="28"/>
-      <c r="BF53" s="28"/>
-      <c r="BG53" s="28"/>
-      <c r="BH53" s="28"/>
-      <c r="BI53" s="28"/>
-      <c r="BJ53" s="28"/>
-      <c r="BK53" s="28"/>
-      <c r="BL53" s="28"/>
-      <c r="BM53" s="28"/>
-      <c r="BN53" s="28"/>
-      <c r="BO53" s="28"/>
-      <c r="BP53" s="28"/>
-      <c r="BQ53" s="28"/>
-      <c r="BR53" s="28"/>
-      <c r="BS53" s="28"/>
-      <c r="BT53" s="28"/>
-      <c r="BU53" s="28"/>
-      <c r="BV53" s="28"/>
-      <c r="BW53" s="28"/>
-      <c r="BX53" s="28"/>
-      <c r="BY53" s="28"/>
-      <c r="BZ53" s="28"/>
-      <c r="CA53" s="28"/>
-      <c r="CB53" s="28"/>
-      <c r="CC53" s="28"/>
-      <c r="CD53" s="28"/>
-      <c r="CE53" s="28"/>
-      <c r="CF53" s="28"/>
-      <c r="CG53" s="28"/>
-      <c r="CH53" s="28"/>
-      <c r="CI53" s="28"/>
-      <c r="CJ53" s="28"/>
-      <c r="CK53" s="28"/>
-      <c r="CL53" s="28"/>
-      <c r="CM53" s="28"/>
-      <c r="CN53" s="28"/>
-      <c r="CO53" s="28"/>
-      <c r="CP53" s="28"/>
-      <c r="CQ53" s="28"/>
-      <c r="CR53" s="28"/>
-      <c r="CS53" s="28"/>
-      <c r="CT53" s="28"/>
-      <c r="CU53" s="28"/>
-      <c r="CV53" s="28"/>
-      <c r="CW53" s="28"/>
-      <c r="CX53" s="28"/>
-      <c r="CY53" s="28"/>
-      <c r="CZ53" s="28"/>
-      <c r="DA53" s="28"/>
-      <c r="DB53" s="28"/>
-      <c r="DC53" s="28"/>
-      <c r="DD53" s="28"/>
-      <c r="DE53" s="28"/>
-      <c r="DF53" s="28"/>
-      <c r="DG53" s="28"/>
-      <c r="DH53" s="28"/>
-      <c r="DI53" s="28"/>
-      <c r="DJ53" s="28"/>
-      <c r="DK53" s="28"/>
-      <c r="DL53" s="28"/>
-      <c r="DM53" s="28"/>
-      <c r="DN53" s="28"/>
-      <c r="DO53" s="28"/>
-      <c r="DP53" s="28"/>
-      <c r="DQ53" s="28"/>
-      <c r="DR53" s="28"/>
-      <c r="DS53" s="28"/>
-      <c r="DT53" s="28"/>
-      <c r="DU53" s="28"/>
-      <c r="DV53" s="28"/>
-      <c r="DW53" s="28"/>
-      <c r="DX53" s="28"/>
-      <c r="DY53" s="28"/>
-      <c r="DZ53" s="28"/>
-      <c r="EA53" s="28"/>
-      <c r="EB53" s="28"/>
-      <c r="EC53" s="28"/>
-      <c r="ED53" s="28"/>
-      <c r="EE53" s="28"/>
-      <c r="EF53" s="28"/>
-      <c r="EG53" s="28"/>
-      <c r="EH53" s="28"/>
-      <c r="EI53" s="28"/>
-      <c r="EJ53" s="28"/>
-      <c r="EK53" s="28"/>
-      <c r="EL53" s="28"/>
-      <c r="EM53" s="28"/>
-      <c r="EN53" s="28"/>
-      <c r="EO53" s="28"/>
-      <c r="EP53" s="28"/>
-      <c r="EQ53" s="28"/>
-      <c r="ER53" s="28"/>
-      <c r="ES53" s="28"/>
-      <c r="ET53" s="28"/>
-      <c r="EU53" s="28"/>
-      <c r="EV53" s="28"/>
-      <c r="EW53" s="28"/>
-      <c r="EX53" s="28"/>
-      <c r="EY53" s="28"/>
-      <c r="EZ53" s="28"/>
-      <c r="FA53" s="28"/>
-      <c r="FB53" s="28"/>
-      <c r="FC53" s="28"/>
-      <c r="FD53" s="28"/>
-      <c r="FE53" s="28"/>
-      <c r="FF53" s="28"/>
-      <c r="FG53" s="28"/>
-      <c r="FH53" s="28"/>
-      <c r="FI53" s="28"/>
-      <c r="FJ53" s="28"/>
-      <c r="FK53" s="28"/>
-      <c r="FL53" s="28"/>
-      <c r="FM53" s="28"/>
-      <c r="FN53" s="28"/>
-      <c r="FO53" s="28"/>
-      <c r="FP53" s="28"/>
-      <c r="FQ53" s="28"/>
-      <c r="FR53" s="28"/>
-      <c r="FS53" s="28"/>
-      <c r="FT53" s="28"/>
-      <c r="FU53" s="28"/>
-      <c r="FV53" s="28"/>
-      <c r="FW53" s="28"/>
-      <c r="FX53" s="28"/>
-      <c r="FY53" s="28"/>
-      <c r="FZ53" s="28"/>
-      <c r="GA53" s="28"/>
-      <c r="GB53" s="28"/>
-      <c r="GC53" s="28"/>
-      <c r="GD53" s="28"/>
-      <c r="GE53" s="28"/>
-      <c r="GF53" s="28"/>
-      <c r="GG53" s="28"/>
-      <c r="GH53" s="28"/>
-      <c r="GI53" s="28"/>
-      <c r="GJ53" s="28"/>
-      <c r="GK53" s="28"/>
-      <c r="GL53" s="28"/>
-      <c r="GM53" s="28"/>
-      <c r="GN53" s="28"/>
-      <c r="GO53" s="28"/>
-      <c r="GP53" s="28"/>
-      <c r="GQ53" s="28"/>
-      <c r="GR53" s="28"/>
-      <c r="GS53" s="28"/>
-      <c r="GT53" s="28"/>
-      <c r="GU53" s="28"/>
-      <c r="GV53" s="28"/>
-      <c r="GW53" s="28"/>
-      <c r="GX53" s="28"/>
-      <c r="GY53" s="28"/>
-      <c r="GZ53" s="28"/>
-      <c r="HA53" s="28"/>
-      <c r="HB53" s="28"/>
-      <c r="HC53" s="28"/>
-      <c r="HD53" s="28"/>
-      <c r="HE53" s="28"/>
-      <c r="HF53" s="28"/>
-      <c r="HG53" s="28"/>
-      <c r="HH53" s="28"/>
-      <c r="HI53" s="28"/>
-      <c r="HJ53" s="28"/>
-      <c r="HK53" s="28"/>
-      <c r="HL53" s="28"/>
-      <c r="HM53" s="28"/>
-      <c r="HN53" s="28"/>
-      <c r="HO53" s="28"/>
-      <c r="HP53" s="28"/>
-      <c r="HQ53" s="28"/>
-      <c r="HR53" s="28"/>
-      <c r="HS53" s="28"/>
-      <c r="HT53" s="28"/>
-      <c r="HU53" s="28"/>
-      <c r="HV53" s="28"/>
-      <c r="HW53" s="28"/>
-      <c r="HX53" s="28"/>
-      <c r="HY53" s="28"/>
-      <c r="HZ53" s="28"/>
-      <c r="IA53" s="28"/>
-      <c r="IB53" s="28"/>
-      <c r="IC53" s="28"/>
-      <c r="ID53" s="28"/>
-      <c r="IE53" s="28"/>
-      <c r="IF53" s="28"/>
-      <c r="IG53" s="28"/>
-      <c r="IH53" s="28"/>
-      <c r="II53" s="28"/>
-      <c r="IJ53" s="28"/>
-      <c r="IK53" s="28"/>
-      <c r="IL53" s="28"/>
-      <c r="IM53" s="28"/>
-      <c r="IN53" s="28"/>
-      <c r="IO53" s="28"/>
-      <c r="IP53" s="28"/>
-      <c r="IQ53" s="28"/>
-      <c r="IR53" s="28"/>
-      <c r="IS53" s="28"/>
-      <c r="IT53" s="28"/>
-      <c r="IU53" s="28"/>
-      <c r="IV53" s="28"/>
-      <c r="IW53" s="28"/>
-      <c r="IX53" s="28"/>
-      <c r="IY53" s="28"/>
-      <c r="IZ53" s="28"/>
-      <c r="JA53" s="28"/>
-      <c r="JB53" s="28"/>
-      <c r="JC53" s="28"/>
-      <c r="JD53" s="28"/>
-      <c r="JE53" s="28"/>
-      <c r="JF53" s="28"/>
-      <c r="JG53" s="28"/>
-      <c r="JH53" s="28"/>
-      <c r="JI53" s="28"/>
-      <c r="JJ53" s="28"/>
-      <c r="JK53" s="28"/>
-      <c r="JL53" s="28"/>
-      <c r="JM53" s="28"/>
-      <c r="JN53" s="28"/>
-      <c r="JO53" s="28"/>
-      <c r="JP53" s="28"/>
-      <c r="JQ53" s="28"/>
-      <c r="JR53" s="28"/>
-      <c r="JS53" s="28"/>
-      <c r="JT53" s="28"/>
-      <c r="JU53" s="28"/>
-      <c r="JV53" s="28"/>
-      <c r="JW53" s="28"/>
-      <c r="JX53" s="28"/>
-      <c r="JY53" s="28"/>
-      <c r="JZ53" s="28"/>
-      <c r="KA53" s="28"/>
+    <row r="52" spans="1:287" ht="13.2">
+      <c r="A52" s="34"/>
+    </row>
+    <row r="53" spans="1:287" ht="13.2">
+      <c r="A53" s="34"/>
     </row>
     <row r="54" spans="1:287" ht="13.2">
       <c r="A54" s="34"/>
@@ -19225,14 +18770,9 @@
     <row r="999" spans="1:1" ht="13.2">
       <c r="A999" s="34"/>
     </row>
-    <row r="1000" spans="1:1" ht="13.2">
-      <c r="A1000" s="34"/>
-    </row>
-    <row r="1001" spans="1:1" ht="13.2">
-      <c r="A1001" s="34"/>
-    </row>
   </sheetData>
-  <mergeCells count="8">
+  <mergeCells count="9">
+    <mergeCell ref="A33:J33"/>
     <mergeCell ref="A29:J29"/>
     <mergeCell ref="A13:J13"/>
     <mergeCell ref="A24:J24"/>
@@ -19243,16 +18783,16 @@
     <mergeCell ref="A7:J7"/>
   </mergeCells>
   <dataValidations count="4">
-    <dataValidation type="list" allowBlank="1" sqref="I8:I12 I14:I23 I25:I28 I30:I53" xr:uid="{00000000-0002-0000-0000-000000000000}">
+    <dataValidation type="list" allowBlank="1" sqref="I8:I12 I14:I23 I25:I28 I30:I32 I34:I51" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>"STILL,ON GOING,DELIVERED,DELIVERED (LATE)"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" sqref="C8:C12 C14:C23 C25:C28 C30:C53" xr:uid="{00000000-0002-0000-0000-000002000000}">
+    <dataValidation type="list" allowBlank="1" sqref="C8:C12 C14:C23 C25:C28 C30:C32 C34:C51" xr:uid="{00000000-0002-0000-0000-000002000000}">
       <formula1>"Hazem Mekawy,Esraa Awad,Nada Mohamed,Mina Helmi,Alzahraa El-Sallakh"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" sqref="B8:B12 B14:B23 B25:B28 B30:B33" xr:uid="{8C288E01-D924-4500-863C-FF5C93406017}">
+    <dataValidation type="list" allowBlank="1" sqref="B8:B12 B14:B23 B25:B28 B30:B32 B34:B38" xr:uid="{8C288E01-D924-4500-863C-FF5C93406017}">
       <formula1>"Documentation, Code Implementation"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" sqref="B33:B53" xr:uid="{00000000-0002-0000-0000-000001000000}">
+    <dataValidation type="list" allowBlank="1" sqref="B34:B51" xr:uid="{00000000-0002-0000-0000-000001000000}">
       <formula1>"Technical,Non -Technical"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
Updating PP delivery dates Signed-off-by: Hazemmekawy <dextermekawy@gmail.com>
</commit_message>
<xml_diff>
--- a/SW deliveries log/PP.xlsx
+++ b/SW deliveries log/PP.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\ITI COURSES\Software Engineering\SWE_WORKSPACE\SW deliveries log\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D57DEC64-0A7A-46DF-9E51-B48BD23F000C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C381EA20-7938-4F1C-A171-577A2B38CB04}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="106" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -664,10 +664,26 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="20" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="22" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="16" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -682,22 +698,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="22" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="20" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -918,8 +918,8 @@
   </sheetPr>
   <dimension ref="A1:KA999"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B28" workbookViewId="0">
-      <selection activeCell="J38" sqref="J38"/>
+    <sheetView tabSelected="1" topLeftCell="C28" workbookViewId="0">
+      <selection activeCell="F37" sqref="F37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1"/>
@@ -935,13 +935,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:287" ht="28.2">
-      <c r="A1" s="45" t="s">
+      <c r="A1" s="51" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="44"/>
-      <c r="C1" s="44"/>
-      <c r="D1" s="44"/>
-      <c r="E1" s="44"/>
+      <c r="B1" s="49"/>
+      <c r="C1" s="49"/>
+      <c r="D1" s="49"/>
+      <c r="E1" s="49"/>
       <c r="F1" s="1"/>
       <c r="G1" s="1"/>
       <c r="H1" s="1"/>
@@ -1241,11 +1241,11 @@
       <c r="E2" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="46" t="s">
+      <c r="F2" s="52" t="s">
         <v>6</v>
       </c>
-      <c r="G2" s="47"/>
-      <c r="H2" s="47"/>
+      <c r="G2" s="53"/>
+      <c r="H2" s="53"/>
       <c r="I2" s="8"/>
       <c r="J2" s="38"/>
       <c r="K2" s="8"/>
@@ -1829,12 +1829,12 @@
       <c r="A4" s="20" t="s">
         <v>12</v>
       </c>
-      <c r="B4" s="48" t="s">
+      <c r="B4" s="54" t="s">
         <v>13</v>
       </c>
-      <c r="C4" s="44"/>
-      <c r="D4" s="44"/>
-      <c r="E4" s="44"/>
+      <c r="C4" s="49"/>
+      <c r="D4" s="49"/>
+      <c r="E4" s="49"/>
       <c r="F4" s="21"/>
       <c r="G4" s="21"/>
       <c r="H4" s="22"/>
@@ -2153,18 +2153,18 @@
       <c r="KA5" s="19"/>
     </row>
     <row r="6" spans="1:287" ht="30.75" customHeight="1">
-      <c r="A6" s="49" t="s">
+      <c r="A6" s="55" t="s">
         <v>24</v>
       </c>
-      <c r="B6" s="50"/>
-      <c r="C6" s="50"/>
-      <c r="D6" s="50"/>
-      <c r="E6" s="50"/>
-      <c r="F6" s="50"/>
-      <c r="G6" s="50"/>
-      <c r="H6" s="50"/>
-      <c r="I6" s="50"/>
-      <c r="J6" s="50"/>
+      <c r="B6" s="56"/>
+      <c r="C6" s="56"/>
+      <c r="D6" s="56"/>
+      <c r="E6" s="56"/>
+      <c r="F6" s="56"/>
+      <c r="G6" s="56"/>
+      <c r="H6" s="56"/>
+      <c r="I6" s="56"/>
+      <c r="J6" s="56"/>
       <c r="K6" s="28"/>
       <c r="L6" s="28"/>
       <c r="M6" s="28"/>
@@ -2444,18 +2444,18 @@
       <c r="KA6" s="28"/>
     </row>
     <row r="7" spans="1:287" ht="30.75" customHeight="1">
-      <c r="A7" s="43" t="s">
+      <c r="A7" s="50" t="s">
         <v>25</v>
       </c>
-      <c r="B7" s="44"/>
-      <c r="C7" s="44"/>
-      <c r="D7" s="44"/>
-      <c r="E7" s="44"/>
-      <c r="F7" s="44"/>
-      <c r="G7" s="44"/>
-      <c r="H7" s="44"/>
-      <c r="I7" s="44"/>
-      <c r="J7" s="44"/>
+      <c r="B7" s="49"/>
+      <c r="C7" s="49"/>
+      <c r="D7" s="49"/>
+      <c r="E7" s="49"/>
+      <c r="F7" s="49"/>
+      <c r="G7" s="49"/>
+      <c r="H7" s="49"/>
+      <c r="I7" s="49"/>
+      <c r="J7" s="49"/>
       <c r="K7" s="28"/>
       <c r="L7" s="28"/>
       <c r="M7" s="28"/>
@@ -4278,18 +4278,18 @@
       <c r="KA12" s="28"/>
     </row>
     <row r="13" spans="1:287" ht="30.75" customHeight="1">
-      <c r="A13" s="43" t="s">
+      <c r="A13" s="50" t="s">
         <v>40</v>
       </c>
-      <c r="B13" s="44"/>
-      <c r="C13" s="44"/>
-      <c r="D13" s="44"/>
-      <c r="E13" s="44"/>
-      <c r="F13" s="44"/>
-      <c r="G13" s="44"/>
-      <c r="H13" s="44"/>
-      <c r="I13" s="44"/>
-      <c r="J13" s="44"/>
+      <c r="B13" s="49"/>
+      <c r="C13" s="49"/>
+      <c r="D13" s="49"/>
+      <c r="E13" s="49"/>
+      <c r="F13" s="49"/>
+      <c r="G13" s="49"/>
+      <c r="H13" s="49"/>
+      <c r="I13" s="49"/>
+      <c r="J13" s="49"/>
       <c r="K13" s="28"/>
       <c r="L13" s="28"/>
       <c r="M13" s="28"/>
@@ -7641,18 +7641,18 @@
       <c r="KA23" s="28"/>
     </row>
     <row r="24" spans="1:287" ht="30.75" customHeight="1">
-      <c r="A24" s="43" t="s">
+      <c r="A24" s="50" t="s">
         <v>51</v>
       </c>
-      <c r="B24" s="44"/>
-      <c r="C24" s="44"/>
-      <c r="D24" s="44"/>
-      <c r="E24" s="44"/>
-      <c r="F24" s="44"/>
-      <c r="G24" s="44"/>
-      <c r="H24" s="44"/>
-      <c r="I24" s="44"/>
-      <c r="J24" s="44"/>
+      <c r="B24" s="49"/>
+      <c r="C24" s="49"/>
+      <c r="D24" s="49"/>
+      <c r="E24" s="49"/>
+      <c r="F24" s="49"/>
+      <c r="G24" s="49"/>
+      <c r="H24" s="49"/>
+      <c r="I24" s="49"/>
+      <c r="J24" s="49"/>
       <c r="K24" s="28"/>
       <c r="L24" s="28"/>
       <c r="M24" s="28"/>
@@ -9160,18 +9160,18 @@
       <c r="KA28" s="28"/>
     </row>
     <row r="29" spans="1:287" s="42" customFormat="1" ht="30.75" customHeight="1">
-      <c r="A29" s="51" t="s">
+      <c r="A29" s="48" t="s">
         <v>54</v>
       </c>
-      <c r="B29" s="44"/>
-      <c r="C29" s="44"/>
-      <c r="D29" s="44"/>
-      <c r="E29" s="44"/>
-      <c r="F29" s="44"/>
-      <c r="G29" s="44"/>
-      <c r="H29" s="44"/>
-      <c r="I29" s="44"/>
-      <c r="J29" s="44"/>
+      <c r="B29" s="49"/>
+      <c r="C29" s="49"/>
+      <c r="D29" s="49"/>
+      <c r="E29" s="49"/>
+      <c r="F29" s="49"/>
+      <c r="G29" s="49"/>
+      <c r="H29" s="49"/>
+      <c r="I29" s="49"/>
+      <c r="J29" s="49"/>
       <c r="K29" s="30"/>
       <c r="L29" s="30"/>
       <c r="M29" s="30"/>
@@ -10372,18 +10372,18 @@
       <c r="KA32" s="28"/>
     </row>
     <row r="33" spans="1:287" ht="30.75" customHeight="1">
-      <c r="A33" s="52" t="s">
+      <c r="A33" s="46" t="s">
         <v>60</v>
       </c>
-      <c r="B33" s="53"/>
-      <c r="C33" s="53"/>
-      <c r="D33" s="53"/>
-      <c r="E33" s="53"/>
-      <c r="F33" s="53"/>
-      <c r="G33" s="53"/>
-      <c r="H33" s="53"/>
-      <c r="I33" s="53"/>
-      <c r="J33" s="53"/>
+      <c r="B33" s="47"/>
+      <c r="C33" s="47"/>
+      <c r="D33" s="47"/>
+      <c r="E33" s="47"/>
+      <c r="F33" s="47"/>
+      <c r="G33" s="47"/>
+      <c r="H33" s="47"/>
+      <c r="I33" s="47"/>
+      <c r="J33" s="47"/>
       <c r="K33" s="28"/>
       <c r="L33" s="28"/>
       <c r="M33" s="28"/>
@@ -10663,7 +10663,7 @@
       <c r="KA33" s="28"/>
     </row>
     <row r="34" spans="1:287" s="41" customFormat="1" ht="56.4" customHeight="1">
-      <c r="A34" s="55" t="s">
+      <c r="A34" s="44" t="s">
         <v>62</v>
       </c>
       <c r="B34" s="40" t="s">
@@ -10672,19 +10672,25 @@
       <c r="C34" s="40" t="s">
         <v>8</v>
       </c>
-      <c r="D34" s="56">
+      <c r="D34" s="45">
         <v>43885</v>
       </c>
-      <c r="E34" s="56">
+      <c r="E34" s="45">
         <v>43886</v>
       </c>
-      <c r="F34" s="40"/>
-      <c r="G34" s="40"/>
-      <c r="H34" s="40"/>
-      <c r="I34" s="55" t="s">
-        <v>57</v>
-      </c>
-      <c r="J34" s="54" t="s">
+      <c r="F34" s="45">
+        <v>43887</v>
+      </c>
+      <c r="G34" s="45">
+        <v>43888</v>
+      </c>
+      <c r="H34" s="40">
+        <v>2</v>
+      </c>
+      <c r="I34" s="44" t="s">
+        <v>31</v>
+      </c>
+      <c r="J34" s="43" t="s">
         <v>63</v>
       </c>
       <c r="K34" s="40"/>
@@ -10975,17 +10981,23 @@
       <c r="C35" s="30" t="s">
         <v>38</v>
       </c>
-      <c r="D35" s="56">
+      <c r="D35" s="45">
         <v>43886</v>
       </c>
-      <c r="E35" s="56">
+      <c r="E35" s="45">
         <v>43887</v>
       </c>
-      <c r="F35" s="28"/>
-      <c r="G35" s="28"/>
-      <c r="H35" s="28"/>
-      <c r="I35" s="55" t="s">
-        <v>57</v>
+      <c r="F35" s="45">
+        <v>43888</v>
+      </c>
+      <c r="G35" s="45">
+        <v>43888</v>
+      </c>
+      <c r="H35" s="28">
+        <v>1</v>
+      </c>
+      <c r="I35" s="44" t="s">
+        <v>31</v>
       </c>
       <c r="J35" s="40"/>
       <c r="K35" s="28"/>
@@ -11276,17 +11288,19 @@
       <c r="C36" s="30" t="s">
         <v>30</v>
       </c>
-      <c r="D36" s="56">
+      <c r="D36" s="45">
         <v>43887</v>
       </c>
-      <c r="E36" s="56">
+      <c r="E36" s="45">
         <v>43888</v>
       </c>
-      <c r="F36" s="28"/>
-      <c r="G36" s="28"/>
+      <c r="F36" s="45">
+        <v>43888</v>
+      </c>
+      <c r="G36" s="45"/>
       <c r="H36" s="28"/>
-      <c r="I36" s="55" t="s">
-        <v>57</v>
+      <c r="I36" s="44" t="s">
+        <v>28</v>
       </c>
       <c r="J36" s="40"/>
       <c r="K36" s="28"/>
@@ -11577,16 +11591,16 @@
       <c r="C37" s="30" t="s">
         <v>34</v>
       </c>
-      <c r="D37" s="56">
+      <c r="D37" s="45">
         <v>43889</v>
       </c>
-      <c r="E37" s="56">
+      <c r="E37" s="45">
         <v>43889</v>
       </c>
-      <c r="F37" s="28"/>
-      <c r="G37" s="28"/>
+      <c r="F37" s="45"/>
+      <c r="G37" s="45"/>
       <c r="H37" s="28"/>
-      <c r="I37" s="55" t="s">
+      <c r="I37" s="44" t="s">
         <v>57</v>
       </c>
       <c r="J37" s="40"/>
@@ -11878,16 +11892,16 @@
       <c r="C38" s="30" t="s">
         <v>8</v>
       </c>
-      <c r="D38" s="56">
+      <c r="D38" s="45">
         <v>43889</v>
       </c>
-      <c r="E38" s="56">
+      <c r="E38" s="45">
         <v>43889</v>
       </c>
-      <c r="F38" s="28"/>
-      <c r="G38" s="28"/>
+      <c r="F38" s="45"/>
+      <c r="G38" s="45"/>
       <c r="H38" s="28"/>
-      <c r="I38" s="55" t="s">
+      <c r="I38" s="44" t="s">
         <v>57</v>
       </c>
       <c r="J38" s="40"/>
@@ -12178,7 +12192,7 @@
       <c r="F39" s="28"/>
       <c r="G39" s="28"/>
       <c r="H39" s="28"/>
-      <c r="I39" s="55"/>
+      <c r="I39" s="44"/>
       <c r="J39" s="40"/>
       <c r="K39" s="28"/>
       <c r="L39" s="28"/>

</xml_diff>

<commit_message>
- Updating the PP delivery dates - Updating SIQ sheet - Updating RTM Document
Signed-off-by: Hazemmekawy <dextermekawy@gmail.com>
</commit_message>
<xml_diff>
--- a/SW deliveries log/PP.xlsx
+++ b/SW deliveries log/PP.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\ITI COURSES\Software Engineering\SWE_WORKSPACE\SW deliveries log\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C381EA20-7938-4F1C-A171-577A2B38CB04}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{796D7422-A64C-4C2C-9AF8-594883D18248}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="106" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="64">
   <si>
     <t>Sovy - Digital Calculator PO1_DGC_PROJECT PLAN</t>
   </si>
@@ -191,9 +191,6 @@
   </si>
   <si>
     <t>RTM Document Update</t>
-  </si>
-  <si>
-    <t>STILL</t>
   </si>
   <si>
     <t>TASK TYPE</t>
@@ -918,8 +915,8 @@
   </sheetPr>
   <dimension ref="A1:KA999"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C28" workbookViewId="0">
-      <selection activeCell="F37" sqref="F37"/>
+    <sheetView tabSelected="1" topLeftCell="E33" workbookViewId="0">
+      <selection activeCell="J39" sqref="J39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1"/>
@@ -1848,7 +1845,7 @@
         <v>15</v>
       </c>
       <c r="B5" s="24" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C5" s="24" t="s">
         <v>16</v>
@@ -2739,7 +2736,7 @@
         <v>26</v>
       </c>
       <c r="B8" s="30" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C8" s="30" t="s">
         <v>8</v>
@@ -3046,7 +3043,7 @@
         <v>29</v>
       </c>
       <c r="B9" s="30" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C9" s="30" t="s">
         <v>30</v>
@@ -3355,7 +3352,7 @@
         <v>33</v>
       </c>
       <c r="B10" s="30" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C10" s="30" t="s">
         <v>34</v>
@@ -3664,7 +3661,7 @@
         <v>33</v>
       </c>
       <c r="B11" s="30" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C11" s="30" t="s">
         <v>36</v>
@@ -3973,7 +3970,7 @@
         <v>37</v>
       </c>
       <c r="B12" s="30" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C12" s="30" t="s">
         <v>38</v>
@@ -4573,7 +4570,7 @@
         <v>41</v>
       </c>
       <c r="B14" s="30" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C14" s="30" t="s">
         <v>38</v>
@@ -4880,7 +4877,7 @@
         <v>42</v>
       </c>
       <c r="B15" s="30" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C15" s="30" t="s">
         <v>36</v>
@@ -5187,7 +5184,7 @@
         <v>43</v>
       </c>
       <c r="B16" s="30" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C16" s="30" t="s">
         <v>34</v>
@@ -5494,7 +5491,7 @@
         <v>44</v>
       </c>
       <c r="B17" s="30" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C17" s="30" t="s">
         <v>30</v>
@@ -5801,7 +5798,7 @@
         <v>47</v>
       </c>
       <c r="B18" s="30" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C18" s="30" t="s">
         <v>8</v>
@@ -6108,7 +6105,7 @@
         <v>45</v>
       </c>
       <c r="B19" s="30" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C19" s="30" t="s">
         <v>8</v>
@@ -6415,7 +6412,7 @@
         <v>46</v>
       </c>
       <c r="B20" s="30" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C20" s="30" t="s">
         <v>36</v>
@@ -6722,7 +6719,7 @@
         <v>48</v>
       </c>
       <c r="B21" s="30" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C21" s="30" t="s">
         <v>38</v>
@@ -7029,7 +7026,7 @@
         <v>49</v>
       </c>
       <c r="B22" s="30" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C22" s="30" t="s">
         <v>34</v>
@@ -7336,7 +7333,7 @@
         <v>50</v>
       </c>
       <c r="B23" s="30" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C23" s="30" t="s">
         <v>8</v>
@@ -7936,7 +7933,7 @@
         <v>41</v>
       </c>
       <c r="B25" s="30" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C25" s="30" t="s">
         <v>34</v>
@@ -8243,7 +8240,7 @@
         <v>48</v>
       </c>
       <c r="B26" s="30" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C26" s="30" t="s">
         <v>34</v>
@@ -8547,10 +8544,10 @@
     </row>
     <row r="27" spans="1:287" ht="30.75" customHeight="1">
       <c r="A27" s="33" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B27" s="30" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C27" s="30" t="s">
         <v>8</v>
@@ -8857,7 +8854,7 @@
         <v>53</v>
       </c>
       <c r="B28" s="30" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C28" s="30" t="s">
         <v>30</v>
@@ -9455,7 +9452,7 @@
         <v>53</v>
       </c>
       <c r="B30" s="30" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C30" s="30" t="s">
         <v>30</v>
@@ -9476,7 +9473,7 @@
         <v>3</v>
       </c>
       <c r="I30" s="33" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="J30" s="40"/>
       <c r="K30" s="30"/>
@@ -9762,7 +9759,7 @@
         <v>47</v>
       </c>
       <c r="B31" s="30" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C31" s="30" t="s">
         <v>38</v>
@@ -9783,7 +9780,7 @@
         <v>1</v>
       </c>
       <c r="I31" s="33" t="s">
-        <v>57</v>
+        <v>31</v>
       </c>
       <c r="J31" s="40"/>
       <c r="K31" s="30"/>
@@ -10069,7 +10066,7 @@
         <v>55</v>
       </c>
       <c r="B32" s="30" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C32" s="30" t="s">
         <v>36</v>
@@ -10373,7 +10370,7 @@
     </row>
     <row r="33" spans="1:287" ht="30.75" customHeight="1">
       <c r="A33" s="46" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B33" s="47"/>
       <c r="C33" s="47"/>
@@ -10664,10 +10661,10 @@
     </row>
     <row r="34" spans="1:287" s="41" customFormat="1" ht="56.4" customHeight="1">
       <c r="A34" s="44" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B34" s="40" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C34" s="40" t="s">
         <v>8</v>
@@ -10691,7 +10688,7 @@
         <v>31</v>
       </c>
       <c r="J34" s="43" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="K34" s="40"/>
       <c r="L34" s="40"/>
@@ -10976,7 +10973,7 @@
         <v>48</v>
       </c>
       <c r="B35" s="40" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C35" s="30" t="s">
         <v>38</v>
@@ -11283,7 +11280,7 @@
         <v>53</v>
       </c>
       <c r="B36" s="40" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C36" s="30" t="s">
         <v>30</v>
@@ -11297,10 +11294,14 @@
       <c r="F36" s="45">
         <v>43888</v>
       </c>
-      <c r="G36" s="45"/>
-      <c r="H36" s="28"/>
+      <c r="G36" s="45">
+        <v>43888</v>
+      </c>
+      <c r="H36" s="28">
+        <v>1</v>
+      </c>
       <c r="I36" s="44" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="J36" s="40"/>
       <c r="K36" s="28"/>
@@ -11583,13 +11584,13 @@
     </row>
     <row r="37" spans="1:287" ht="30.75" customHeight="1">
       <c r="A37" s="33" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B37" s="40" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C37" s="30" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="D37" s="45">
         <v>43889</v>
@@ -11597,11 +11598,17 @@
       <c r="E37" s="45">
         <v>43889</v>
       </c>
-      <c r="F37" s="45"/>
-      <c r="G37" s="45"/>
-      <c r="H37" s="28"/>
+      <c r="F37" s="45">
+        <v>43888</v>
+      </c>
+      <c r="G37" s="45">
+        <v>43888</v>
+      </c>
+      <c r="H37" s="28">
+        <v>1</v>
+      </c>
       <c r="I37" s="44" t="s">
-        <v>57</v>
+        <v>31</v>
       </c>
       <c r="J37" s="40"/>
       <c r="K37" s="28"/>
@@ -11887,7 +11894,7 @@
         <v>56</v>
       </c>
       <c r="B38" s="40" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C38" s="30" t="s">
         <v>8</v>
@@ -11898,11 +11905,13 @@
       <c r="E38" s="45">
         <v>43889</v>
       </c>
-      <c r="F38" s="45"/>
+      <c r="F38" s="45">
+        <v>43889</v>
+      </c>
       <c r="G38" s="45"/>
       <c r="H38" s="28"/>
       <c r="I38" s="44" t="s">
-        <v>57</v>
+        <v>28</v>
       </c>
       <c r="J38" s="40"/>
       <c r="K38" s="28"/>
@@ -18796,9 +18805,9 @@
     <mergeCell ref="A6:J6"/>
     <mergeCell ref="A7:J7"/>
   </mergeCells>
-  <dataValidations count="4">
-    <dataValidation type="list" allowBlank="1" sqref="I8:I12 I14:I23 I25:I28 I30:I32 I34:I51" xr:uid="{00000000-0002-0000-0000-000000000000}">
-      <formula1>"STILL,ON GOING,DELIVERED,DELIVERED (LATE)"</formula1>
+  <dataValidations count="5">
+    <dataValidation type="list" allowBlank="1" sqref="I39:I51" xr:uid="{00000000-0002-0000-0000-000000000000}">
+      <formula1>"STILL,ON GOING,DELIVERED"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" sqref="C8:C12 C14:C23 C25:C28 C30:C32 C34:C51" xr:uid="{00000000-0002-0000-0000-000002000000}">
       <formula1>"Hazem Mekawy,Esraa Awad,Nada Mohamed,Mina Helmi,Alzahraa El-Sallakh"</formula1>
@@ -18809,6 +18818,9 @@
     <dataValidation type="list" allowBlank="1" sqref="B34:B51" xr:uid="{00000000-0002-0000-0000-000001000000}">
       <formula1>"Technical,Non -Technical"</formula1>
     </dataValidation>
+    <dataValidation type="list" allowBlank="1" sqref="I8 I9 I10 I11 I12 I12 I14 I15 I16 I17 I18:I23 I25 I26:I28 I30:I32 I34:I38" xr:uid="{D54F693B-0EBC-4A9C-B3BB-6C4EBEAEDD84}">
+      <formula1>"STILL,ON GOING,DELIVERED"</formula1>
+    </dataValidation>
   </dataValidations>
   <hyperlinks>
     <hyperlink ref="B4" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>

</xml_diff>

<commit_message>
Updating the PP for WEEK6 Signed-off-by: Hazemmekawy <dextermekawy@gmail.com>
</commit_message>
<xml_diff>
--- a/SW deliveries log/PP.xlsx
+++ b/SW deliveries log/PP.xlsx
@@ -8,19 +8,27 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\ITI COURSES\Software Engineering\SWE_WORKSPACE\SW deliveries log\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F8D6AB5-D1AF-4926-BE93-F5FDCE83EF5A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66F6C639-225A-4AB2-9A63-52AD90BB3AB5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="106" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PP" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="181029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="72">
   <si>
     <t>Sovy - Digital Calculator PO1_DGC_PROJECT PLAN</t>
   </si>
@@ -236,6 +244,9 @@
   <si>
     <t>Releasing the Documents 
 based on the documents reviews</t>
+  </si>
+  <si>
+    <t>WEEK 6</t>
   </si>
 </sst>
 </file>
@@ -551,7 +562,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="56">
+  <cellXfs count="57">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -681,20 +692,11 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="15" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="21" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="21" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -706,6 +708,16 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="15" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="21" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -927,7 +939,7 @@
   <dimension ref="A1:KA1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="D49" sqref="D49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1"/>
@@ -943,13 +955,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:287" ht="28.2">
-      <c r="A1" s="50" t="s">
+      <c r="A1" s="46" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="46"/>
-      <c r="C1" s="46"/>
-      <c r="D1" s="46"/>
-      <c r="E1" s="46"/>
+      <c r="B1" s="47"/>
+      <c r="C1" s="47"/>
+      <c r="D1" s="47"/>
+      <c r="E1" s="47"/>
       <c r="F1" s="1"/>
       <c r="G1" s="1"/>
       <c r="H1" s="1"/>
@@ -1249,11 +1261,11 @@
       <c r="E2" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="51" t="s">
+      <c r="F2" s="48" t="s">
         <v>6</v>
       </c>
-      <c r="G2" s="52"/>
-      <c r="H2" s="52"/>
+      <c r="G2" s="49"/>
+      <c r="H2" s="49"/>
       <c r="I2" s="8"/>
       <c r="J2" s="36"/>
       <c r="K2" s="8"/>
@@ -1837,12 +1849,12 @@
       <c r="A4" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="B4" s="53" t="s">
+      <c r="B4" s="50" t="s">
         <v>12</v>
       </c>
-      <c r="C4" s="46"/>
-      <c r="D4" s="46"/>
-      <c r="E4" s="46"/>
+      <c r="C4" s="47"/>
+      <c r="D4" s="47"/>
+      <c r="E4" s="47"/>
       <c r="F4" s="19"/>
       <c r="G4" s="19"/>
       <c r="H4" s="20"/>
@@ -2161,18 +2173,18 @@
       <c r="KA5" s="17"/>
     </row>
     <row r="6" spans="1:287" ht="30.75" customHeight="1">
-      <c r="A6" s="54" t="s">
+      <c r="A6" s="51" t="s">
         <v>23</v>
       </c>
-      <c r="B6" s="55"/>
-      <c r="C6" s="55"/>
-      <c r="D6" s="55"/>
-      <c r="E6" s="55"/>
-      <c r="F6" s="55"/>
-      <c r="G6" s="55"/>
-      <c r="H6" s="55"/>
-      <c r="I6" s="55"/>
-      <c r="J6" s="55"/>
+      <c r="B6" s="52"/>
+      <c r="C6" s="52"/>
+      <c r="D6" s="52"/>
+      <c r="E6" s="52"/>
+      <c r="F6" s="52"/>
+      <c r="G6" s="52"/>
+      <c r="H6" s="52"/>
+      <c r="I6" s="52"/>
+      <c r="J6" s="52"/>
       <c r="K6" s="26"/>
       <c r="L6" s="26"/>
       <c r="M6" s="26"/>
@@ -2452,18 +2464,18 @@
       <c r="KA6" s="26"/>
     </row>
     <row r="7" spans="1:287" ht="30.75" customHeight="1">
-      <c r="A7" s="45" t="s">
+      <c r="A7" s="53" t="s">
         <v>24</v>
       </c>
-      <c r="B7" s="46"/>
-      <c r="C7" s="46"/>
-      <c r="D7" s="46"/>
-      <c r="E7" s="46"/>
-      <c r="F7" s="46"/>
-      <c r="G7" s="46"/>
-      <c r="H7" s="46"/>
-      <c r="I7" s="46"/>
-      <c r="J7" s="46"/>
+      <c r="B7" s="47"/>
+      <c r="C7" s="47"/>
+      <c r="D7" s="47"/>
+      <c r="E7" s="47"/>
+      <c r="F7" s="47"/>
+      <c r="G7" s="47"/>
+      <c r="H7" s="47"/>
+      <c r="I7" s="47"/>
+      <c r="J7" s="47"/>
       <c r="K7" s="26"/>
       <c r="L7" s="26"/>
       <c r="M7" s="26"/>
@@ -4286,18 +4298,18 @@
       <c r="KA12" s="26"/>
     </row>
     <row r="13" spans="1:287" ht="30.75" customHeight="1">
-      <c r="A13" s="45" t="s">
+      <c r="A13" s="53" t="s">
         <v>39</v>
       </c>
-      <c r="B13" s="46"/>
-      <c r="C13" s="46"/>
-      <c r="D13" s="46"/>
-      <c r="E13" s="46"/>
-      <c r="F13" s="46"/>
-      <c r="G13" s="46"/>
-      <c r="H13" s="46"/>
-      <c r="I13" s="46"/>
-      <c r="J13" s="46"/>
+      <c r="B13" s="47"/>
+      <c r="C13" s="47"/>
+      <c r="D13" s="47"/>
+      <c r="E13" s="47"/>
+      <c r="F13" s="47"/>
+      <c r="G13" s="47"/>
+      <c r="H13" s="47"/>
+      <c r="I13" s="47"/>
+      <c r="J13" s="47"/>
       <c r="K13" s="26"/>
       <c r="L13" s="26"/>
       <c r="M13" s="26"/>
@@ -7649,18 +7661,18 @@
       <c r="KA23" s="26"/>
     </row>
     <row r="24" spans="1:287" ht="30.75" customHeight="1">
-      <c r="A24" s="45" t="s">
+      <c r="A24" s="53" t="s">
         <v>50</v>
       </c>
-      <c r="B24" s="46"/>
-      <c r="C24" s="46"/>
-      <c r="D24" s="46"/>
-      <c r="E24" s="46"/>
-      <c r="F24" s="46"/>
-      <c r="G24" s="46"/>
-      <c r="H24" s="46"/>
-      <c r="I24" s="46"/>
-      <c r="J24" s="46"/>
+      <c r="B24" s="47"/>
+      <c r="C24" s="47"/>
+      <c r="D24" s="47"/>
+      <c r="E24" s="47"/>
+      <c r="F24" s="47"/>
+      <c r="G24" s="47"/>
+      <c r="H24" s="47"/>
+      <c r="I24" s="47"/>
+      <c r="J24" s="47"/>
       <c r="K24" s="26"/>
       <c r="L24" s="26"/>
       <c r="M24" s="26"/>
@@ -9168,18 +9180,18 @@
       <c r="KA28" s="26"/>
     </row>
     <row r="29" spans="1:287" s="40" customFormat="1" ht="30.75" customHeight="1">
-      <c r="A29" s="49" t="s">
+      <c r="A29" s="56" t="s">
         <v>53</v>
       </c>
-      <c r="B29" s="46"/>
-      <c r="C29" s="46"/>
-      <c r="D29" s="46"/>
-      <c r="E29" s="46"/>
-      <c r="F29" s="46"/>
-      <c r="G29" s="46"/>
-      <c r="H29" s="46"/>
-      <c r="I29" s="46"/>
-      <c r="J29" s="46"/>
+      <c r="B29" s="47"/>
+      <c r="C29" s="47"/>
+      <c r="D29" s="47"/>
+      <c r="E29" s="47"/>
+      <c r="F29" s="47"/>
+      <c r="G29" s="47"/>
+      <c r="H29" s="47"/>
+      <c r="I29" s="47"/>
+      <c r="J29" s="47"/>
       <c r="K29" s="28"/>
       <c r="L29" s="28"/>
       <c r="M29" s="28"/>
@@ -10380,18 +10392,18 @@
       <c r="KA32" s="26"/>
     </row>
     <row r="33" spans="1:287" ht="30.75" customHeight="1">
-      <c r="A33" s="47" t="s">
+      <c r="A33" s="54" t="s">
         <v>58</v>
       </c>
-      <c r="B33" s="48"/>
-      <c r="C33" s="48"/>
-      <c r="D33" s="48"/>
-      <c r="E33" s="48"/>
-      <c r="F33" s="48"/>
-      <c r="G33" s="48"/>
-      <c r="H33" s="48"/>
-      <c r="I33" s="48"/>
-      <c r="J33" s="48"/>
+      <c r="B33" s="55"/>
+      <c r="C33" s="55"/>
+      <c r="D33" s="55"/>
+      <c r="E33" s="55"/>
+      <c r="F33" s="55"/>
+      <c r="G33" s="55"/>
+      <c r="H33" s="55"/>
+      <c r="I33" s="55"/>
+      <c r="J33" s="55"/>
       <c r="K33" s="26"/>
       <c r="L33" s="26"/>
       <c r="M33" s="26"/>
@@ -12206,18 +12218,18 @@
       <c r="KA38" s="26"/>
     </row>
     <row r="39" spans="1:287" s="44" customFormat="1" ht="30.75" customHeight="1">
-      <c r="A39" s="45" t="s">
+      <c r="A39" s="53" t="s">
         <v>63</v>
       </c>
-      <c r="B39" s="46"/>
-      <c r="C39" s="46"/>
-      <c r="D39" s="46"/>
-      <c r="E39" s="46"/>
-      <c r="F39" s="46"/>
-      <c r="G39" s="46"/>
-      <c r="H39" s="46"/>
-      <c r="I39" s="46"/>
-      <c r="J39" s="46"/>
+      <c r="B39" s="47"/>
+      <c r="C39" s="47"/>
+      <c r="D39" s="47"/>
+      <c r="E39" s="47"/>
+      <c r="F39" s="47"/>
+      <c r="G39" s="47"/>
+      <c r="H39" s="47"/>
+      <c r="I39" s="47"/>
+      <c r="J39" s="47"/>
       <c r="K39" s="28"/>
       <c r="L39" s="28"/>
       <c r="M39" s="28"/>
@@ -12512,11 +12524,17 @@
       <c r="E40" s="43">
         <v>43892</v>
       </c>
-      <c r="F40" s="43"/>
-      <c r="G40" s="43"/>
-      <c r="H40" s="28"/>
+      <c r="F40" s="43">
+        <v>43892</v>
+      </c>
+      <c r="G40" s="43">
+        <v>43893</v>
+      </c>
+      <c r="H40" s="28">
+        <v>2</v>
+      </c>
       <c r="I40" s="31" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="J40" s="38" t="s">
         <v>67</v>
@@ -13122,11 +13140,17 @@
       <c r="E42" s="43">
         <v>43893</v>
       </c>
-      <c r="F42" s="26"/>
-      <c r="G42" s="26"/>
-      <c r="H42" s="26"/>
-      <c r="I42" s="27" t="s">
-        <v>65</v>
+      <c r="F42" s="43">
+        <v>43893</v>
+      </c>
+      <c r="G42" s="43">
+        <v>43895</v>
+      </c>
+      <c r="H42" s="26">
+        <v>3</v>
+      </c>
+      <c r="I42" s="31" t="s">
+        <v>30</v>
       </c>
       <c r="J42" s="38" t="s">
         <v>68</v>
@@ -13425,11 +13449,17 @@
       <c r="E43" s="43">
         <v>43894</v>
       </c>
-      <c r="F43" s="26"/>
-      <c r="G43" s="26"/>
-      <c r="H43" s="26"/>
-      <c r="I43" s="27" t="s">
-        <v>65</v>
+      <c r="F43" s="43">
+        <v>43894</v>
+      </c>
+      <c r="G43" s="43">
+        <v>43895</v>
+      </c>
+      <c r="H43" s="26">
+        <v>2</v>
+      </c>
+      <c r="I43" s="31" t="s">
+        <v>30</v>
       </c>
       <c r="J43" s="38" t="s">
         <v>69</v>
@@ -13728,7 +13758,9 @@
       <c r="E44" s="43">
         <v>43895</v>
       </c>
-      <c r="F44" s="43"/>
+      <c r="F44" s="28" t="s">
+        <v>26</v>
+      </c>
       <c r="G44" s="28" t="s">
         <v>26</v>
       </c>
@@ -14031,8 +14063,12 @@
       <c r="E45" s="43">
         <v>43895</v>
       </c>
-      <c r="F45" s="26"/>
-      <c r="G45" s="26"/>
+      <c r="F45" s="28" t="s">
+        <v>26</v>
+      </c>
+      <c r="G45" s="28" t="s">
+        <v>26</v>
+      </c>
       <c r="H45" s="26"/>
       <c r="I45" s="27" t="s">
         <v>65</v>
@@ -14316,299 +14352,307 @@
       <c r="JZ45" s="26"/>
       <c r="KA45" s="26"/>
     </row>
-    <row r="46" spans="1:287" ht="30.75" customHeight="1">
-      <c r="A46" s="31"/>
-      <c r="B46" s="38"/>
-      <c r="C46" s="28"/>
-      <c r="D46" s="26"/>
-      <c r="E46" s="26"/>
-      <c r="F46" s="26"/>
-      <c r="G46" s="26"/>
-      <c r="H46" s="26"/>
-      <c r="I46" s="27"/>
-      <c r="J46" s="38"/>
-      <c r="K46" s="26"/>
-      <c r="L46" s="26"/>
-      <c r="M46" s="26"/>
-      <c r="N46" s="26"/>
-      <c r="O46" s="26"/>
-      <c r="P46" s="26"/>
-      <c r="Q46" s="26"/>
-      <c r="R46" s="26"/>
-      <c r="S46" s="26"/>
-      <c r="T46" s="26"/>
-      <c r="U46" s="26"/>
-      <c r="V46" s="26"/>
-      <c r="W46" s="26"/>
-      <c r="X46" s="26"/>
-      <c r="Y46" s="26"/>
-      <c r="Z46" s="26"/>
-      <c r="AA46" s="26"/>
-      <c r="AB46" s="26"/>
-      <c r="AC46" s="26"/>
-      <c r="AD46" s="26"/>
-      <c r="AE46" s="26"/>
-      <c r="AF46" s="26"/>
-      <c r="AG46" s="26"/>
-      <c r="AH46" s="26"/>
-      <c r="AI46" s="26"/>
-      <c r="AJ46" s="26"/>
-      <c r="AK46" s="26"/>
-      <c r="AL46" s="26"/>
-      <c r="AM46" s="26"/>
-      <c r="AN46" s="26"/>
-      <c r="AO46" s="26"/>
-      <c r="AP46" s="26"/>
-      <c r="AQ46" s="26"/>
-      <c r="AR46" s="26"/>
-      <c r="AS46" s="26"/>
-      <c r="AT46" s="26"/>
-      <c r="AU46" s="26"/>
-      <c r="AV46" s="26"/>
-      <c r="AW46" s="26"/>
-      <c r="AX46" s="26"/>
-      <c r="AY46" s="26"/>
-      <c r="AZ46" s="26"/>
-      <c r="BA46" s="26"/>
-      <c r="BB46" s="26"/>
-      <c r="BC46" s="26"/>
-      <c r="BD46" s="26"/>
-      <c r="BE46" s="26"/>
-      <c r="BF46" s="26"/>
-      <c r="BG46" s="26"/>
-      <c r="BH46" s="26"/>
-      <c r="BI46" s="26"/>
-      <c r="BJ46" s="26"/>
-      <c r="BK46" s="26"/>
-      <c r="BL46" s="26"/>
-      <c r="BM46" s="26"/>
-      <c r="BN46" s="26"/>
-      <c r="BO46" s="26"/>
-      <c r="BP46" s="26"/>
-      <c r="BQ46" s="26"/>
-      <c r="BR46" s="26"/>
-      <c r="BS46" s="26"/>
-      <c r="BT46" s="26"/>
-      <c r="BU46" s="26"/>
-      <c r="BV46" s="26"/>
-      <c r="BW46" s="26"/>
-      <c r="BX46" s="26"/>
-      <c r="BY46" s="26"/>
-      <c r="BZ46" s="26"/>
-      <c r="CA46" s="26"/>
-      <c r="CB46" s="26"/>
-      <c r="CC46" s="26"/>
-      <c r="CD46" s="26"/>
-      <c r="CE46" s="26"/>
-      <c r="CF46" s="26"/>
-      <c r="CG46" s="26"/>
-      <c r="CH46" s="26"/>
-      <c r="CI46" s="26"/>
-      <c r="CJ46" s="26"/>
-      <c r="CK46" s="26"/>
-      <c r="CL46" s="26"/>
-      <c r="CM46" s="26"/>
-      <c r="CN46" s="26"/>
-      <c r="CO46" s="26"/>
-      <c r="CP46" s="26"/>
-      <c r="CQ46" s="26"/>
-      <c r="CR46" s="26"/>
-      <c r="CS46" s="26"/>
-      <c r="CT46" s="26"/>
-      <c r="CU46" s="26"/>
-      <c r="CV46" s="26"/>
-      <c r="CW46" s="26"/>
-      <c r="CX46" s="26"/>
-      <c r="CY46" s="26"/>
-      <c r="CZ46" s="26"/>
-      <c r="DA46" s="26"/>
-      <c r="DB46" s="26"/>
-      <c r="DC46" s="26"/>
-      <c r="DD46" s="26"/>
-      <c r="DE46" s="26"/>
-      <c r="DF46" s="26"/>
-      <c r="DG46" s="26"/>
-      <c r="DH46" s="26"/>
-      <c r="DI46" s="26"/>
-      <c r="DJ46" s="26"/>
-      <c r="DK46" s="26"/>
-      <c r="DL46" s="26"/>
-      <c r="DM46" s="26"/>
-      <c r="DN46" s="26"/>
-      <c r="DO46" s="26"/>
-      <c r="DP46" s="26"/>
-      <c r="DQ46" s="26"/>
-      <c r="DR46" s="26"/>
-      <c r="DS46" s="26"/>
-      <c r="DT46" s="26"/>
-      <c r="DU46" s="26"/>
-      <c r="DV46" s="26"/>
-      <c r="DW46" s="26"/>
-      <c r="DX46" s="26"/>
-      <c r="DY46" s="26"/>
-      <c r="DZ46" s="26"/>
-      <c r="EA46" s="26"/>
-      <c r="EB46" s="26"/>
-      <c r="EC46" s="26"/>
-      <c r="ED46" s="26"/>
-      <c r="EE46" s="26"/>
-      <c r="EF46" s="26"/>
-      <c r="EG46" s="26"/>
-      <c r="EH46" s="26"/>
-      <c r="EI46" s="26"/>
-      <c r="EJ46" s="26"/>
-      <c r="EK46" s="26"/>
-      <c r="EL46" s="26"/>
-      <c r="EM46" s="26"/>
-      <c r="EN46" s="26"/>
-      <c r="EO46" s="26"/>
-      <c r="EP46" s="26"/>
-      <c r="EQ46" s="26"/>
-      <c r="ER46" s="26"/>
-      <c r="ES46" s="26"/>
-      <c r="ET46" s="26"/>
-      <c r="EU46" s="26"/>
-      <c r="EV46" s="26"/>
-      <c r="EW46" s="26"/>
-      <c r="EX46" s="26"/>
-      <c r="EY46" s="26"/>
-      <c r="EZ46" s="26"/>
-      <c r="FA46" s="26"/>
-      <c r="FB46" s="26"/>
-      <c r="FC46" s="26"/>
-      <c r="FD46" s="26"/>
-      <c r="FE46" s="26"/>
-      <c r="FF46" s="26"/>
-      <c r="FG46" s="26"/>
-      <c r="FH46" s="26"/>
-      <c r="FI46" s="26"/>
-      <c r="FJ46" s="26"/>
-      <c r="FK46" s="26"/>
-      <c r="FL46" s="26"/>
-      <c r="FM46" s="26"/>
-      <c r="FN46" s="26"/>
-      <c r="FO46" s="26"/>
-      <c r="FP46" s="26"/>
-      <c r="FQ46" s="26"/>
-      <c r="FR46" s="26"/>
-      <c r="FS46" s="26"/>
-      <c r="FT46" s="26"/>
-      <c r="FU46" s="26"/>
-      <c r="FV46" s="26"/>
-      <c r="FW46" s="26"/>
-      <c r="FX46" s="26"/>
-      <c r="FY46" s="26"/>
-      <c r="FZ46" s="26"/>
-      <c r="GA46" s="26"/>
-      <c r="GB46" s="26"/>
-      <c r="GC46" s="26"/>
-      <c r="GD46" s="26"/>
-      <c r="GE46" s="26"/>
-      <c r="GF46" s="26"/>
-      <c r="GG46" s="26"/>
-      <c r="GH46" s="26"/>
-      <c r="GI46" s="26"/>
-      <c r="GJ46" s="26"/>
-      <c r="GK46" s="26"/>
-      <c r="GL46" s="26"/>
-      <c r="GM46" s="26"/>
-      <c r="GN46" s="26"/>
-      <c r="GO46" s="26"/>
-      <c r="GP46" s="26"/>
-      <c r="GQ46" s="26"/>
-      <c r="GR46" s="26"/>
-      <c r="GS46" s="26"/>
-      <c r="GT46" s="26"/>
-      <c r="GU46" s="26"/>
-      <c r="GV46" s="26"/>
-      <c r="GW46" s="26"/>
-      <c r="GX46" s="26"/>
-      <c r="GY46" s="26"/>
-      <c r="GZ46" s="26"/>
-      <c r="HA46" s="26"/>
-      <c r="HB46" s="26"/>
-      <c r="HC46" s="26"/>
-      <c r="HD46" s="26"/>
-      <c r="HE46" s="26"/>
-      <c r="HF46" s="26"/>
-      <c r="HG46" s="26"/>
-      <c r="HH46" s="26"/>
-      <c r="HI46" s="26"/>
-      <c r="HJ46" s="26"/>
-      <c r="HK46" s="26"/>
-      <c r="HL46" s="26"/>
-      <c r="HM46" s="26"/>
-      <c r="HN46" s="26"/>
-      <c r="HO46" s="26"/>
-      <c r="HP46" s="26"/>
-      <c r="HQ46" s="26"/>
-      <c r="HR46" s="26"/>
-      <c r="HS46" s="26"/>
-      <c r="HT46" s="26"/>
-      <c r="HU46" s="26"/>
-      <c r="HV46" s="26"/>
-      <c r="HW46" s="26"/>
-      <c r="HX46" s="26"/>
-      <c r="HY46" s="26"/>
-      <c r="HZ46" s="26"/>
-      <c r="IA46" s="26"/>
-      <c r="IB46" s="26"/>
-      <c r="IC46" s="26"/>
-      <c r="ID46" s="26"/>
-      <c r="IE46" s="26"/>
-      <c r="IF46" s="26"/>
-      <c r="IG46" s="26"/>
-      <c r="IH46" s="26"/>
-      <c r="II46" s="26"/>
-      <c r="IJ46" s="26"/>
-      <c r="IK46" s="26"/>
-      <c r="IL46" s="26"/>
-      <c r="IM46" s="26"/>
-      <c r="IN46" s="26"/>
-      <c r="IO46" s="26"/>
-      <c r="IP46" s="26"/>
-      <c r="IQ46" s="26"/>
-      <c r="IR46" s="26"/>
-      <c r="IS46" s="26"/>
-      <c r="IT46" s="26"/>
-      <c r="IU46" s="26"/>
-      <c r="IV46" s="26"/>
-      <c r="IW46" s="26"/>
-      <c r="IX46" s="26"/>
-      <c r="IY46" s="26"/>
-      <c r="IZ46" s="26"/>
-      <c r="JA46" s="26"/>
-      <c r="JB46" s="26"/>
-      <c r="JC46" s="26"/>
-      <c r="JD46" s="26"/>
-      <c r="JE46" s="26"/>
-      <c r="JF46" s="26"/>
-      <c r="JG46" s="26"/>
-      <c r="JH46" s="26"/>
-      <c r="JI46" s="26"/>
-      <c r="JJ46" s="26"/>
-      <c r="JK46" s="26"/>
-      <c r="JL46" s="26"/>
-      <c r="JM46" s="26"/>
-      <c r="JN46" s="26"/>
-      <c r="JO46" s="26"/>
-      <c r="JP46" s="26"/>
-      <c r="JQ46" s="26"/>
-      <c r="JR46" s="26"/>
-      <c r="JS46" s="26"/>
-      <c r="JT46" s="26"/>
-      <c r="JU46" s="26"/>
-      <c r="JV46" s="26"/>
-      <c r="JW46" s="26"/>
-      <c r="JX46" s="26"/>
-      <c r="JY46" s="26"/>
-      <c r="JZ46" s="26"/>
-      <c r="KA46" s="26"/>
+    <row r="46" spans="1:287" s="45" customFormat="1" ht="30.75" customHeight="1">
+      <c r="A46" s="53" t="s">
+        <v>71</v>
+      </c>
+      <c r="B46" s="47"/>
+      <c r="C46" s="47"/>
+      <c r="D46" s="47"/>
+      <c r="E46" s="47"/>
+      <c r="F46" s="47"/>
+      <c r="G46" s="47"/>
+      <c r="H46" s="47"/>
+      <c r="I46" s="47"/>
+      <c r="J46" s="47"/>
+      <c r="K46" s="28"/>
+      <c r="L46" s="28"/>
+      <c r="M46" s="28"/>
+      <c r="N46" s="28"/>
+      <c r="O46" s="28"/>
+      <c r="P46" s="28"/>
+      <c r="Q46" s="28"/>
+      <c r="R46" s="28"/>
+      <c r="S46" s="28"/>
+      <c r="T46" s="28"/>
+      <c r="U46" s="28"/>
+      <c r="V46" s="28"/>
+      <c r="W46" s="28"/>
+      <c r="X46" s="28"/>
+      <c r="Y46" s="28"/>
+      <c r="Z46" s="28"/>
+      <c r="AA46" s="28"/>
+      <c r="AB46" s="28"/>
+      <c r="AC46" s="28"/>
+      <c r="AD46" s="28"/>
+      <c r="AE46" s="28"/>
+      <c r="AF46" s="28"/>
+      <c r="AG46" s="28"/>
+      <c r="AH46" s="28"/>
+      <c r="AI46" s="28"/>
+      <c r="AJ46" s="28"/>
+      <c r="AK46" s="28"/>
+      <c r="AL46" s="28"/>
+      <c r="AM46" s="28"/>
+      <c r="AN46" s="28"/>
+      <c r="AO46" s="28"/>
+      <c r="AP46" s="28"/>
+      <c r="AQ46" s="28"/>
+      <c r="AR46" s="28"/>
+      <c r="AS46" s="28"/>
+      <c r="AT46" s="28"/>
+      <c r="AU46" s="28"/>
+      <c r="AV46" s="28"/>
+      <c r="AW46" s="28"/>
+      <c r="AX46" s="28"/>
+      <c r="AY46" s="28"/>
+      <c r="AZ46" s="28"/>
+      <c r="BA46" s="28"/>
+      <c r="BB46" s="28"/>
+      <c r="BC46" s="28"/>
+      <c r="BD46" s="28"/>
+      <c r="BE46" s="28"/>
+      <c r="BF46" s="28"/>
+      <c r="BG46" s="28"/>
+      <c r="BH46" s="28"/>
+      <c r="BI46" s="28"/>
+      <c r="BJ46" s="28"/>
+      <c r="BK46" s="28"/>
+      <c r="BL46" s="28"/>
+      <c r="BM46" s="28"/>
+      <c r="BN46" s="28"/>
+      <c r="BO46" s="28"/>
+      <c r="BP46" s="28"/>
+      <c r="BQ46" s="28"/>
+      <c r="BR46" s="28"/>
+      <c r="BS46" s="28"/>
+      <c r="BT46" s="28"/>
+      <c r="BU46" s="28"/>
+      <c r="BV46" s="28"/>
+      <c r="BW46" s="28"/>
+      <c r="BX46" s="28"/>
+      <c r="BY46" s="28"/>
+      <c r="BZ46" s="28"/>
+      <c r="CA46" s="28"/>
+      <c r="CB46" s="28"/>
+      <c r="CC46" s="28"/>
+      <c r="CD46" s="28"/>
+      <c r="CE46" s="28"/>
+      <c r="CF46" s="28"/>
+      <c r="CG46" s="28"/>
+      <c r="CH46" s="28"/>
+      <c r="CI46" s="28"/>
+      <c r="CJ46" s="28"/>
+      <c r="CK46" s="28"/>
+      <c r="CL46" s="28"/>
+      <c r="CM46" s="28"/>
+      <c r="CN46" s="28"/>
+      <c r="CO46" s="28"/>
+      <c r="CP46" s="28"/>
+      <c r="CQ46" s="28"/>
+      <c r="CR46" s="28"/>
+      <c r="CS46" s="28"/>
+      <c r="CT46" s="28"/>
+      <c r="CU46" s="28"/>
+      <c r="CV46" s="28"/>
+      <c r="CW46" s="28"/>
+      <c r="CX46" s="28"/>
+      <c r="CY46" s="28"/>
+      <c r="CZ46" s="28"/>
+      <c r="DA46" s="28"/>
+      <c r="DB46" s="28"/>
+      <c r="DC46" s="28"/>
+      <c r="DD46" s="28"/>
+      <c r="DE46" s="28"/>
+      <c r="DF46" s="28"/>
+      <c r="DG46" s="28"/>
+      <c r="DH46" s="28"/>
+      <c r="DI46" s="28"/>
+      <c r="DJ46" s="28"/>
+      <c r="DK46" s="28"/>
+      <c r="DL46" s="28"/>
+      <c r="DM46" s="28"/>
+      <c r="DN46" s="28"/>
+      <c r="DO46" s="28"/>
+      <c r="DP46" s="28"/>
+      <c r="DQ46" s="28"/>
+      <c r="DR46" s="28"/>
+      <c r="DS46" s="28"/>
+      <c r="DT46" s="28"/>
+      <c r="DU46" s="28"/>
+      <c r="DV46" s="28"/>
+      <c r="DW46" s="28"/>
+      <c r="DX46" s="28"/>
+      <c r="DY46" s="28"/>
+      <c r="DZ46" s="28"/>
+      <c r="EA46" s="28"/>
+      <c r="EB46" s="28"/>
+      <c r="EC46" s="28"/>
+      <c r="ED46" s="28"/>
+      <c r="EE46" s="28"/>
+      <c r="EF46" s="28"/>
+      <c r="EG46" s="28"/>
+      <c r="EH46" s="28"/>
+      <c r="EI46" s="28"/>
+      <c r="EJ46" s="28"/>
+      <c r="EK46" s="28"/>
+      <c r="EL46" s="28"/>
+      <c r="EM46" s="28"/>
+      <c r="EN46" s="28"/>
+      <c r="EO46" s="28"/>
+      <c r="EP46" s="28"/>
+      <c r="EQ46" s="28"/>
+      <c r="ER46" s="28"/>
+      <c r="ES46" s="28"/>
+      <c r="ET46" s="28"/>
+      <c r="EU46" s="28"/>
+      <c r="EV46" s="28"/>
+      <c r="EW46" s="28"/>
+      <c r="EX46" s="28"/>
+      <c r="EY46" s="28"/>
+      <c r="EZ46" s="28"/>
+      <c r="FA46" s="28"/>
+      <c r="FB46" s="28"/>
+      <c r="FC46" s="28"/>
+      <c r="FD46" s="28"/>
+      <c r="FE46" s="28"/>
+      <c r="FF46" s="28"/>
+      <c r="FG46" s="28"/>
+      <c r="FH46" s="28"/>
+      <c r="FI46" s="28"/>
+      <c r="FJ46" s="28"/>
+      <c r="FK46" s="28"/>
+      <c r="FL46" s="28"/>
+      <c r="FM46" s="28"/>
+      <c r="FN46" s="28"/>
+      <c r="FO46" s="28"/>
+      <c r="FP46" s="28"/>
+      <c r="FQ46" s="28"/>
+      <c r="FR46" s="28"/>
+      <c r="FS46" s="28"/>
+      <c r="FT46" s="28"/>
+      <c r="FU46" s="28"/>
+      <c r="FV46" s="28"/>
+      <c r="FW46" s="28"/>
+      <c r="FX46" s="28"/>
+      <c r="FY46" s="28"/>
+      <c r="FZ46" s="28"/>
+      <c r="GA46" s="28"/>
+      <c r="GB46" s="28"/>
+      <c r="GC46" s="28"/>
+      <c r="GD46" s="28"/>
+      <c r="GE46" s="28"/>
+      <c r="GF46" s="28"/>
+      <c r="GG46" s="28"/>
+      <c r="GH46" s="28"/>
+      <c r="GI46" s="28"/>
+      <c r="GJ46" s="28"/>
+      <c r="GK46" s="28"/>
+      <c r="GL46" s="28"/>
+      <c r="GM46" s="28"/>
+      <c r="GN46" s="28"/>
+      <c r="GO46" s="28"/>
+      <c r="GP46" s="28"/>
+      <c r="GQ46" s="28"/>
+      <c r="GR46" s="28"/>
+      <c r="GS46" s="28"/>
+      <c r="GT46" s="28"/>
+      <c r="GU46" s="28"/>
+      <c r="GV46" s="28"/>
+      <c r="GW46" s="28"/>
+      <c r="GX46" s="28"/>
+      <c r="GY46" s="28"/>
+      <c r="GZ46" s="28"/>
+      <c r="HA46" s="28"/>
+      <c r="HB46" s="28"/>
+      <c r="HC46" s="28"/>
+      <c r="HD46" s="28"/>
+      <c r="HE46" s="28"/>
+      <c r="HF46" s="28"/>
+      <c r="HG46" s="28"/>
+      <c r="HH46" s="28"/>
+      <c r="HI46" s="28"/>
+      <c r="HJ46" s="28"/>
+      <c r="HK46" s="28"/>
+      <c r="HL46" s="28"/>
+      <c r="HM46" s="28"/>
+      <c r="HN46" s="28"/>
+      <c r="HO46" s="28"/>
+      <c r="HP46" s="28"/>
+      <c r="HQ46" s="28"/>
+      <c r="HR46" s="28"/>
+      <c r="HS46" s="28"/>
+      <c r="HT46" s="28"/>
+      <c r="HU46" s="28"/>
+      <c r="HV46" s="28"/>
+      <c r="HW46" s="28"/>
+      <c r="HX46" s="28"/>
+      <c r="HY46" s="28"/>
+      <c r="HZ46" s="28"/>
+      <c r="IA46" s="28"/>
+      <c r="IB46" s="28"/>
+      <c r="IC46" s="28"/>
+      <c r="ID46" s="28"/>
+      <c r="IE46" s="28"/>
+      <c r="IF46" s="28"/>
+      <c r="IG46" s="28"/>
+      <c r="IH46" s="28"/>
+      <c r="II46" s="28"/>
+      <c r="IJ46" s="28"/>
+      <c r="IK46" s="28"/>
+      <c r="IL46" s="28"/>
+      <c r="IM46" s="28"/>
+      <c r="IN46" s="28"/>
+      <c r="IO46" s="28"/>
+      <c r="IP46" s="28"/>
+      <c r="IQ46" s="28"/>
+      <c r="IR46" s="28"/>
+      <c r="IS46" s="28"/>
+      <c r="IT46" s="28"/>
+      <c r="IU46" s="28"/>
+      <c r="IV46" s="28"/>
+      <c r="IW46" s="28"/>
+      <c r="IX46" s="28"/>
+      <c r="IY46" s="28"/>
+      <c r="IZ46" s="28"/>
+      <c r="JA46" s="28"/>
+      <c r="JB46" s="28"/>
+      <c r="JC46" s="28"/>
+      <c r="JD46" s="28"/>
+      <c r="JE46" s="28"/>
+      <c r="JF46" s="28"/>
+      <c r="JG46" s="28"/>
+      <c r="JH46" s="28"/>
+      <c r="JI46" s="28"/>
+      <c r="JJ46" s="28"/>
+      <c r="JK46" s="28"/>
+      <c r="JL46" s="28"/>
+      <c r="JM46" s="28"/>
+      <c r="JN46" s="28"/>
+      <c r="JO46" s="28"/>
+      <c r="JP46" s="28"/>
+      <c r="JQ46" s="28"/>
+      <c r="JR46" s="28"/>
+      <c r="JS46" s="28"/>
+      <c r="JT46" s="28"/>
+      <c r="JU46" s="28"/>
+      <c r="JV46" s="28"/>
+      <c r="JW46" s="28"/>
+      <c r="JX46" s="28"/>
+      <c r="JY46" s="28"/>
+      <c r="JZ46" s="28"/>
+      <c r="KA46" s="28"/>
     </row>
     <row r="47" spans="1:287" ht="30.75" customHeight="1">
-      <c r="A47" s="31"/>
-      <c r="B47" s="38"/>
-      <c r="C47" s="28"/>
+      <c r="A47" s="31" t="s">
+        <v>62</v>
+      </c>
+      <c r="B47" s="38" t="s">
+        <v>57</v>
+      </c>
+      <c r="C47" s="28" t="s">
+        <v>35</v>
+      </c>
       <c r="D47" s="26"/>
       <c r="E47" s="26"/>
       <c r="F47" s="26"/>
@@ -14895,9 +14939,15 @@
       <c r="KA47" s="26"/>
     </row>
     <row r="48" spans="1:287" ht="30.75" customHeight="1">
-      <c r="A48" s="31"/>
-      <c r="B48" s="38"/>
-      <c r="C48" s="28"/>
+      <c r="A48" s="31" t="s">
+        <v>55</v>
+      </c>
+      <c r="B48" s="38" t="s">
+        <v>57</v>
+      </c>
+      <c r="C48" s="28" t="s">
+        <v>8</v>
+      </c>
       <c r="D48" s="26"/>
       <c r="E48" s="26"/>
       <c r="F48" s="26"/>
@@ -15184,9 +15234,15 @@
       <c r="KA48" s="26"/>
     </row>
     <row r="49" spans="1:287" ht="30.75" customHeight="1">
-      <c r="A49" s="31"/>
-      <c r="B49" s="38"/>
-      <c r="C49" s="28"/>
+      <c r="A49" s="42" t="s">
+        <v>70</v>
+      </c>
+      <c r="B49" s="38" t="s">
+        <v>57</v>
+      </c>
+      <c r="C49" s="28" t="s">
+        <v>8</v>
+      </c>
       <c r="D49" s="26"/>
       <c r="E49" s="26"/>
       <c r="F49" s="26"/>
@@ -19309,29 +19365,30 @@
       <c r="A1000" s="32"/>
     </row>
   </sheetData>
-  <mergeCells count="10">
+  <mergeCells count="11">
+    <mergeCell ref="A46:J46"/>
+    <mergeCell ref="A39:J39"/>
+    <mergeCell ref="A33:J33"/>
+    <mergeCell ref="A29:J29"/>
+    <mergeCell ref="A13:J13"/>
+    <mergeCell ref="A24:J24"/>
     <mergeCell ref="A1:E1"/>
     <mergeCell ref="F2:H2"/>
     <mergeCell ref="B4:E4"/>
     <mergeCell ref="A6:J6"/>
     <mergeCell ref="A7:J7"/>
-    <mergeCell ref="A39:J39"/>
-    <mergeCell ref="A33:J33"/>
-    <mergeCell ref="A29:J29"/>
-    <mergeCell ref="A13:J13"/>
-    <mergeCell ref="A24:J24"/>
   </mergeCells>
   <dataValidations count="4">
-    <dataValidation type="list" allowBlank="1" sqref="I8:I12 I14:I23 I25:I28 I30:I32 I34:I38 I40:I52" xr:uid="{00000000-0002-0000-0000-000000000000}">
+    <dataValidation type="list" allowBlank="1" sqref="I8:I12 I14:I23 I25:I28 I30:I32 I34:I38 I40:I45 I47:I52" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>"STILL,ON GOING,DELIVERED"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" sqref="C8:C12 C14:C23 C25:C28 C30:C32 C34:C38 C40:C52" xr:uid="{00000000-0002-0000-0000-000002000000}">
+    <dataValidation type="list" allowBlank="1" sqref="C8:C12 C14:C23 C25:C28 C30:C32 C34:C38 C40:C45 C47:C52" xr:uid="{00000000-0002-0000-0000-000002000000}">
       <formula1>"Hazem Mekawy,Esraa Awad,Nada Mohamed,Mina Helmi,Alzahraa El-Sallakh"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" sqref="B8:B12 B14:B23 B25:B28 B30:B32 B34:B38 B40:B75" xr:uid="{8C288E01-D924-4500-863C-FF5C93406017}">
+    <dataValidation type="list" allowBlank="1" sqref="B8:B12 B14:B23 B25:B28 B30:B32 B34:B38 B40:B45 B47:B75" xr:uid="{8C288E01-D924-4500-863C-FF5C93406017}">
       <formula1>"Documentation, Code Implementation"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" sqref="B34:B38 B40:B177" xr:uid="{00000000-0002-0000-0000-000001000000}">
+    <dataValidation type="list" allowBlank="1" sqref="B34:B38 B40:B45 B47:B177" xr:uid="{00000000-0002-0000-0000-000001000000}">
       <formula1>"Technical,Non -Technical"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>